<commit_message>
Update 2026_멀티.xlsx (2026-01-23 11:02:00)
</commit_message>
<xml_diff>
--- a/2026_멀티.xlsx
+++ b/2026_멀티.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyejinha/Desktop/Workspace/Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4640EDA-0BFD-FB45-AC50-CAEF6DFB27BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D61DA59-81A7-FD41-BB33-70A55DA85EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="17060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="87">
   <si>
     <t>기준일자</t>
   </si>
@@ -271,6 +271,21 @@
   </si>
   <si>
     <t>애플</t>
+  </si>
+  <si>
+    <t>YOFC</t>
+  </si>
+  <si>
+    <t>WUXIAPPTEC</t>
+  </si>
+  <si>
+    <t>LAOPUGOLD</t>
+  </si>
+  <si>
+    <t>BIRENTECH</t>
+  </si>
+  <si>
+    <t>BABA-W</t>
   </si>
 </sst>
 </file>
@@ -16515,56 +16530,56 @@
         <v>46044</v>
       </c>
       <c r="B170" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C170" s="10"/>
-      <c r="D170" s="9">
-        <v>6869</v>
+      <c r="D170" s="9" t="s">
+        <v>64</v>
       </c>
       <c r="E170" s="9">
         <v>0</v>
       </c>
-      <c r="F170" s="9">
-        <v>0</v>
+      <c r="F170" s="11">
+        <v>10000</v>
       </c>
       <c r="G170" s="9">
-        <v>0</v>
-      </c>
-      <c r="H170" s="9">
-        <v>0</v>
+        <v>48.203000000000003</v>
+      </c>
+      <c r="H170" s="11">
+        <v>482030</v>
       </c>
       <c r="I170" s="9">
-        <v>51.6</v>
-      </c>
-      <c r="J170" s="9">
-        <v>0</v>
-      </c>
-      <c r="K170" s="9">
-        <v>0</v>
-      </c>
-      <c r="L170" s="9">
-        <v>0</v>
+        <v>51.54</v>
+      </c>
+      <c r="J170" s="11">
+        <v>515400</v>
+      </c>
+      <c r="K170" s="11">
+        <v>33370</v>
+      </c>
+      <c r="L170" s="12">
+        <v>57390049</v>
       </c>
       <c r="M170" s="9">
         <v>0</v>
       </c>
-      <c r="N170" s="11">
-        <v>349976</v>
-      </c>
-      <c r="O170" s="11">
-        <v>349976</v>
+      <c r="N170" s="9">
+        <v>0</v>
+      </c>
+      <c r="O170" s="9">
+        <v>0</v>
       </c>
       <c r="P170" s="9">
         <v>0</v>
       </c>
       <c r="Q170" s="9" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="R170" s="9" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="S170" s="9" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="T170" s="10"/>
       <c r="U170" s="9">
@@ -16573,32 +16588,32 @@
       <c r="V170" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="W170" s="9">
-        <v>0</v>
-      </c>
-      <c r="X170" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y170" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z170" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA170" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB170" s="9">
-        <v>0</v>
+      <c r="W170" s="11">
+        <v>1455.7</v>
+      </c>
+      <c r="X170" s="12">
+        <v>701691071</v>
+      </c>
+      <c r="Y170" s="11">
+        <v>1472.8</v>
+      </c>
+      <c r="Z170" s="12">
+        <v>759081120</v>
+      </c>
+      <c r="AA170" s="12">
+        <v>49147336</v>
+      </c>
+      <c r="AB170" s="12">
+        <v>8242713</v>
       </c>
       <c r="AC170" s="9">
         <v>0</v>
       </c>
-      <c r="AD170" s="12">
-        <v>72042766</v>
-      </c>
-      <c r="AE170" s="12">
-        <v>72042766</v>
+      <c r="AD170" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE170" s="9">
+        <v>0</v>
       </c>
       <c r="AF170" s="9">
         <v>0</v>
@@ -16609,35 +16624,35 @@
         <v>46044</v>
       </c>
       <c r="B171" s="9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C171" s="10"/>
-      <c r="D171" s="9">
-        <v>2359</v>
+      <c r="D171" s="9" t="s">
+        <v>77</v>
       </c>
       <c r="E171" s="9">
         <v>0</v>
       </c>
       <c r="F171" s="11">
-        <v>25000</v>
+        <v>20000</v>
       </c>
       <c r="G171" s="9">
-        <v>118.559</v>
+        <v>34.24</v>
       </c>
       <c r="H171" s="11">
-        <v>2963990</v>
+        <v>684800</v>
       </c>
       <c r="I171" s="9">
-        <v>112.8</v>
+        <v>34.380000000000003</v>
       </c>
       <c r="J171" s="11">
-        <v>2820000</v>
+        <v>687600</v>
       </c>
       <c r="K171" s="11">
-        <v>-143990</v>
+        <v>2800</v>
       </c>
       <c r="L171" s="12">
-        <v>-27405750</v>
+        <v>1247680</v>
       </c>
       <c r="M171" s="9">
         <v>0</v>
@@ -16652,13 +16667,13 @@
         <v>0</v>
       </c>
       <c r="Q171" s="9" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="R171" s="9" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="S171" s="9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="T171" s="10"/>
       <c r="U171" s="9">
@@ -16667,23 +16682,23 @@
       <c r="V171" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="W171" s="9">
-        <v>188.95</v>
+      <c r="W171" s="11">
+        <v>1477</v>
       </c>
       <c r="X171" s="12">
-        <v>560075550</v>
-      </c>
-      <c r="Y171" s="9">
-        <v>188.89</v>
+        <v>1011449600</v>
+      </c>
+      <c r="Y171" s="11">
+        <v>1472.8</v>
       </c>
       <c r="Z171" s="12">
-        <v>532669800</v>
+        <v>1012697280</v>
       </c>
       <c r="AA171" s="12">
-        <v>-27198271</v>
+        <v>4123840</v>
       </c>
       <c r="AB171" s="12">
-        <v>-207479</v>
+        <v>-2876160</v>
       </c>
       <c r="AC171" s="9">
         <v>0</v>
@@ -16703,56 +16718,56 @@
         <v>46044</v>
       </c>
       <c r="B172" s="9" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="C172" s="10"/>
-      <c r="D172" s="9">
-        <v>6181</v>
+      <c r="D172" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="E172" s="9">
         <v>0</v>
       </c>
-      <c r="F172" s="9">
-        <v>0</v>
+      <c r="F172" s="11">
+        <v>3000</v>
       </c>
       <c r="G172" s="9">
-        <v>0</v>
-      </c>
-      <c r="H172" s="9">
-        <v>0</v>
+        <v>247.65</v>
+      </c>
+      <c r="H172" s="11">
+        <v>742950</v>
       </c>
       <c r="I172" s="9">
-        <v>717.5</v>
-      </c>
-      <c r="J172" s="9">
-        <v>0</v>
-      </c>
-      <c r="K172" s="9">
-        <v>0</v>
-      </c>
-      <c r="L172" s="9">
-        <v>0</v>
+        <v>248.35</v>
+      </c>
+      <c r="J172" s="11">
+        <v>745050</v>
+      </c>
+      <c r="K172" s="11">
+        <v>2100</v>
+      </c>
+      <c r="L172" s="12">
+        <v>-27510</v>
       </c>
       <c r="M172" s="9">
         <v>0</v>
       </c>
-      <c r="N172" s="11">
-        <v>-6374.88</v>
+      <c r="N172" s="9">
+        <v>0</v>
       </c>
       <c r="O172" s="9">
         <v>0</v>
       </c>
-      <c r="P172" s="11">
-        <v>6374.88</v>
+      <c r="P172" s="9">
+        <v>0</v>
       </c>
       <c r="Q172" s="9" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="R172" s="9" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="S172" s="9" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="T172" s="10"/>
       <c r="U172" s="9">
@@ -16761,32 +16776,32 @@
       <c r="V172" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="W172" s="9">
-        <v>0</v>
-      </c>
-      <c r="X172" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y172" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z172" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA172" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB172" s="9">
-        <v>0</v>
+      <c r="W172" s="11">
+        <v>1477</v>
+      </c>
+      <c r="X172" s="12">
+        <v>1097337150</v>
+      </c>
+      <c r="Y172" s="11">
+        <v>1472.8</v>
+      </c>
+      <c r="Z172" s="12">
+        <v>1097309640</v>
+      </c>
+      <c r="AA172" s="12">
+        <v>3092880</v>
+      </c>
+      <c r="AB172" s="12">
+        <v>-3120390</v>
       </c>
       <c r="AC172" s="9">
         <v>0</v>
       </c>
-      <c r="AD172" s="12">
-        <v>1362525</v>
-      </c>
-      <c r="AE172" s="12">
-        <v>1362525</v>
+      <c r="AD172" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE172" s="9">
+        <v>0</v>
       </c>
       <c r="AF172" s="9">
         <v>0</v>
@@ -16797,56 +16812,56 @@
         <v>46044</v>
       </c>
       <c r="B173" s="9" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C173" s="10"/>
-      <c r="D173" s="9">
-        <v>6082</v>
+      <c r="D173" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="E173" s="9">
         <v>0</v>
       </c>
-      <c r="F173" s="9">
-        <v>0</v>
+      <c r="F173" s="11">
+        <v>83000</v>
       </c>
       <c r="G173" s="9">
-        <v>0</v>
-      </c>
-      <c r="H173" s="9">
-        <v>0</v>
+        <v>12.374000000000001</v>
+      </c>
+      <c r="H173" s="11">
+        <v>1027042</v>
       </c>
       <c r="I173" s="9">
-        <v>36.92</v>
-      </c>
-      <c r="J173" s="9">
-        <v>0</v>
-      </c>
-      <c r="K173" s="9">
-        <v>0</v>
-      </c>
-      <c r="L173" s="9">
-        <v>0</v>
+        <v>10.51</v>
+      </c>
+      <c r="J173" s="11">
+        <v>872330</v>
+      </c>
+      <c r="K173" s="11">
+        <v>-154712</v>
+      </c>
+      <c r="L173" s="12">
+        <v>-200026995</v>
       </c>
       <c r="M173" s="9">
         <v>0</v>
       </c>
-      <c r="N173" s="11">
-        <v>205980</v>
-      </c>
-      <c r="O173" s="11">
-        <v>205980</v>
+      <c r="N173" s="9">
+        <v>0</v>
+      </c>
+      <c r="O173" s="9">
+        <v>0</v>
       </c>
       <c r="P173" s="9">
         <v>0</v>
       </c>
       <c r="Q173" s="9" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="R173" s="9" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="S173" s="9" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="T173" s="10"/>
       <c r="U173" s="9">
@@ -16855,32 +16870,32 @@
       <c r="V173" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="W173" s="9">
-        <v>0</v>
-      </c>
-      <c r="X173" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y173" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z173" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA173" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB173" s="9">
-        <v>0</v>
+      <c r="W173" s="11">
+        <v>1445.69</v>
+      </c>
+      <c r="X173" s="12">
+        <v>1484794619</v>
+      </c>
+      <c r="Y173" s="11">
+        <v>1472.8</v>
+      </c>
+      <c r="Z173" s="12">
+        <v>1284767624</v>
+      </c>
+      <c r="AA173" s="12">
+        <v>-227859833</v>
+      </c>
+      <c r="AB173" s="12">
+        <v>27832838</v>
       </c>
       <c r="AC173" s="9">
         <v>0</v>
       </c>
-      <c r="AD173" s="12">
-        <v>49395681</v>
-      </c>
-      <c r="AE173" s="12">
-        <v>49395681</v>
+      <c r="AD173" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE173" s="9">
+        <v>0</v>
       </c>
       <c r="AF173" s="9">
         <v>0</v>
@@ -16891,90 +16906,90 @@
         <v>46044</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C174" s="10"/>
-      <c r="D174" s="9">
-        <v>9988</v>
+      <c r="D174" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="E174" s="9">
         <v>0</v>
       </c>
       <c r="F174" s="11">
-        <v>70500</v>
+        <v>2500</v>
       </c>
       <c r="G174" s="9">
-        <v>147.79</v>
+        <v>681.92</v>
       </c>
       <c r="H174" s="11">
-        <v>10419200</v>
+        <v>1704800</v>
       </c>
       <c r="I174" s="9">
-        <v>163.30000000000001</v>
+        <v>688.98</v>
       </c>
       <c r="J174" s="11">
-        <v>11512650</v>
+        <v>1722450</v>
       </c>
       <c r="K174" s="11">
-        <v>1093450</v>
+        <v>17650</v>
       </c>
       <c r="L174" s="12">
-        <v>239825858</v>
-      </c>
-      <c r="M174" s="9">
-        <v>0</v>
-      </c>
-      <c r="N174" s="9">
-        <v>0</v>
-      </c>
-      <c r="O174" s="9">
-        <v>0</v>
+        <v>90606840</v>
+      </c>
+      <c r="M174" s="11">
+        <v>8700</v>
+      </c>
+      <c r="N174" s="11">
+        <v>8700</v>
+      </c>
+      <c r="O174" s="11">
+        <v>8700</v>
       </c>
       <c r="P174" s="9">
         <v>0</v>
       </c>
       <c r="Q174" s="9" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="R174" s="9" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="S174" s="9" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="T174" s="10"/>
       <c r="U174" s="9">
         <v>0</v>
       </c>
       <c r="V174" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="W174" s="9">
-        <v>185.69</v>
+        <v>42</v>
+      </c>
+      <c r="W174" s="11">
+        <v>1434.9</v>
       </c>
       <c r="X174" s="12">
-        <v>1934798600</v>
-      </c>
-      <c r="Y174" s="9">
-        <v>188.89</v>
+        <v>2446217520</v>
+      </c>
+      <c r="Y174" s="11">
+        <v>1472.8</v>
       </c>
       <c r="Z174" s="12">
-        <v>2174624458</v>
+        <v>2536824360</v>
       </c>
       <c r="AA174" s="12">
-        <v>206541770</v>
+        <v>25994920</v>
       </c>
       <c r="AB174" s="12">
-        <v>33284088</v>
-      </c>
-      <c r="AC174" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD174" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE174" s="9">
-        <v>0</v>
+        <v>64611920</v>
+      </c>
+      <c r="AC174" s="12">
+        <v>84621980</v>
+      </c>
+      <c r="AD174" s="12">
+        <v>84621980</v>
+      </c>
+      <c r="AE174" s="12">
+        <v>84621980</v>
       </c>
       <c r="AF174" s="9">
         <v>0</v>
@@ -16985,35 +17000,35 @@
         <v>46044</v>
       </c>
       <c r="B175" s="9" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="C175" s="10"/>
-      <c r="D175" s="9">
-        <v>6861</v>
+      <c r="D175" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="E175" s="9">
         <v>0</v>
       </c>
       <c r="F175" s="11">
-        <v>1900</v>
-      </c>
-      <c r="G175" s="11">
-        <v>55916.79</v>
+        <v>4200</v>
+      </c>
+      <c r="G175" s="9">
+        <v>396.31</v>
       </c>
       <c r="H175" s="11">
-        <v>106241900</v>
-      </c>
-      <c r="I175" s="11">
-        <v>59590</v>
+        <v>1664502</v>
+      </c>
+      <c r="I175" s="9">
+        <v>451.79</v>
       </c>
       <c r="J175" s="11">
-        <v>113221000</v>
+        <v>1897518</v>
       </c>
       <c r="K175" s="11">
-        <v>6979100</v>
+        <v>233016</v>
       </c>
       <c r="L175" s="12">
-        <v>71255638</v>
+        <v>406270591</v>
       </c>
       <c r="M175" s="9">
         <v>0</v>
@@ -17028,38 +17043,38 @@
         <v>0</v>
       </c>
       <c r="Q175" s="9" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="R175" s="9" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="S175" s="9" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="T175" s="10"/>
       <c r="U175" s="9">
         <v>0</v>
       </c>
       <c r="V175" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="W175" s="9">
-        <v>924.45</v>
+        <v>42</v>
+      </c>
+      <c r="W175" s="11">
+        <v>1434.89</v>
       </c>
       <c r="X175" s="12">
-        <v>982163868</v>
-      </c>
-      <c r="Y175" s="9">
-        <v>930.41</v>
+        <v>2388393919</v>
+      </c>
+      <c r="Y175" s="11">
+        <v>1472.8</v>
       </c>
       <c r="Z175" s="12">
-        <v>1053419506</v>
+        <v>2794664510</v>
       </c>
       <c r="AA175" s="12">
-        <v>64934244</v>
+        <v>343185964</v>
       </c>
       <c r="AB175" s="12">
-        <v>6321393</v>
+        <v>63084626</v>
       </c>
       <c r="AC175" s="9">
         <v>0</v>
@@ -17079,56 +17094,56 @@
         <v>46044</v>
       </c>
       <c r="B176" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C176" s="10"/>
       <c r="D176" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E176" s="9">
         <v>0</v>
       </c>
-      <c r="F176" s="9">
-        <v>0</v>
+      <c r="F176" s="11">
+        <v>24000</v>
       </c>
       <c r="G176" s="9">
-        <v>0</v>
-      </c>
-      <c r="H176" s="9">
-        <v>0</v>
-      </c>
-      <c r="I176" s="11">
-        <v>17990</v>
-      </c>
-      <c r="J176" s="9">
-        <v>0</v>
-      </c>
-      <c r="K176" s="9">
-        <v>0</v>
-      </c>
-      <c r="L176" s="9">
-        <v>0</v>
+        <v>17.655000000000001</v>
+      </c>
+      <c r="H176" s="11">
+        <v>423736.8</v>
+      </c>
+      <c r="I176" s="9">
+        <v>16.04</v>
+      </c>
+      <c r="J176" s="11">
+        <v>384960</v>
+      </c>
+      <c r="K176" s="11">
+        <v>-38776.800000000003</v>
+      </c>
+      <c r="L176" s="12">
+        <v>-53423960</v>
       </c>
       <c r="M176" s="9">
         <v>0</v>
       </c>
-      <c r="N176" s="11">
-        <v>4480700</v>
-      </c>
-      <c r="O176" s="11">
-        <v>4480700</v>
+      <c r="N176" s="9">
+        <v>0</v>
+      </c>
+      <c r="O176" s="9">
+        <v>0</v>
       </c>
       <c r="P176" s="9">
         <v>0</v>
       </c>
       <c r="Q176" s="9" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="R176" s="9" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="S176" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="T176" s="10"/>
       <c r="U176" s="9">
@@ -17137,32 +17152,32 @@
       <c r="V176" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="W176" s="9">
-        <v>0</v>
-      </c>
-      <c r="X176" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y176" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z176" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA176" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB176" s="9">
-        <v>0</v>
+      <c r="W176" s="11">
+        <v>1464.09</v>
+      </c>
+      <c r="X176" s="12">
+        <v>620393048</v>
+      </c>
+      <c r="Y176" s="11">
+        <v>1472.8</v>
+      </c>
+      <c r="Z176" s="12">
+        <v>566969088</v>
+      </c>
+      <c r="AA176" s="12">
+        <v>-57110471</v>
+      </c>
+      <c r="AB176" s="12">
+        <v>3686511</v>
       </c>
       <c r="AC176" s="9">
         <v>0</v>
       </c>
-      <c r="AD176" s="12">
-        <v>37760160</v>
-      </c>
-      <c r="AE176" s="12">
-        <v>37760160</v>
+      <c r="AD176" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE176" s="9">
+        <v>0</v>
       </c>
       <c r="AF176" s="9">
         <v>0</v>
@@ -17173,35 +17188,35 @@
         <v>46044</v>
       </c>
       <c r="B177" s="9" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="C177" s="10"/>
-      <c r="D177" s="9">
-        <v>9984</v>
+      <c r="D177" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="E177" s="9">
         <v>0</v>
       </c>
       <c r="F177" s="11">
-        <v>23000</v>
-      </c>
-      <c r="G177" s="11">
-        <v>4066.73</v>
+        <v>1400</v>
+      </c>
+      <c r="G177" s="9">
+        <v>432.53800000000001</v>
       </c>
       <c r="H177" s="11">
-        <v>93534900</v>
-      </c>
-      <c r="I177" s="11">
-        <v>4326</v>
+        <v>605554.04</v>
+      </c>
+      <c r="I177" s="9">
+        <v>449.36</v>
       </c>
       <c r="J177" s="11">
-        <v>99498000</v>
+        <v>629104</v>
       </c>
       <c r="K177" s="11">
-        <v>5963100</v>
+        <v>23549.96</v>
       </c>
       <c r="L177" s="12">
-        <v>59119786</v>
+        <v>50428786</v>
       </c>
       <c r="M177" s="9">
         <v>0</v>
@@ -17216,13 +17231,13 @@
         <v>0</v>
       </c>
       <c r="Q177" s="9" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="R177" s="9" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="S177" s="9" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="T177" s="10"/>
       <c r="U177" s="9">
@@ -17231,23 +17246,23 @@
       <c r="V177" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="W177" s="9">
-        <v>926.51</v>
+      <c r="W177" s="11">
+        <v>1446.79</v>
       </c>
       <c r="X177" s="12">
-        <v>866619555</v>
-      </c>
-      <c r="Y177" s="9">
-        <v>930.41</v>
+        <v>876115585</v>
+      </c>
+      <c r="Y177" s="11">
+        <v>1472.8</v>
       </c>
       <c r="Z177" s="12">
-        <v>925739341</v>
+        <v>926544371</v>
       </c>
       <c r="AA177" s="12">
-        <v>55481278</v>
+        <v>34684381</v>
       </c>
       <c r="AB177" s="12">
-        <v>3638508</v>
+        <v>15744405</v>
       </c>
       <c r="AC177" s="9">
         <v>0</v>
@@ -17267,35 +17282,35 @@
         <v>46044</v>
       </c>
       <c r="B178" s="9" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C178" s="10"/>
       <c r="D178" s="9" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E178" s="9">
         <v>0</v>
       </c>
       <c r="F178" s="11">
-        <v>10000</v>
+        <v>3500</v>
       </c>
       <c r="G178" s="9">
-        <v>48.203000000000003</v>
+        <v>169.042</v>
       </c>
       <c r="H178" s="11">
-        <v>482030</v>
+        <v>591649.80000000005</v>
       </c>
       <c r="I178" s="9">
-        <v>52</v>
+        <v>160.36000000000001</v>
       </c>
       <c r="J178" s="11">
-        <v>520000</v>
+        <v>561260</v>
       </c>
       <c r="K178" s="11">
-        <v>37970</v>
+        <v>-30389.8</v>
       </c>
       <c r="L178" s="12">
-        <v>64164929</v>
+        <v>-29375202</v>
       </c>
       <c r="M178" s="9">
         <v>0</v>
@@ -17316,7 +17331,7 @@
         <v>40</v>
       </c>
       <c r="S178" s="9" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="T178" s="10"/>
       <c r="U178" s="9">
@@ -17326,22 +17341,22 @@
         <v>34</v>
       </c>
       <c r="W178" s="11">
-        <v>1455.7</v>
+        <v>1446.79</v>
       </c>
       <c r="X178" s="12">
-        <v>701691071</v>
+        <v>855998930</v>
       </c>
       <c r="Y178" s="11">
         <v>1472.8</v>
       </c>
       <c r="Z178" s="12">
-        <v>765856000</v>
+        <v>826623728</v>
       </c>
       <c r="AA178" s="12">
-        <v>55922216</v>
+        <v>-44758097</v>
       </c>
       <c r="AB178" s="12">
-        <v>8242713</v>
+        <v>15382895</v>
       </c>
       <c r="AC178" s="9">
         <v>0</v>
@@ -17361,56 +17376,54 @@
         <v>46044</v>
       </c>
       <c r="B179" s="9" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="C179" s="10"/>
-      <c r="D179" s="9" t="s">
-        <v>77</v>
+      <c r="D179" s="9">
+        <v>6869</v>
       </c>
       <c r="E179" s="9">
         <v>0</v>
       </c>
-      <c r="F179" s="11">
-        <v>20000</v>
+      <c r="F179" s="9">
+        <v>0</v>
       </c>
       <c r="G179" s="9">
-        <v>34.24</v>
-      </c>
-      <c r="H179" s="11">
-        <v>684800</v>
-      </c>
-      <c r="I179" s="9">
-        <v>34.74</v>
-      </c>
-      <c r="J179" s="11">
-        <v>694800</v>
-      </c>
-      <c r="K179" s="11">
-        <v>10000</v>
-      </c>
-      <c r="L179" s="12">
-        <v>11851840</v>
+        <v>0</v>
+      </c>
+      <c r="H179" s="9">
+        <v>0</v>
+      </c>
+      <c r="I179" s="10"/>
+      <c r="J179" s="9">
+        <v>0</v>
+      </c>
+      <c r="K179" s="9">
+        <v>0</v>
+      </c>
+      <c r="L179" s="9">
+        <v>0</v>
       </c>
       <c r="M179" s="9">
         <v>0</v>
       </c>
-      <c r="N179" s="9">
-        <v>0</v>
-      </c>
-      <c r="O179" s="9">
-        <v>0</v>
+      <c r="N179" s="11">
+        <v>349976</v>
+      </c>
+      <c r="O179" s="11">
+        <v>349976</v>
       </c>
       <c r="P179" s="9">
         <v>0</v>
       </c>
       <c r="Q179" s="9" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="R179" s="9" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="S179" s="9" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="T179" s="10"/>
       <c r="U179" s="9">
@@ -17419,32 +17432,32 @@
       <c r="V179" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="W179" s="11">
-        <v>1477</v>
-      </c>
-      <c r="X179" s="12">
-        <v>1011449600</v>
-      </c>
-      <c r="Y179" s="11">
-        <v>1472.8</v>
-      </c>
-      <c r="Z179" s="12">
-        <v>1023301440</v>
-      </c>
-      <c r="AA179" s="12">
-        <v>14728000</v>
-      </c>
-      <c r="AB179" s="12">
-        <v>-2876160</v>
+      <c r="W179" s="9">
+        <v>0</v>
+      </c>
+      <c r="X179" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y179" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z179" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA179" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB179" s="9">
+        <v>0</v>
       </c>
       <c r="AC179" s="9">
         <v>0</v>
       </c>
-      <c r="AD179" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE179" s="9">
-        <v>0</v>
+      <c r="AD179" s="12">
+        <v>72042766</v>
+      </c>
+      <c r="AE179" s="12">
+        <v>72042766</v>
       </c>
       <c r="AF179" s="9">
         <v>0</v>
@@ -17455,35 +17468,35 @@
         <v>46044</v>
       </c>
       <c r="B180" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C180" s="10"/>
-      <c r="D180" s="9" t="s">
-        <v>80</v>
+      <c r="D180" s="9">
+        <v>2359</v>
       </c>
       <c r="E180" s="9">
         <v>0</v>
       </c>
       <c r="F180" s="11">
-        <v>3000</v>
+        <v>25000</v>
       </c>
       <c r="G180" s="9">
-        <v>247.65</v>
+        <v>118.559</v>
       </c>
       <c r="H180" s="11">
-        <v>742950</v>
+        <v>2963990</v>
       </c>
       <c r="I180" s="9">
-        <v>248.21</v>
+        <v>113.2</v>
       </c>
       <c r="J180" s="11">
-        <v>744630</v>
+        <v>2830000</v>
       </c>
       <c r="K180" s="11">
-        <v>1680</v>
+        <v>-133990</v>
       </c>
       <c r="L180" s="12">
-        <v>-646086</v>
+        <v>-25516850</v>
       </c>
       <c r="M180" s="9">
         <v>0</v>
@@ -17498,13 +17511,13 @@
         <v>0</v>
       </c>
       <c r="Q180" s="9" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="R180" s="9" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="S180" s="9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="T180" s="10"/>
       <c r="U180" s="9">
@@ -17513,23 +17526,23 @@
       <c r="V180" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="W180" s="11">
-        <v>1477</v>
+      <c r="W180" s="9">
+        <v>188.95</v>
       </c>
       <c r="X180" s="12">
-        <v>1097337150</v>
-      </c>
-      <c r="Y180" s="11">
-        <v>1472.8</v>
+        <v>560075550</v>
+      </c>
+      <c r="Y180" s="9">
+        <v>188.89</v>
       </c>
       <c r="Z180" s="12">
-        <v>1096691064</v>
+        <v>534558700</v>
       </c>
       <c r="AA180" s="12">
-        <v>2474304</v>
+        <v>-25309371</v>
       </c>
       <c r="AB180" s="12">
-        <v>-3120390</v>
+        <v>-207479</v>
       </c>
       <c r="AC180" s="9">
         <v>0</v>
@@ -17549,56 +17562,54 @@
         <v>46044</v>
       </c>
       <c r="B181" s="9" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="C181" s="10"/>
-      <c r="D181" s="9" t="s">
-        <v>55</v>
+      <c r="D181" s="9">
+        <v>6181</v>
       </c>
       <c r="E181" s="9">
         <v>0</v>
       </c>
-      <c r="F181" s="11">
-        <v>83000</v>
+      <c r="F181" s="9">
+        <v>0</v>
       </c>
       <c r="G181" s="9">
-        <v>12.374000000000001</v>
-      </c>
-      <c r="H181" s="11">
-        <v>1027042</v>
-      </c>
-      <c r="I181" s="9">
-        <v>11.1</v>
-      </c>
-      <c r="J181" s="11">
-        <v>921300</v>
-      </c>
-      <c r="K181" s="11">
-        <v>-105742</v>
-      </c>
-      <c r="L181" s="12">
-        <v>-127903979</v>
+        <v>0</v>
+      </c>
+      <c r="H181" s="9">
+        <v>0</v>
+      </c>
+      <c r="I181" s="10"/>
+      <c r="J181" s="9">
+        <v>0</v>
+      </c>
+      <c r="K181" s="9">
+        <v>0</v>
+      </c>
+      <c r="L181" s="9">
+        <v>0</v>
       </c>
       <c r="M181" s="9">
         <v>0</v>
       </c>
-      <c r="N181" s="9">
-        <v>0</v>
+      <c r="N181" s="11">
+        <v>-6374.88</v>
       </c>
       <c r="O181" s="9">
         <v>0</v>
       </c>
-      <c r="P181" s="9">
-        <v>0</v>
+      <c r="P181" s="11">
+        <v>6374.88</v>
       </c>
       <c r="Q181" s="9" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="R181" s="9" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="S181" s="9" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="T181" s="10"/>
       <c r="U181" s="9">
@@ -17607,32 +17618,32 @@
       <c r="V181" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="W181" s="11">
-        <v>1445.69</v>
-      </c>
-      <c r="X181" s="12">
-        <v>1484794619</v>
-      </c>
-      <c r="Y181" s="11">
-        <v>1472.8</v>
-      </c>
-      <c r="Z181" s="12">
-        <v>1356890640</v>
-      </c>
-      <c r="AA181" s="12">
-        <v>-155736817</v>
-      </c>
-      <c r="AB181" s="12">
-        <v>27832838</v>
+      <c r="W181" s="9">
+        <v>0</v>
+      </c>
+      <c r="X181" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y181" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z181" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA181" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB181" s="9">
+        <v>0</v>
       </c>
       <c r="AC181" s="9">
         <v>0</v>
       </c>
-      <c r="AD181" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE181" s="9">
-        <v>0</v>
+      <c r="AD181" s="12">
+        <v>1362525</v>
+      </c>
+      <c r="AE181" s="12">
+        <v>1362525</v>
       </c>
       <c r="AF181" s="9">
         <v>0</v>
@@ -17643,90 +17654,88 @@
         <v>46044</v>
       </c>
       <c r="B182" s="9" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C182" s="10"/>
-      <c r="D182" s="9" t="s">
-        <v>44</v>
+      <c r="D182" s="9">
+        <v>6082</v>
       </c>
       <c r="E182" s="9">
         <v>0</v>
       </c>
-      <c r="F182" s="11">
-        <v>2500</v>
+      <c r="F182" s="9">
+        <v>0</v>
       </c>
       <c r="G182" s="9">
-        <v>681.92</v>
-      </c>
-      <c r="H182" s="11">
-        <v>1704800</v>
-      </c>
-      <c r="I182" s="9">
-        <v>686.64</v>
-      </c>
-      <c r="J182" s="11">
-        <v>1716600</v>
-      </c>
-      <c r="K182" s="11">
-        <v>11800</v>
-      </c>
-      <c r="L182" s="12">
-        <v>81990960</v>
-      </c>
-      <c r="M182" s="11">
-        <v>8700</v>
+        <v>0</v>
+      </c>
+      <c r="H182" s="9">
+        <v>0</v>
+      </c>
+      <c r="I182" s="10"/>
+      <c r="J182" s="9">
+        <v>0</v>
+      </c>
+      <c r="K182" s="9">
+        <v>0</v>
+      </c>
+      <c r="L182" s="9">
+        <v>0</v>
+      </c>
+      <c r="M182" s="9">
+        <v>0</v>
       </c>
       <c r="N182" s="11">
-        <v>8700</v>
+        <v>205980</v>
       </c>
       <c r="O182" s="11">
-        <v>8700</v>
+        <v>205980</v>
       </c>
       <c r="P182" s="9">
         <v>0</v>
       </c>
       <c r="Q182" s="9" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="R182" s="9" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="S182" s="9" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="T182" s="10"/>
       <c r="U182" s="9">
         <v>0</v>
       </c>
       <c r="V182" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="W182" s="11">
-        <v>1434.9</v>
-      </c>
-      <c r="X182" s="12">
-        <v>2446217520</v>
-      </c>
-      <c r="Y182" s="11">
-        <v>1472.8</v>
-      </c>
-      <c r="Z182" s="12">
-        <v>2528208480</v>
-      </c>
-      <c r="AA182" s="12">
-        <v>17379040</v>
-      </c>
-      <c r="AB182" s="12">
-        <v>64611920</v>
-      </c>
-      <c r="AC182" s="12">
-        <v>84621980</v>
+        <v>34</v>
+      </c>
+      <c r="W182" s="9">
+        <v>0</v>
+      </c>
+      <c r="X182" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y182" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z182" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA182" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB182" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC182" s="9">
+        <v>0</v>
       </c>
       <c r="AD182" s="12">
-        <v>84621980</v>
+        <v>49395681</v>
       </c>
       <c r="AE182" s="12">
-        <v>84621980</v>
+        <v>49395681</v>
       </c>
       <c r="AF182" s="9">
         <v>0</v>
@@ -17737,35 +17746,35 @@
         <v>46044</v>
       </c>
       <c r="B183" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C183" s="10"/>
-      <c r="D183" s="9" t="s">
-        <v>38</v>
+      <c r="D183" s="9">
+        <v>9988</v>
       </c>
       <c r="E183" s="9">
         <v>0</v>
       </c>
       <c r="F183" s="11">
-        <v>4200</v>
+        <v>70500</v>
       </c>
       <c r="G183" s="9">
-        <v>396.31</v>
+        <v>147.79</v>
       </c>
       <c r="H183" s="11">
-        <v>1664502</v>
+        <v>10419200</v>
       </c>
       <c r="I183" s="9">
-        <v>441.25</v>
+        <v>164.8</v>
       </c>
       <c r="J183" s="11">
-        <v>1853250</v>
+        <v>11618400</v>
       </c>
       <c r="K183" s="11">
-        <v>188748</v>
+        <v>1199200</v>
       </c>
       <c r="L183" s="12">
-        <v>341072681</v>
+        <v>259800976</v>
       </c>
       <c r="M183" s="9">
         <v>0</v>
@@ -17780,38 +17789,38 @@
         <v>0</v>
       </c>
       <c r="Q183" s="9" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="R183" s="9" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="S183" s="9" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="T183" s="10"/>
       <c r="U183" s="9">
         <v>0</v>
       </c>
       <c r="V183" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="W183" s="11">
-        <v>1434.89</v>
+        <v>34</v>
+      </c>
+      <c r="W183" s="9">
+        <v>185.69</v>
       </c>
       <c r="X183" s="12">
-        <v>2388393919</v>
-      </c>
-      <c r="Y183" s="11">
-        <v>1472.8</v>
+        <v>1934798600</v>
+      </c>
+      <c r="Y183" s="9">
+        <v>188.89</v>
       </c>
       <c r="Z183" s="12">
-        <v>2729466600</v>
+        <v>2194599576</v>
       </c>
       <c r="AA183" s="12">
-        <v>277988054</v>
+        <v>226516888</v>
       </c>
       <c r="AB183" s="12">
-        <v>63084626</v>
+        <v>33284088</v>
       </c>
       <c r="AC183" s="9">
         <v>0</v>
@@ -17831,35 +17840,35 @@
         <v>46044</v>
       </c>
       <c r="B184" s="9" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C184" s="10"/>
-      <c r="D184" s="9" t="s">
-        <v>67</v>
+      <c r="D184" s="9">
+        <v>6861</v>
       </c>
       <c r="E184" s="9">
         <v>0</v>
       </c>
       <c r="F184" s="11">
-        <v>24000</v>
-      </c>
-      <c r="G184" s="9">
-        <v>17.655000000000001</v>
+        <v>1900</v>
+      </c>
+      <c r="G184" s="11">
+        <v>55916.79</v>
       </c>
       <c r="H184" s="11">
-        <v>423736.8</v>
-      </c>
-      <c r="I184" s="9">
-        <v>15.99</v>
+        <v>106241900</v>
+      </c>
+      <c r="I184" s="11">
+        <v>59310</v>
       </c>
       <c r="J184" s="11">
-        <v>383760</v>
+        <v>112689000</v>
       </c>
       <c r="K184" s="11">
-        <v>-39976.800000000003</v>
+        <v>6447100</v>
       </c>
       <c r="L184" s="12">
-        <v>-55191320</v>
+        <v>66305856</v>
       </c>
       <c r="M184" s="9">
         <v>0</v>
@@ -17874,13 +17883,13 @@
         <v>0</v>
       </c>
       <c r="Q184" s="9" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="R184" s="9" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="S184" s="9" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="T184" s="10"/>
       <c r="U184" s="9">
@@ -17889,23 +17898,23 @@
       <c r="V184" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="W184" s="11">
-        <v>1464.09</v>
+      <c r="W184" s="9">
+        <v>924.45</v>
       </c>
       <c r="X184" s="12">
-        <v>620393048</v>
-      </c>
-      <c r="Y184" s="11">
-        <v>1472.8</v>
+        <v>982163868</v>
+      </c>
+      <c r="Y184" s="9">
+        <v>930.41</v>
       </c>
       <c r="Z184" s="12">
-        <v>565201728</v>
+        <v>1048469724</v>
       </c>
       <c r="AA184" s="12">
-        <v>-58877831</v>
+        <v>59984463</v>
       </c>
       <c r="AB184" s="12">
-        <v>3686511</v>
+        <v>6321393</v>
       </c>
       <c r="AC184" s="9">
         <v>0</v>
@@ -17925,56 +17934,54 @@
         <v>46044</v>
       </c>
       <c r="B185" s="9" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="C185" s="10"/>
       <c r="D185" s="9" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="E185" s="9">
         <v>0</v>
       </c>
-      <c r="F185" s="11">
-        <v>1400</v>
+      <c r="F185" s="9">
+        <v>0</v>
       </c>
       <c r="G185" s="9">
-        <v>432.53800000000001</v>
-      </c>
-      <c r="H185" s="11">
-        <v>605554.04</v>
-      </c>
-      <c r="I185" s="9">
-        <v>433.75</v>
-      </c>
-      <c r="J185" s="11">
-        <v>607250</v>
-      </c>
-      <c r="K185" s="11">
-        <v>1695.96</v>
-      </c>
-      <c r="L185" s="12">
-        <v>18242215</v>
+        <v>0</v>
+      </c>
+      <c r="H185" s="9">
+        <v>0</v>
+      </c>
+      <c r="I185" s="10"/>
+      <c r="J185" s="9">
+        <v>0</v>
+      </c>
+      <c r="K185" s="9">
+        <v>0</v>
+      </c>
+      <c r="L185" s="9">
+        <v>0</v>
       </c>
       <c r="M185" s="9">
         <v>0</v>
       </c>
-      <c r="N185" s="9">
-        <v>0</v>
-      </c>
-      <c r="O185" s="9">
-        <v>0</v>
+      <c r="N185" s="11">
+        <v>4480700</v>
+      </c>
+      <c r="O185" s="11">
+        <v>4480700</v>
       </c>
       <c r="P185" s="9">
         <v>0</v>
       </c>
       <c r="Q185" s="9" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="R185" s="9" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="S185" s="9" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="T185" s="10"/>
       <c r="U185" s="9">
@@ -17983,32 +17990,32 @@
       <c r="V185" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="W185" s="11">
-        <v>1446.79</v>
-      </c>
-      <c r="X185" s="12">
-        <v>876115585</v>
-      </c>
-      <c r="Y185" s="11">
-        <v>1472.8</v>
-      </c>
-      <c r="Z185" s="12">
-        <v>894357800</v>
-      </c>
-      <c r="AA185" s="12">
-        <v>2497809</v>
-      </c>
-      <c r="AB185" s="12">
-        <v>15744405</v>
+      <c r="W185" s="9">
+        <v>0</v>
+      </c>
+      <c r="X185" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y185" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z185" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA185" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB185" s="9">
+        <v>0</v>
       </c>
       <c r="AC185" s="9">
         <v>0</v>
       </c>
-      <c r="AD185" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE185" s="9">
-        <v>0</v>
+      <c r="AD185" s="12">
+        <v>37760160</v>
+      </c>
+      <c r="AE185" s="12">
+        <v>37760160</v>
       </c>
       <c r="AF185" s="9">
         <v>0</v>
@@ -18019,35 +18026,35 @@
         <v>46044</v>
       </c>
       <c r="B186" s="9" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="C186" s="10"/>
-      <c r="D186" s="9" t="s">
-        <v>52</v>
+      <c r="D186" s="9">
+        <v>9984</v>
       </c>
       <c r="E186" s="9">
         <v>0</v>
       </c>
       <c r="F186" s="11">
-        <v>3500</v>
-      </c>
-      <c r="G186" s="9">
-        <v>169.042</v>
+        <v>23000</v>
+      </c>
+      <c r="G186" s="11">
+        <v>4066.73</v>
       </c>
       <c r="H186" s="11">
-        <v>591649.80000000005</v>
-      </c>
-      <c r="I186" s="9">
-        <v>161.18</v>
+        <v>93534900</v>
+      </c>
+      <c r="I186" s="11">
+        <v>4325</v>
       </c>
       <c r="J186" s="11">
-        <v>564130</v>
+        <v>99475000</v>
       </c>
       <c r="K186" s="11">
-        <v>-27519.8</v>
+        <v>5940100</v>
       </c>
       <c r="L186" s="12">
-        <v>-25148266</v>
+        <v>58905792</v>
       </c>
       <c r="M186" s="9">
         <v>0</v>
@@ -18062,13 +18069,13 @@
         <v>0</v>
       </c>
       <c r="Q186" s="9" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="R186" s="9" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="S186" s="9" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="T186" s="10"/>
       <c r="U186" s="9">
@@ -18077,23 +18084,23 @@
       <c r="V186" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="W186" s="11">
-        <v>1446.79</v>
+      <c r="W186" s="9">
+        <v>926.51</v>
       </c>
       <c r="X186" s="12">
-        <v>855998930</v>
-      </c>
-      <c r="Y186" s="11">
-        <v>1472.8</v>
+        <v>866619555</v>
+      </c>
+      <c r="Y186" s="9">
+        <v>930.41</v>
       </c>
       <c r="Z186" s="12">
-        <v>830850664</v>
+        <v>925525347</v>
       </c>
       <c r="AA186" s="12">
-        <v>-40531161</v>
+        <v>55267284</v>
       </c>
       <c r="AB186" s="12">
-        <v>15382895</v>
+        <v>3638508</v>
       </c>
       <c r="AC186" s="9">
         <v>0</v>

</xml_diff>

<commit_message>
Update 2026_멀티.xlsx (2026-01-23 15:47:13)
</commit_message>
<xml_diff>
--- a/2026_멀티.xlsx
+++ b/2026_멀티.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyejinha/Desktop/Workspace/Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D61DA59-81A7-FD41-BB33-70A55DA85EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EAFBA28-31D3-774C-AAB7-BC0727DA8A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="17060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="29000" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="89">
   <si>
     <t>기준일자</t>
   </si>
@@ -286,6 +286,12 @@
   </si>
   <si>
     <t>BABA-W</t>
+  </si>
+  <si>
+    <t>CNE1000055Y4</t>
+  </si>
+  <si>
+    <t>JLMAG</t>
   </si>
 </sst>
 </file>
@@ -666,7 +672,7 @@
   <dimension ref="A1:AF1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="A170" sqref="A170:AF186"/>
+      <selection activeCell="A187" sqref="A187:AF204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -18021,7 +18027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:32" ht="18" thickBot="1">
+    <row r="186" spans="1:32">
       <c r="A186" s="8">
         <v>46044</v>
       </c>
@@ -18115,617 +18121,1697 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:32" ht="18" thickBot="1">
-      <c r="A187" s="3"/>
-      <c r="B187" s="4"/>
-      <c r="C187" s="2"/>
-      <c r="D187" s="1"/>
-      <c r="E187" s="5"/>
-      <c r="F187" s="6"/>
-      <c r="G187" s="5"/>
-      <c r="H187" s="6"/>
-      <c r="I187" s="5"/>
-      <c r="J187" s="6"/>
-      <c r="K187" s="6"/>
-      <c r="L187" s="7"/>
-      <c r="M187" s="5"/>
-      <c r="N187" s="5"/>
-      <c r="O187" s="5"/>
-      <c r="P187" s="5"/>
-      <c r="Q187" s="1"/>
-      <c r="R187" s="1"/>
-      <c r="S187" s="4"/>
-      <c r="T187" s="2"/>
-      <c r="U187" s="5"/>
-      <c r="V187" s="1"/>
-      <c r="W187" s="6"/>
-      <c r="X187" s="7"/>
-      <c r="Y187" s="6"/>
-      <c r="Z187" s="7"/>
-      <c r="AA187" s="7"/>
-      <c r="AB187" s="7"/>
-      <c r="AC187" s="5"/>
-      <c r="AD187" s="5"/>
-      <c r="AE187" s="5"/>
-      <c r="AF187" s="5"/>
-    </row>
-    <row r="188" spans="1:32" ht="18" thickBot="1">
-      <c r="A188" s="3"/>
-      <c r="B188" s="4"/>
-      <c r="C188" s="2"/>
-      <c r="D188" s="5"/>
-      <c r="E188" s="5"/>
-      <c r="F188" s="6"/>
-      <c r="G188" s="5"/>
-      <c r="H188" s="6"/>
-      <c r="I188" s="5"/>
-      <c r="J188" s="6"/>
-      <c r="K188" s="6"/>
-      <c r="L188" s="7"/>
-      <c r="M188" s="5"/>
-      <c r="N188" s="5"/>
-      <c r="O188" s="5"/>
-      <c r="P188" s="5"/>
-      <c r="Q188" s="1"/>
-      <c r="R188" s="1"/>
-      <c r="S188" s="1"/>
-      <c r="T188" s="2"/>
-      <c r="U188" s="5"/>
-      <c r="V188" s="1"/>
-      <c r="W188" s="5"/>
-      <c r="X188" s="7"/>
-      <c r="Y188" s="5"/>
-      <c r="Z188" s="7"/>
-      <c r="AA188" s="7"/>
-      <c r="AB188" s="7"/>
-      <c r="AC188" s="5"/>
-      <c r="AD188" s="5"/>
-      <c r="AE188" s="5"/>
-      <c r="AF188" s="5"/>
-    </row>
-    <row r="189" spans="1:32" ht="18" thickBot="1">
-      <c r="A189" s="3"/>
-      <c r="B189" s="4"/>
-      <c r="C189" s="2"/>
-      <c r="D189" s="5"/>
-      <c r="E189" s="5"/>
-      <c r="F189" s="6"/>
-      <c r="G189" s="5"/>
-      <c r="H189" s="6"/>
-      <c r="I189" s="5"/>
-      <c r="J189" s="6"/>
-      <c r="K189" s="6"/>
-      <c r="L189" s="7"/>
-      <c r="M189" s="5"/>
-      <c r="N189" s="5"/>
-      <c r="O189" s="5"/>
-      <c r="P189" s="5"/>
-      <c r="Q189" s="1"/>
-      <c r="R189" s="1"/>
-      <c r="S189" s="4"/>
-      <c r="T189" s="2"/>
-      <c r="U189" s="5"/>
-      <c r="V189" s="1"/>
-      <c r="W189" s="5"/>
-      <c r="X189" s="7"/>
-      <c r="Y189" s="5"/>
-      <c r="Z189" s="7"/>
-      <c r="AA189" s="7"/>
-      <c r="AB189" s="7"/>
-      <c r="AC189" s="5"/>
-      <c r="AD189" s="5"/>
-      <c r="AE189" s="5"/>
-      <c r="AF189" s="5"/>
-    </row>
-    <row r="190" spans="1:32" ht="18" thickBot="1">
-      <c r="A190" s="3"/>
-      <c r="B190" s="4"/>
-      <c r="C190" s="2"/>
-      <c r="D190" s="5"/>
-      <c r="E190" s="5"/>
-      <c r="F190" s="6"/>
-      <c r="G190" s="5"/>
-      <c r="H190" s="6"/>
-      <c r="I190" s="5"/>
-      <c r="J190" s="6"/>
-      <c r="K190" s="6"/>
-      <c r="L190" s="7"/>
-      <c r="M190" s="5"/>
-      <c r="N190" s="5"/>
-      <c r="O190" s="5"/>
-      <c r="P190" s="5"/>
-      <c r="Q190" s="1"/>
-      <c r="R190" s="1"/>
-      <c r="S190" s="1"/>
-      <c r="T190" s="2"/>
-      <c r="U190" s="5"/>
-      <c r="V190" s="1"/>
-      <c r="W190" s="5"/>
-      <c r="X190" s="7"/>
-      <c r="Y190" s="5"/>
-      <c r="Z190" s="7"/>
-      <c r="AA190" s="7"/>
-      <c r="AB190" s="7"/>
-      <c r="AC190" s="5"/>
-      <c r="AD190" s="5"/>
-      <c r="AE190" s="5"/>
-      <c r="AF190" s="5"/>
-    </row>
-    <row r="191" spans="1:32" ht="18" thickBot="1">
-      <c r="A191" s="3"/>
-      <c r="B191" s="4"/>
-      <c r="C191" s="2"/>
-      <c r="D191" s="5"/>
-      <c r="E191" s="5"/>
-      <c r="F191" s="6"/>
-      <c r="G191" s="6"/>
-      <c r="H191" s="6"/>
-      <c r="I191" s="6"/>
-      <c r="J191" s="6"/>
-      <c r="K191" s="6"/>
-      <c r="L191" s="7"/>
-      <c r="M191" s="5"/>
-      <c r="N191" s="5"/>
-      <c r="O191" s="5"/>
-      <c r="P191" s="5"/>
-      <c r="Q191" s="1"/>
-      <c r="R191" s="1"/>
-      <c r="S191" s="1"/>
-      <c r="T191" s="2"/>
-      <c r="U191" s="5"/>
-      <c r="V191" s="1"/>
-      <c r="W191" s="5"/>
-      <c r="X191" s="7"/>
-      <c r="Y191" s="5"/>
-      <c r="Z191" s="7"/>
-      <c r="AA191" s="7"/>
-      <c r="AB191" s="7"/>
-      <c r="AC191" s="5"/>
-      <c r="AD191" s="5"/>
-      <c r="AE191" s="5"/>
-      <c r="AF191" s="5"/>
-    </row>
-    <row r="192" spans="1:32" ht="18" thickBot="1">
-      <c r="A192" s="3"/>
-      <c r="B192" s="4"/>
-      <c r="C192" s="2"/>
-      <c r="D192" s="5"/>
-      <c r="E192" s="5"/>
-      <c r="F192" s="6"/>
-      <c r="G192" s="6"/>
-      <c r="H192" s="6"/>
-      <c r="I192" s="6"/>
-      <c r="J192" s="6"/>
-      <c r="K192" s="6"/>
-      <c r="L192" s="7"/>
-      <c r="M192" s="5"/>
-      <c r="N192" s="5"/>
-      <c r="O192" s="5"/>
-      <c r="P192" s="5"/>
-      <c r="Q192" s="1"/>
-      <c r="R192" s="1"/>
-      <c r="S192" s="1"/>
-      <c r="T192" s="2"/>
-      <c r="U192" s="5"/>
-      <c r="V192" s="1"/>
-      <c r="W192" s="5"/>
-      <c r="X192" s="7"/>
-      <c r="Y192" s="5"/>
-      <c r="Z192" s="7"/>
-      <c r="AA192" s="7"/>
-      <c r="AB192" s="7"/>
-      <c r="AC192" s="5"/>
-      <c r="AD192" s="5"/>
-      <c r="AE192" s="5"/>
-      <c r="AF192" s="5"/>
-    </row>
-    <row r="193" spans="1:32" ht="18" thickBot="1">
-      <c r="A193" s="3"/>
-      <c r="B193" s="4"/>
-      <c r="C193" s="2"/>
-      <c r="D193" s="1"/>
-      <c r="E193" s="5"/>
-      <c r="F193" s="6"/>
-      <c r="G193" s="5"/>
-      <c r="H193" s="6"/>
-      <c r="I193" s="5"/>
-      <c r="J193" s="6"/>
-      <c r="K193" s="6"/>
-      <c r="L193" s="7"/>
-      <c r="M193" s="5"/>
-      <c r="N193" s="5"/>
-      <c r="O193" s="5"/>
-      <c r="P193" s="5"/>
-      <c r="Q193" s="1"/>
-      <c r="R193" s="1"/>
-      <c r="S193" s="4"/>
-      <c r="T193" s="2"/>
-      <c r="U193" s="5"/>
-      <c r="V193" s="1"/>
-      <c r="W193" s="6"/>
-      <c r="X193" s="7"/>
-      <c r="Y193" s="6"/>
-      <c r="Z193" s="7"/>
-      <c r="AA193" s="7"/>
-      <c r="AB193" s="7"/>
-      <c r="AC193" s="5"/>
-      <c r="AD193" s="5"/>
-      <c r="AE193" s="5"/>
-      <c r="AF193" s="5"/>
-    </row>
-    <row r="194" spans="1:32" ht="18" thickBot="1">
-      <c r="A194" s="3"/>
-      <c r="B194" s="4"/>
-      <c r="C194" s="2"/>
-      <c r="D194" s="1"/>
-      <c r="E194" s="5"/>
-      <c r="F194" s="6"/>
-      <c r="G194" s="5"/>
-      <c r="H194" s="6"/>
-      <c r="I194" s="5"/>
-      <c r="J194" s="6"/>
-      <c r="K194" s="6"/>
-      <c r="L194" s="7"/>
-      <c r="M194" s="5"/>
-      <c r="N194" s="5"/>
-      <c r="O194" s="5"/>
-      <c r="P194" s="5"/>
-      <c r="Q194" s="1"/>
-      <c r="R194" s="1"/>
-      <c r="S194" s="1"/>
-      <c r="T194" s="2"/>
-      <c r="U194" s="5"/>
-      <c r="V194" s="1"/>
-      <c r="W194" s="6"/>
-      <c r="X194" s="7"/>
-      <c r="Y194" s="6"/>
-      <c r="Z194" s="7"/>
-      <c r="AA194" s="7"/>
-      <c r="AB194" s="7"/>
-      <c r="AC194" s="5"/>
-      <c r="AD194" s="5"/>
-      <c r="AE194" s="5"/>
-      <c r="AF194" s="5"/>
-    </row>
-    <row r="195" spans="1:32" ht="18" thickBot="1">
-      <c r="A195" s="3"/>
-      <c r="B195" s="4"/>
-      <c r="C195" s="2"/>
-      <c r="D195" s="1"/>
-      <c r="E195" s="5"/>
-      <c r="F195" s="6"/>
-      <c r="G195" s="5"/>
-      <c r="H195" s="6"/>
-      <c r="I195" s="5"/>
-      <c r="J195" s="6"/>
-      <c r="K195" s="6"/>
-      <c r="L195" s="7"/>
-      <c r="M195" s="5"/>
-      <c r="N195" s="5"/>
-      <c r="O195" s="5"/>
-      <c r="P195" s="5"/>
-      <c r="Q195" s="1"/>
-      <c r="R195" s="1"/>
-      <c r="S195" s="1"/>
-      <c r="T195" s="2"/>
-      <c r="U195" s="5"/>
-      <c r="V195" s="1"/>
-      <c r="W195" s="6"/>
-      <c r="X195" s="7"/>
-      <c r="Y195" s="6"/>
-      <c r="Z195" s="7"/>
-      <c r="AA195" s="7"/>
-      <c r="AB195" s="7"/>
-      <c r="AC195" s="5"/>
-      <c r="AD195" s="5"/>
-      <c r="AE195" s="5"/>
-      <c r="AF195" s="5"/>
-    </row>
-    <row r="196" spans="1:32" ht="18" thickBot="1">
-      <c r="A196" s="3"/>
-      <c r="B196" s="4"/>
-      <c r="C196" s="2"/>
-      <c r="D196" s="1"/>
-      <c r="E196" s="5"/>
-      <c r="F196" s="6"/>
-      <c r="G196" s="5"/>
-      <c r="H196" s="6"/>
-      <c r="I196" s="5"/>
-      <c r="J196" s="6"/>
-      <c r="K196" s="6"/>
-      <c r="L196" s="7"/>
-      <c r="M196" s="5"/>
-      <c r="N196" s="5"/>
-      <c r="O196" s="5"/>
-      <c r="P196" s="5"/>
-      <c r="Q196" s="1"/>
-      <c r="R196" s="1"/>
-      <c r="S196" s="1"/>
-      <c r="T196" s="2"/>
-      <c r="U196" s="5"/>
-      <c r="V196" s="1"/>
-      <c r="W196" s="6"/>
-      <c r="X196" s="7"/>
-      <c r="Y196" s="6"/>
-      <c r="Z196" s="7"/>
-      <c r="AA196" s="7"/>
-      <c r="AB196" s="7"/>
-      <c r="AC196" s="5"/>
-      <c r="AD196" s="5"/>
-      <c r="AE196" s="5"/>
-      <c r="AF196" s="5"/>
-    </row>
-    <row r="197" spans="1:32" ht="18" thickBot="1">
-      <c r="A197" s="3"/>
-      <c r="B197" s="4"/>
-      <c r="C197" s="2"/>
-      <c r="D197" s="1"/>
-      <c r="E197" s="5"/>
-      <c r="F197" s="6"/>
-      <c r="G197" s="5"/>
-      <c r="H197" s="6"/>
-      <c r="I197" s="5"/>
-      <c r="J197" s="6"/>
-      <c r="K197" s="6"/>
-      <c r="L197" s="7"/>
-      <c r="M197" s="5"/>
-      <c r="N197" s="5"/>
-      <c r="O197" s="5"/>
-      <c r="P197" s="5"/>
-      <c r="Q197" s="1"/>
-      <c r="R197" s="1"/>
-      <c r="S197" s="4"/>
-      <c r="T197" s="2"/>
-      <c r="U197" s="5"/>
-      <c r="V197" s="1"/>
-      <c r="W197" s="6"/>
-      <c r="X197" s="7"/>
-      <c r="Y197" s="6"/>
-      <c r="Z197" s="7"/>
-      <c r="AA197" s="7"/>
-      <c r="AB197" s="7"/>
-      <c r="AC197" s="5"/>
-      <c r="AD197" s="5"/>
-      <c r="AE197" s="5"/>
-      <c r="AF197" s="5"/>
-    </row>
-    <row r="198" spans="1:32" ht="18" thickBot="1">
-      <c r="A198" s="3"/>
-      <c r="B198" s="4"/>
-      <c r="C198" s="2"/>
-      <c r="D198" s="1"/>
-      <c r="E198" s="5"/>
-      <c r="F198" s="6"/>
-      <c r="G198" s="5"/>
-      <c r="H198" s="6"/>
-      <c r="I198" s="5"/>
-      <c r="J198" s="6"/>
-      <c r="K198" s="6"/>
-      <c r="L198" s="7"/>
-      <c r="M198" s="5"/>
-      <c r="N198" s="5"/>
-      <c r="O198" s="5"/>
-      <c r="P198" s="5"/>
-      <c r="Q198" s="1"/>
-      <c r="R198" s="1"/>
-      <c r="S198" s="4"/>
-      <c r="T198" s="2"/>
-      <c r="U198" s="5"/>
-      <c r="V198" s="1"/>
-      <c r="W198" s="6"/>
-      <c r="X198" s="7"/>
-      <c r="Y198" s="6"/>
-      <c r="Z198" s="7"/>
-      <c r="AA198" s="7"/>
-      <c r="AB198" s="7"/>
-      <c r="AC198" s="5"/>
-      <c r="AD198" s="5"/>
-      <c r="AE198" s="5"/>
-      <c r="AF198" s="5"/>
-    </row>
-    <row r="199" spans="1:32" ht="18" thickBot="1">
-      <c r="A199" s="3"/>
-      <c r="B199" s="4"/>
-      <c r="C199" s="2"/>
-      <c r="D199" s="1"/>
-      <c r="E199" s="5"/>
-      <c r="F199" s="6"/>
-      <c r="G199" s="5"/>
-      <c r="H199" s="6"/>
-      <c r="I199" s="5"/>
-      <c r="J199" s="6"/>
-      <c r="K199" s="6"/>
-      <c r="L199" s="7"/>
-      <c r="M199" s="5"/>
-      <c r="N199" s="5"/>
-      <c r="O199" s="5"/>
-      <c r="P199" s="5"/>
-      <c r="Q199" s="1"/>
-      <c r="R199" s="1"/>
-      <c r="S199" s="4"/>
-      <c r="T199" s="2"/>
-      <c r="U199" s="5"/>
-      <c r="V199" s="1"/>
-      <c r="W199" s="6"/>
-      <c r="X199" s="7"/>
-      <c r="Y199" s="6"/>
-      <c r="Z199" s="7"/>
-      <c r="AA199" s="7"/>
-      <c r="AB199" s="7"/>
-      <c r="AC199" s="5"/>
-      <c r="AD199" s="5"/>
-      <c r="AE199" s="5"/>
-      <c r="AF199" s="5"/>
-    </row>
-    <row r="200" spans="1:32" ht="18" thickBot="1">
-      <c r="A200" s="3"/>
-      <c r="B200" s="4"/>
-      <c r="C200" s="2"/>
-      <c r="D200" s="1"/>
-      <c r="E200" s="5"/>
-      <c r="F200" s="6"/>
-      <c r="G200" s="5"/>
-      <c r="H200" s="6"/>
-      <c r="I200" s="5"/>
-      <c r="J200" s="6"/>
-      <c r="K200" s="6"/>
-      <c r="L200" s="7"/>
-      <c r="M200" s="5"/>
-      <c r="N200" s="5"/>
-      <c r="O200" s="5"/>
-      <c r="P200" s="5"/>
-      <c r="Q200" s="1"/>
-      <c r="R200" s="1"/>
-      <c r="S200" s="4"/>
-      <c r="T200" s="2"/>
-      <c r="U200" s="5"/>
-      <c r="V200" s="1"/>
-      <c r="W200" s="6"/>
-      <c r="X200" s="7"/>
-      <c r="Y200" s="6"/>
-      <c r="Z200" s="7"/>
-      <c r="AA200" s="7"/>
-      <c r="AB200" s="7"/>
-      <c r="AC200" s="5"/>
-      <c r="AD200" s="5"/>
-      <c r="AE200" s="5"/>
-      <c r="AF200" s="5"/>
-    </row>
-    <row r="201" spans="1:32" ht="18" thickBot="1">
-      <c r="A201" s="3"/>
-      <c r="B201" s="4"/>
-      <c r="C201" s="2"/>
-      <c r="D201" s="1"/>
-      <c r="E201" s="5"/>
-      <c r="F201" s="6"/>
-      <c r="G201" s="5"/>
-      <c r="H201" s="6"/>
-      <c r="I201" s="5"/>
-      <c r="J201" s="6"/>
-      <c r="K201" s="6"/>
-      <c r="L201" s="7"/>
-      <c r="M201" s="5"/>
-      <c r="N201" s="5"/>
-      <c r="O201" s="5"/>
-      <c r="P201" s="5"/>
-      <c r="Q201" s="1"/>
-      <c r="R201" s="1"/>
-      <c r="S201" s="4"/>
-      <c r="T201" s="2"/>
-      <c r="U201" s="5"/>
-      <c r="V201" s="1"/>
-      <c r="W201" s="6"/>
-      <c r="X201" s="7"/>
-      <c r="Y201" s="6"/>
-      <c r="Z201" s="7"/>
-      <c r="AA201" s="7"/>
-      <c r="AB201" s="7"/>
-      <c r="AC201" s="5"/>
-      <c r="AD201" s="5"/>
-      <c r="AE201" s="5"/>
-      <c r="AF201" s="5"/>
-    </row>
-    <row r="202" spans="1:32" ht="18" thickBot="1">
-      <c r="A202" s="3"/>
-      <c r="B202" s="4"/>
-      <c r="C202" s="2"/>
-      <c r="D202" s="1"/>
-      <c r="E202" s="5"/>
-      <c r="F202" s="5"/>
-      <c r="G202" s="6"/>
-      <c r="H202" s="6"/>
-      <c r="I202" s="6"/>
-      <c r="J202" s="6"/>
-      <c r="K202" s="6"/>
-      <c r="L202" s="7"/>
-      <c r="M202" s="5"/>
-      <c r="N202" s="5"/>
-      <c r="O202" s="5"/>
-      <c r="P202" s="5"/>
-      <c r="Q202" s="1"/>
-      <c r="R202" s="1"/>
-      <c r="S202" s="1"/>
-      <c r="T202" s="2"/>
-      <c r="U202" s="5"/>
-      <c r="V202" s="1"/>
-      <c r="W202" s="6"/>
-      <c r="X202" s="7"/>
-      <c r="Y202" s="6"/>
-      <c r="Z202" s="7"/>
-      <c r="AA202" s="7"/>
-      <c r="AB202" s="7"/>
-      <c r="AC202" s="5"/>
-      <c r="AD202" s="5"/>
-      <c r="AE202" s="5"/>
-      <c r="AF202" s="5"/>
-    </row>
-    <row r="203" spans="1:32" ht="18" thickBot="1">
-      <c r="A203" s="3"/>
-      <c r="B203" s="4"/>
-      <c r="C203" s="2"/>
-      <c r="D203" s="1"/>
-      <c r="E203" s="5"/>
-      <c r="F203" s="6"/>
-      <c r="G203" s="5"/>
-      <c r="H203" s="6"/>
-      <c r="I203" s="5"/>
-      <c r="J203" s="6"/>
-      <c r="K203" s="6"/>
-      <c r="L203" s="7"/>
-      <c r="M203" s="5"/>
-      <c r="N203" s="5"/>
-      <c r="O203" s="5"/>
-      <c r="P203" s="5"/>
-      <c r="Q203" s="1"/>
-      <c r="R203" s="1"/>
-      <c r="S203" s="1"/>
-      <c r="T203" s="2"/>
-      <c r="U203" s="5"/>
-      <c r="V203" s="1"/>
-      <c r="W203" s="6"/>
-      <c r="X203" s="7"/>
-      <c r="Y203" s="6"/>
-      <c r="Z203" s="7"/>
-      <c r="AA203" s="7"/>
-      <c r="AB203" s="7"/>
-      <c r="AC203" s="5"/>
-      <c r="AD203" s="5"/>
-      <c r="AE203" s="5"/>
-      <c r="AF203" s="5"/>
+    <row r="187" spans="1:32">
+      <c r="A187" s="8">
+        <v>46045</v>
+      </c>
+      <c r="B187" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C187" s="10"/>
+      <c r="D187" s="9">
+        <v>6869</v>
+      </c>
+      <c r="E187" s="9">
+        <v>0</v>
+      </c>
+      <c r="F187" s="9">
+        <v>0</v>
+      </c>
+      <c r="G187" s="9">
+        <v>0</v>
+      </c>
+      <c r="H187" s="9">
+        <v>0</v>
+      </c>
+      <c r="I187" s="9">
+        <v>54.1</v>
+      </c>
+      <c r="J187" s="9">
+        <v>0</v>
+      </c>
+      <c r="K187" s="9">
+        <v>0</v>
+      </c>
+      <c r="L187" s="9">
+        <v>0</v>
+      </c>
+      <c r="M187" s="9">
+        <v>0</v>
+      </c>
+      <c r="N187" s="11">
+        <v>349976</v>
+      </c>
+      <c r="O187" s="11">
+        <v>349976</v>
+      </c>
+      <c r="P187" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q187" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="R187" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="S187" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="T187" s="10"/>
+      <c r="U187" s="9">
+        <v>0</v>
+      </c>
+      <c r="V187" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W187" s="9">
+        <v>0</v>
+      </c>
+      <c r="X187" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y187" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z187" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA187" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB187" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC187" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD187" s="12">
+        <v>72042766</v>
+      </c>
+      <c r="AE187" s="12">
+        <v>72042766</v>
+      </c>
+      <c r="AF187" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:32">
+      <c r="A188" s="8">
+        <v>46045</v>
+      </c>
+      <c r="B188" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C188" s="10"/>
+      <c r="D188" s="9">
+        <v>2359</v>
+      </c>
+      <c r="E188" s="9">
+        <v>0</v>
+      </c>
+      <c r="F188" s="11">
+        <v>25000</v>
+      </c>
+      <c r="G188" s="9">
+        <v>118.559</v>
+      </c>
+      <c r="H188" s="11">
+        <v>2963990</v>
+      </c>
+      <c r="I188" s="9">
+        <v>113.7</v>
+      </c>
+      <c r="J188" s="11">
+        <v>2842500</v>
+      </c>
+      <c r="K188" s="11">
+        <v>-121490</v>
+      </c>
+      <c r="L188" s="12">
+        <v>-24719100</v>
+      </c>
+      <c r="M188" s="9">
+        <v>0</v>
+      </c>
+      <c r="N188" s="9">
+        <v>0</v>
+      </c>
+      <c r="O188" s="9">
+        <v>0</v>
+      </c>
+      <c r="P188" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q188" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="R188" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="S188" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="T188" s="10"/>
+      <c r="U188" s="9">
+        <v>0</v>
+      </c>
+      <c r="V188" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W188" s="9">
+        <v>188.95</v>
+      </c>
+      <c r="X188" s="12">
+        <v>560075550</v>
+      </c>
+      <c r="Y188" s="9">
+        <v>188.34</v>
+      </c>
+      <c r="Z188" s="12">
+        <v>535356450</v>
+      </c>
+      <c r="AA188" s="12">
+        <v>-22881426</v>
+      </c>
+      <c r="AB188" s="12">
+        <v>-1837674</v>
+      </c>
+      <c r="AC188" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD188" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE188" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF188" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:32">
+      <c r="A189" s="8">
+        <v>46045</v>
+      </c>
+      <c r="B189" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C189" s="10"/>
+      <c r="D189" s="9">
+        <v>6680</v>
+      </c>
+      <c r="E189" s="9">
+        <v>0</v>
+      </c>
+      <c r="F189" s="11">
+        <v>130000</v>
+      </c>
+      <c r="G189" s="9">
+        <v>22.469000000000001</v>
+      </c>
+      <c r="H189" s="11">
+        <v>2921022</v>
+      </c>
+      <c r="I189" s="9">
+        <v>23.82</v>
+      </c>
+      <c r="J189" s="11">
+        <v>3096600</v>
+      </c>
+      <c r="K189" s="11">
+        <v>175578</v>
+      </c>
+      <c r="L189" s="12">
+        <v>31461799</v>
+      </c>
+      <c r="M189" s="9">
+        <v>0</v>
+      </c>
+      <c r="N189" s="9">
+        <v>0</v>
+      </c>
+      <c r="O189" s="9">
+        <v>0</v>
+      </c>
+      <c r="P189" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q189" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="R189" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="S189" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="T189" s="10"/>
+      <c r="U189" s="9">
+        <v>0</v>
+      </c>
+      <c r="V189" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W189" s="9">
+        <v>188.88</v>
+      </c>
+      <c r="X189" s="12">
+        <v>551751845</v>
+      </c>
+      <c r="Y189" s="9">
+        <v>188.34</v>
+      </c>
+      <c r="Z189" s="12">
+        <v>583213644</v>
+      </c>
+      <c r="AA189" s="12">
+        <v>33068360</v>
+      </c>
+      <c r="AB189" s="12">
+        <v>-1606562</v>
+      </c>
+      <c r="AC189" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD189" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE189" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF189" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:32">
+      <c r="A190" s="8">
+        <v>46045</v>
+      </c>
+      <c r="B190" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C190" s="10"/>
+      <c r="D190" s="9">
+        <v>6181</v>
+      </c>
+      <c r="E190" s="9">
+        <v>0</v>
+      </c>
+      <c r="F190" s="9">
+        <v>0</v>
+      </c>
+      <c r="G190" s="9">
+        <v>0</v>
+      </c>
+      <c r="H190" s="9">
+        <v>0</v>
+      </c>
+      <c r="I190" s="9">
+        <v>788.5</v>
+      </c>
+      <c r="J190" s="9">
+        <v>0</v>
+      </c>
+      <c r="K190" s="9">
+        <v>0</v>
+      </c>
+      <c r="L190" s="9">
+        <v>0</v>
+      </c>
+      <c r="M190" s="9">
+        <v>0</v>
+      </c>
+      <c r="N190" s="11">
+        <v>-6374.88</v>
+      </c>
+      <c r="O190" s="9">
+        <v>0</v>
+      </c>
+      <c r="P190" s="11">
+        <v>6374.88</v>
+      </c>
+      <c r="Q190" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="R190" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="S190" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="T190" s="10"/>
+      <c r="U190" s="9">
+        <v>0</v>
+      </c>
+      <c r="V190" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W190" s="9">
+        <v>0</v>
+      </c>
+      <c r="X190" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y190" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z190" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA190" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB190" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC190" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD190" s="12">
+        <v>1362525</v>
+      </c>
+      <c r="AE190" s="12">
+        <v>1362525</v>
+      </c>
+      <c r="AF190" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:32">
+      <c r="A191" s="8">
+        <v>46045</v>
+      </c>
+      <c r="B191" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C191" s="10"/>
+      <c r="D191" s="9">
+        <v>6082</v>
+      </c>
+      <c r="E191" s="9">
+        <v>0</v>
+      </c>
+      <c r="F191" s="9">
+        <v>0</v>
+      </c>
+      <c r="G191" s="9">
+        <v>0</v>
+      </c>
+      <c r="H191" s="9">
+        <v>0</v>
+      </c>
+      <c r="I191" s="9">
+        <v>35.840000000000003</v>
+      </c>
+      <c r="J191" s="9">
+        <v>0</v>
+      </c>
+      <c r="K191" s="9">
+        <v>0</v>
+      </c>
+      <c r="L191" s="9">
+        <v>0</v>
+      </c>
+      <c r="M191" s="9">
+        <v>0</v>
+      </c>
+      <c r="N191" s="11">
+        <v>205980</v>
+      </c>
+      <c r="O191" s="11">
+        <v>205980</v>
+      </c>
+      <c r="P191" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q191" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="R191" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="S191" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="T191" s="10"/>
+      <c r="U191" s="9">
+        <v>0</v>
+      </c>
+      <c r="V191" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W191" s="9">
+        <v>0</v>
+      </c>
+      <c r="X191" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y191" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z191" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA191" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB191" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC191" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD191" s="12">
+        <v>49395681</v>
+      </c>
+      <c r="AE191" s="12">
+        <v>49395681</v>
+      </c>
+      <c r="AF191" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:32">
+      <c r="A192" s="8">
+        <v>46045</v>
+      </c>
+      <c r="B192" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C192" s="10"/>
+      <c r="D192" s="9">
+        <v>9988</v>
+      </c>
+      <c r="E192" s="9">
+        <v>0</v>
+      </c>
+      <c r="F192" s="11">
+        <v>70500</v>
+      </c>
+      <c r="G192" s="9">
+        <v>147.79</v>
+      </c>
+      <c r="H192" s="11">
+        <v>10419200</v>
+      </c>
+      <c r="I192" s="9">
+        <v>169.2</v>
+      </c>
+      <c r="J192" s="11">
+        <v>11928600</v>
+      </c>
+      <c r="K192" s="11">
+        <v>1509400</v>
+      </c>
+      <c r="L192" s="12">
+        <v>311833924</v>
+      </c>
+      <c r="M192" s="9">
+        <v>0</v>
+      </c>
+      <c r="N192" s="9">
+        <v>0</v>
+      </c>
+      <c r="O192" s="9">
+        <v>0</v>
+      </c>
+      <c r="P192" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q192" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="R192" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="S192" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="T192" s="10"/>
+      <c r="U192" s="9">
+        <v>0</v>
+      </c>
+      <c r="V192" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W192" s="9">
+        <v>185.69</v>
+      </c>
+      <c r="X192" s="12">
+        <v>1934798600</v>
+      </c>
+      <c r="Y192" s="9">
+        <v>188.34</v>
+      </c>
+      <c r="Z192" s="12">
+        <v>2246632524</v>
+      </c>
+      <c r="AA192" s="12">
+        <v>284280396</v>
+      </c>
+      <c r="AB192" s="12">
+        <v>27553528</v>
+      </c>
+      <c r="AC192" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD192" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE192" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF192" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:32">
+      <c r="A193" s="8">
+        <v>46045</v>
+      </c>
+      <c r="B193" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C193" s="10"/>
+      <c r="D193" s="9">
+        <v>6861</v>
+      </c>
+      <c r="E193" s="9">
+        <v>0</v>
+      </c>
+      <c r="F193" s="11">
+        <v>1900</v>
+      </c>
+      <c r="G193" s="11">
+        <v>55916.79</v>
+      </c>
+      <c r="H193" s="11">
+        <v>106241900</v>
+      </c>
+      <c r="I193" s="11">
+        <v>59970</v>
+      </c>
+      <c r="J193" s="11">
+        <v>113943000</v>
+      </c>
+      <c r="K193" s="11">
+        <v>7701100</v>
+      </c>
+      <c r="L193" s="12">
+        <v>74110530</v>
+      </c>
+      <c r="M193" s="9">
+        <v>0</v>
+      </c>
+      <c r="N193" s="9">
+        <v>0</v>
+      </c>
+      <c r="O193" s="9">
+        <v>0</v>
+      </c>
+      <c r="P193" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q193" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="R193" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="S193" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="T193" s="10"/>
+      <c r="U193" s="9">
+        <v>0</v>
+      </c>
+      <c r="V193" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W193" s="9">
+        <v>924.45</v>
+      </c>
+      <c r="X193" s="12">
+        <v>982163868</v>
+      </c>
+      <c r="Y193" s="9">
+        <v>927.02</v>
+      </c>
+      <c r="Z193" s="12">
+        <v>1056274398</v>
+      </c>
+      <c r="AA193" s="12">
+        <v>71390737</v>
+      </c>
+      <c r="AB193" s="12">
+        <v>2719793</v>
+      </c>
+      <c r="AC193" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD193" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE193" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF193" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:32">
+      <c r="A194" s="8">
+        <v>46045</v>
+      </c>
+      <c r="B194" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C194" s="10"/>
+      <c r="D194" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E194" s="9">
+        <v>0</v>
+      </c>
+      <c r="F194" s="9">
+        <v>0</v>
+      </c>
+      <c r="G194" s="9">
+        <v>0</v>
+      </c>
+      <c r="H194" s="9">
+        <v>0</v>
+      </c>
+      <c r="I194" s="11">
+        <v>17305</v>
+      </c>
+      <c r="J194" s="9">
+        <v>0</v>
+      </c>
+      <c r="K194" s="9">
+        <v>0</v>
+      </c>
+      <c r="L194" s="9">
+        <v>0</v>
+      </c>
+      <c r="M194" s="9">
+        <v>0</v>
+      </c>
+      <c r="N194" s="11">
+        <v>4480700</v>
+      </c>
+      <c r="O194" s="11">
+        <v>4480700</v>
+      </c>
+      <c r="P194" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q194" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="R194" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="S194" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="T194" s="10"/>
+      <c r="U194" s="9">
+        <v>0</v>
+      </c>
+      <c r="V194" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W194" s="9">
+        <v>0</v>
+      </c>
+      <c r="X194" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y194" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z194" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA194" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB194" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC194" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD194" s="12">
+        <v>37760160</v>
+      </c>
+      <c r="AE194" s="12">
+        <v>37760160</v>
+      </c>
+      <c r="AF194" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:32">
+      <c r="A195" s="8">
+        <v>46045</v>
+      </c>
+      <c r="B195" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C195" s="10"/>
+      <c r="D195" s="9">
+        <v>9984</v>
+      </c>
+      <c r="E195" s="9">
+        <v>0</v>
+      </c>
+      <c r="F195" s="11">
+        <v>23000</v>
+      </c>
+      <c r="G195" s="11">
+        <v>4066.73</v>
+      </c>
+      <c r="H195" s="11">
+        <v>93534900</v>
+      </c>
+      <c r="I195" s="11">
+        <v>4206</v>
+      </c>
+      <c r="J195" s="11">
+        <v>96738000</v>
+      </c>
+      <c r="K195" s="11">
+        <v>3203100</v>
+      </c>
+      <c r="L195" s="12">
+        <v>30161052</v>
+      </c>
+      <c r="M195" s="9">
+        <v>0</v>
+      </c>
+      <c r="N195" s="9">
+        <v>0</v>
+      </c>
+      <c r="O195" s="9">
+        <v>0</v>
+      </c>
+      <c r="P195" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q195" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="R195" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="S195" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="T195" s="10"/>
+      <c r="U195" s="9">
+        <v>0</v>
+      </c>
+      <c r="V195" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W195" s="9">
+        <v>926.51</v>
+      </c>
+      <c r="X195" s="12">
+        <v>866619555</v>
+      </c>
+      <c r="Y195" s="9">
+        <v>927.02</v>
+      </c>
+      <c r="Z195" s="12">
+        <v>896780607</v>
+      </c>
+      <c r="AA195" s="12">
+        <v>29693377</v>
+      </c>
+      <c r="AB195" s="12">
+        <v>467674</v>
+      </c>
+      <c r="AC195" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD195" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE195" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF195" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:32">
+      <c r="A196" s="8">
+        <v>46045</v>
+      </c>
+      <c r="B196" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C196" s="10"/>
+      <c r="D196" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E196" s="9">
+        <v>0</v>
+      </c>
+      <c r="F196" s="11">
+        <v>10000</v>
+      </c>
+      <c r="G196" s="9">
+        <v>48.203000000000003</v>
+      </c>
+      <c r="H196" s="11">
+        <v>482030</v>
+      </c>
+      <c r="I196" s="9">
+        <v>52.46</v>
+      </c>
+      <c r="J196" s="11">
+        <v>524600</v>
+      </c>
+      <c r="K196" s="11">
+        <v>42570</v>
+      </c>
+      <c r="L196" s="12">
+        <v>68631569</v>
+      </c>
+      <c r="M196" s="9">
+        <v>0</v>
+      </c>
+      <c r="N196" s="9">
+        <v>0</v>
+      </c>
+      <c r="O196" s="9">
+        <v>0</v>
+      </c>
+      <c r="P196" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q196" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R196" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S196" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="T196" s="10"/>
+      <c r="U196" s="9">
+        <v>0</v>
+      </c>
+      <c r="V196" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W196" s="11">
+        <v>1455.7</v>
+      </c>
+      <c r="X196" s="12">
+        <v>701691071</v>
+      </c>
+      <c r="Y196" s="11">
+        <v>1468.4</v>
+      </c>
+      <c r="Z196" s="12">
+        <v>770322640</v>
+      </c>
+      <c r="AA196" s="12">
+        <v>62509788</v>
+      </c>
+      <c r="AB196" s="12">
+        <v>6121781</v>
+      </c>
+      <c r="AC196" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD196" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE196" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF196" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:32">
+      <c r="A197" s="8">
+        <v>46045</v>
+      </c>
+      <c r="B197" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C197" s="10"/>
+      <c r="D197" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E197" s="9">
+        <v>0</v>
+      </c>
+      <c r="F197" s="11">
+        <v>20000</v>
+      </c>
+      <c r="G197" s="9">
+        <v>34.24</v>
+      </c>
+      <c r="H197" s="11">
+        <v>684800</v>
+      </c>
+      <c r="I197" s="9">
+        <v>34.46</v>
+      </c>
+      <c r="J197" s="11">
+        <v>689200</v>
+      </c>
+      <c r="K197" s="11">
+        <v>4400</v>
+      </c>
+      <c r="L197" s="12">
+        <v>571680</v>
+      </c>
+      <c r="M197" s="9">
+        <v>0</v>
+      </c>
+      <c r="N197" s="9">
+        <v>0</v>
+      </c>
+      <c r="O197" s="9">
+        <v>0</v>
+      </c>
+      <c r="P197" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q197" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R197" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S197" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="T197" s="10"/>
+      <c r="U197" s="9">
+        <v>0</v>
+      </c>
+      <c r="V197" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W197" s="11">
+        <v>1477</v>
+      </c>
+      <c r="X197" s="12">
+        <v>1011449600</v>
+      </c>
+      <c r="Y197" s="11">
+        <v>1468.4</v>
+      </c>
+      <c r="Z197" s="12">
+        <v>1012021280</v>
+      </c>
+      <c r="AA197" s="12">
+        <v>6460960</v>
+      </c>
+      <c r="AB197" s="12">
+        <v>-5889280</v>
+      </c>
+      <c r="AC197" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD197" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE197" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF197" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:32">
+      <c r="A198" s="8">
+        <v>46045</v>
+      </c>
+      <c r="B198" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C198" s="10"/>
+      <c r="D198" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E198" s="9">
+        <v>0</v>
+      </c>
+      <c r="F198" s="11">
+        <v>3000</v>
+      </c>
+      <c r="G198" s="9">
+        <v>247.65</v>
+      </c>
+      <c r="H198" s="11">
+        <v>742950</v>
+      </c>
+      <c r="I198" s="9">
+        <v>249.56</v>
+      </c>
+      <c r="J198" s="11">
+        <v>748680</v>
+      </c>
+      <c r="K198" s="11">
+        <v>5730</v>
+      </c>
+      <c r="L198" s="12">
+        <v>2024562</v>
+      </c>
+      <c r="M198" s="9">
+        <v>0</v>
+      </c>
+      <c r="N198" s="9">
+        <v>0</v>
+      </c>
+      <c r="O198" s="9">
+        <v>0</v>
+      </c>
+      <c r="P198" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q198" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R198" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S198" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="T198" s="10"/>
+      <c r="U198" s="9">
+        <v>0</v>
+      </c>
+      <c r="V198" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W198" s="11">
+        <v>1477</v>
+      </c>
+      <c r="X198" s="12">
+        <v>1097337150</v>
+      </c>
+      <c r="Y198" s="11">
+        <v>1468.4</v>
+      </c>
+      <c r="Z198" s="12">
+        <v>1099361712</v>
+      </c>
+      <c r="AA198" s="12">
+        <v>8413932</v>
+      </c>
+      <c r="AB198" s="12">
+        <v>-6389370</v>
+      </c>
+      <c r="AC198" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD198" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE198" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF198" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:32">
+      <c r="A199" s="8">
+        <v>46045</v>
+      </c>
+      <c r="B199" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C199" s="10"/>
+      <c r="D199" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E199" s="9">
+        <v>0</v>
+      </c>
+      <c r="F199" s="11">
+        <v>83000</v>
+      </c>
+      <c r="G199" s="9">
+        <v>12.374000000000001</v>
+      </c>
+      <c r="H199" s="11">
+        <v>1027042</v>
+      </c>
+      <c r="I199" s="9">
+        <v>10.59</v>
+      </c>
+      <c r="J199" s="11">
+        <v>878970</v>
+      </c>
+      <c r="K199" s="11">
+        <v>-148072</v>
+      </c>
+      <c r="L199" s="12">
+        <v>-194115071</v>
+      </c>
+      <c r="M199" s="9">
+        <v>0</v>
+      </c>
+      <c r="N199" s="9">
+        <v>0</v>
+      </c>
+      <c r="O199" s="9">
+        <v>0</v>
+      </c>
+      <c r="P199" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q199" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R199" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S199" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="T199" s="10"/>
+      <c r="U199" s="9">
+        <v>0</v>
+      </c>
+      <c r="V199" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W199" s="11">
+        <v>1445.69</v>
+      </c>
+      <c r="X199" s="12">
+        <v>1484794619</v>
+      </c>
+      <c r="Y199" s="11">
+        <v>1468.4</v>
+      </c>
+      <c r="Z199" s="12">
+        <v>1290679548</v>
+      </c>
+      <c r="AA199" s="12">
+        <v>-217428924</v>
+      </c>
+      <c r="AB199" s="12">
+        <v>23313853</v>
+      </c>
+      <c r="AC199" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD199" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE199" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF199" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:32">
+      <c r="A200" s="8">
+        <v>46045</v>
+      </c>
+      <c r="B200" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C200" s="10"/>
+      <c r="D200" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E200" s="9">
+        <v>0</v>
+      </c>
+      <c r="F200" s="11">
+        <v>2500</v>
+      </c>
+      <c r="G200" s="9">
+        <v>681.92</v>
+      </c>
+      <c r="H200" s="11">
+        <v>1704800</v>
+      </c>
+      <c r="I200" s="9">
+        <v>690.46</v>
+      </c>
+      <c r="J200" s="11">
+        <v>1726150</v>
+      </c>
+      <c r="K200" s="11">
+        <v>21350</v>
+      </c>
+      <c r="L200" s="12">
+        <v>88461140</v>
+      </c>
+      <c r="M200" s="9">
+        <v>0</v>
+      </c>
+      <c r="N200" s="11">
+        <v>8700</v>
+      </c>
+      <c r="O200" s="11">
+        <v>8700</v>
+      </c>
+      <c r="P200" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q200" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R200" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S200" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="T200" s="10"/>
+      <c r="U200" s="9">
+        <v>0</v>
+      </c>
+      <c r="V200" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="W200" s="11">
+        <v>1434.9</v>
+      </c>
+      <c r="X200" s="12">
+        <v>2446217520</v>
+      </c>
+      <c r="Y200" s="11">
+        <v>1468.4</v>
+      </c>
+      <c r="Z200" s="12">
+        <v>2534678660</v>
+      </c>
+      <c r="AA200" s="12">
+        <v>31350340</v>
+      </c>
+      <c r="AB200" s="12">
+        <v>57110800</v>
+      </c>
+      <c r="AC200" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD200" s="12">
+        <v>84621980</v>
+      </c>
+      <c r="AE200" s="12">
+        <v>84621980</v>
+      </c>
+      <c r="AF200" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:32">
+      <c r="A201" s="8">
+        <v>46045</v>
+      </c>
+      <c r="B201" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C201" s="10"/>
+      <c r="D201" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E201" s="9">
+        <v>0</v>
+      </c>
+      <c r="F201" s="11">
+        <v>4200</v>
+      </c>
+      <c r="G201" s="9">
+        <v>396.31</v>
+      </c>
+      <c r="H201" s="11">
+        <v>1664502</v>
+      </c>
+      <c r="I201" s="9">
+        <v>455.9</v>
+      </c>
+      <c r="J201" s="11">
+        <v>1914780</v>
+      </c>
+      <c r="K201" s="11">
+        <v>250278</v>
+      </c>
+      <c r="L201" s="12">
+        <v>423269033</v>
+      </c>
+      <c r="M201" s="9">
+        <v>0</v>
+      </c>
+      <c r="N201" s="9">
+        <v>0</v>
+      </c>
+      <c r="O201" s="9">
+        <v>0</v>
+      </c>
+      <c r="P201" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q201" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R201" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S201" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="T201" s="10"/>
+      <c r="U201" s="9">
+        <v>0</v>
+      </c>
+      <c r="V201" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="W201" s="11">
+        <v>1434.89</v>
+      </c>
+      <c r="X201" s="12">
+        <v>2388393919</v>
+      </c>
+      <c r="Y201" s="11">
+        <v>1468.4</v>
+      </c>
+      <c r="Z201" s="12">
+        <v>2811662952</v>
+      </c>
+      <c r="AA201" s="12">
+        <v>367508215</v>
+      </c>
+      <c r="AB201" s="12">
+        <v>55760817</v>
+      </c>
+      <c r="AC201" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD201" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE201" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF201" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:32">
+      <c r="A202" s="8">
+        <v>46045</v>
+      </c>
+      <c r="B202" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C202" s="10"/>
+      <c r="D202" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E202" s="9">
+        <v>0</v>
+      </c>
+      <c r="F202" s="11">
+        <v>24000</v>
+      </c>
+      <c r="G202" s="9">
+        <v>17.655000000000001</v>
+      </c>
+      <c r="H202" s="11">
+        <v>423736.8</v>
+      </c>
+      <c r="I202" s="9">
+        <v>16.239999999999998</v>
+      </c>
+      <c r="J202" s="11">
+        <v>389760</v>
+      </c>
+      <c r="K202" s="11">
+        <v>-33976.800000000003</v>
+      </c>
+      <c r="L202" s="12">
+        <v>-48069464</v>
+      </c>
+      <c r="M202" s="9">
+        <v>0</v>
+      </c>
+      <c r="N202" s="9">
+        <v>0</v>
+      </c>
+      <c r="O202" s="9">
+        <v>0</v>
+      </c>
+      <c r="P202" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q202" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R202" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S202" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="T202" s="10"/>
+      <c r="U202" s="9">
+        <v>0</v>
+      </c>
+      <c r="V202" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W202" s="11">
+        <v>1464.09</v>
+      </c>
+      <c r="X202" s="12">
+        <v>620393048</v>
+      </c>
+      <c r="Y202" s="11">
+        <v>1468.4</v>
+      </c>
+      <c r="Z202" s="12">
+        <v>572323584</v>
+      </c>
+      <c r="AA202" s="12">
+        <v>-49891533</v>
+      </c>
+      <c r="AB202" s="12">
+        <v>1822069</v>
+      </c>
+      <c r="AC202" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD202" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE202" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF202" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:32">
+      <c r="A203" s="8">
+        <v>46045</v>
+      </c>
+      <c r="B203" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C203" s="10"/>
+      <c r="D203" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E203" s="9">
+        <v>0</v>
+      </c>
+      <c r="F203" s="11">
+        <v>1400</v>
+      </c>
+      <c r="G203" s="9">
+        <v>432.53800000000001</v>
+      </c>
+      <c r="H203" s="11">
+        <v>605554.04</v>
+      </c>
+      <c r="I203" s="9">
+        <v>451.86</v>
+      </c>
+      <c r="J203" s="11">
+        <v>632604</v>
+      </c>
+      <c r="K203" s="11">
+        <v>27049.96</v>
+      </c>
+      <c r="L203" s="12">
+        <v>52800128</v>
+      </c>
+      <c r="M203" s="9">
+        <v>0</v>
+      </c>
+      <c r="N203" s="9">
+        <v>0</v>
+      </c>
+      <c r="O203" s="9">
+        <v>0</v>
+      </c>
+      <c r="P203" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q203" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R203" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S203" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="T203" s="10"/>
+      <c r="U203" s="9">
+        <v>0</v>
+      </c>
+      <c r="V203" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W203" s="11">
+        <v>1446.79</v>
+      </c>
+      <c r="X203" s="12">
+        <v>876115585</v>
+      </c>
+      <c r="Y203" s="11">
+        <v>1468.4</v>
+      </c>
+      <c r="Z203" s="12">
+        <v>928915713</v>
+      </c>
+      <c r="AA203" s="12">
+        <v>39720161</v>
+      </c>
+      <c r="AB203" s="12">
+        <v>13079967</v>
+      </c>
+      <c r="AC203" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD203" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE203" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF203" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="204" spans="1:32" ht="18" thickBot="1">
-      <c r="A204" s="3"/>
-      <c r="B204" s="4"/>
-      <c r="C204" s="2"/>
-      <c r="D204" s="1"/>
-      <c r="E204" s="5"/>
-      <c r="F204" s="6"/>
-      <c r="G204" s="5"/>
-      <c r="H204" s="6"/>
-      <c r="I204" s="5"/>
-      <c r="J204" s="6"/>
-      <c r="K204" s="6"/>
-      <c r="L204" s="7"/>
-      <c r="M204" s="5"/>
-      <c r="N204" s="5"/>
-      <c r="O204" s="5"/>
-      <c r="P204" s="5"/>
-      <c r="Q204" s="1"/>
-      <c r="R204" s="1"/>
-      <c r="S204" s="1"/>
-      <c r="T204" s="2"/>
-      <c r="U204" s="5"/>
-      <c r="V204" s="1"/>
-      <c r="W204" s="6"/>
-      <c r="X204" s="7"/>
-      <c r="Y204" s="6"/>
-      <c r="Z204" s="7"/>
-      <c r="AA204" s="7"/>
-      <c r="AB204" s="7"/>
-      <c r="AC204" s="5"/>
-      <c r="AD204" s="5"/>
-      <c r="AE204" s="5"/>
-      <c r="AF204" s="5"/>
+      <c r="A204" s="8">
+        <v>46045</v>
+      </c>
+      <c r="B204" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C204" s="10"/>
+      <c r="D204" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E204" s="9">
+        <v>0</v>
+      </c>
+      <c r="F204" s="11">
+        <v>3500</v>
+      </c>
+      <c r="G204" s="9">
+        <v>169.042</v>
+      </c>
+      <c r="H204" s="11">
+        <v>591649.80000000005</v>
+      </c>
+      <c r="I204" s="9">
+        <v>161.88</v>
+      </c>
+      <c r="J204" s="11">
+        <v>566580</v>
+      </c>
+      <c r="K204" s="11">
+        <v>-25069.8</v>
+      </c>
+      <c r="L204" s="12">
+        <v>-24032858</v>
+      </c>
+      <c r="M204" s="9">
+        <v>0</v>
+      </c>
+      <c r="N204" s="9">
+        <v>0</v>
+      </c>
+      <c r="O204" s="9">
+        <v>0</v>
+      </c>
+      <c r="P204" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q204" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R204" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S204" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="T204" s="10"/>
+      <c r="U204" s="9">
+        <v>0</v>
+      </c>
+      <c r="V204" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W204" s="11">
+        <v>1446.79</v>
+      </c>
+      <c r="X204" s="12">
+        <v>855998930</v>
+      </c>
+      <c r="Y204" s="11">
+        <v>1468.4</v>
+      </c>
+      <c r="Z204" s="12">
+        <v>831966072</v>
+      </c>
+      <c r="AA204" s="12">
+        <v>-36812494</v>
+      </c>
+      <c r="AB204" s="12">
+        <v>12779636</v>
+      </c>
+      <c r="AC204" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD204" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE204" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF204" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="205" spans="1:32" ht="18" thickBot="1">
       <c r="A205" s="3"/>

</xml_diff>

<commit_message>
Update 2026_멀티.xlsx (2026-01-26 16:33:56)
</commit_message>
<xml_diff>
--- a/2026_멀티.xlsx
+++ b/2026_멀티.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyejinha/Desktop/Workspace/Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EAFBA28-31D3-774C-AAB7-BC0727DA8A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C44EF6-A360-6045-A77B-40D51964A994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="29000" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="18460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="97">
   <si>
     <t>기준일자</t>
   </si>
@@ -292,6 +292,30 @@
   </si>
   <si>
     <t>JLMAG</t>
+  </si>
+  <si>
+    <t>JP3802400006</t>
+  </si>
+  <si>
+    <t>화낙</t>
+  </si>
+  <si>
+    <t>CA65340P1062</t>
+  </si>
+  <si>
+    <t>NXE</t>
+  </si>
+  <si>
+    <t>넥스젠 에너지</t>
+  </si>
+  <si>
+    <t>US6745991058</t>
+  </si>
+  <si>
+    <t>OXY</t>
+  </si>
+  <si>
+    <t>옥시덴털 페트롤리엄</t>
   </si>
 </sst>
 </file>
@@ -671,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="A187" sqref="A187:AF204"/>
+    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
+      <selection activeCell="A205" sqref="A205:AF225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -19719,7 +19743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:32" ht="18" thickBot="1">
+    <row r="204" spans="1:32">
       <c r="A204" s="8">
         <v>46045</v>
       </c>
@@ -19813,719 +19837,1979 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:32" ht="18" thickBot="1">
-      <c r="A205" s="3"/>
-      <c r="B205" s="4"/>
-      <c r="C205" s="2"/>
-      <c r="D205" s="1"/>
-      <c r="E205" s="5"/>
-      <c r="F205" s="6"/>
-      <c r="G205" s="5"/>
-      <c r="H205" s="6"/>
-      <c r="I205" s="5"/>
-      <c r="J205" s="6"/>
-      <c r="K205" s="6"/>
-      <c r="L205" s="7"/>
-      <c r="M205" s="5"/>
-      <c r="N205" s="5"/>
-      <c r="O205" s="5"/>
-      <c r="P205" s="5"/>
-      <c r="Q205" s="1"/>
-      <c r="R205" s="1"/>
-      <c r="S205" s="4"/>
-      <c r="T205" s="2"/>
-      <c r="U205" s="5"/>
-      <c r="V205" s="1"/>
-      <c r="W205" s="6"/>
-      <c r="X205" s="7"/>
-      <c r="Y205" s="6"/>
-      <c r="Z205" s="7"/>
-      <c r="AA205" s="7"/>
-      <c r="AB205" s="7"/>
-      <c r="AC205" s="5"/>
-      <c r="AD205" s="5"/>
-      <c r="AE205" s="5"/>
-      <c r="AF205" s="5"/>
-    </row>
-    <row r="206" spans="1:32" ht="18" thickBot="1">
-      <c r="A206" s="3"/>
-      <c r="B206" s="4"/>
-      <c r="C206" s="2"/>
-      <c r="D206" s="1"/>
-      <c r="E206" s="5"/>
-      <c r="F206" s="6"/>
-      <c r="G206" s="5"/>
-      <c r="H206" s="6"/>
-      <c r="I206" s="5"/>
-      <c r="J206" s="6"/>
-      <c r="K206" s="6"/>
-      <c r="L206" s="7"/>
-      <c r="M206" s="5"/>
-      <c r="N206" s="5"/>
-      <c r="O206" s="5"/>
-      <c r="P206" s="5"/>
-      <c r="Q206" s="1"/>
-      <c r="R206" s="1"/>
-      <c r="S206" s="1"/>
-      <c r="T206" s="2"/>
-      <c r="U206" s="5"/>
-      <c r="V206" s="1"/>
-      <c r="W206" s="6"/>
-      <c r="X206" s="7"/>
-      <c r="Y206" s="6"/>
-      <c r="Z206" s="7"/>
-      <c r="AA206" s="7"/>
-      <c r="AB206" s="7"/>
-      <c r="AC206" s="5"/>
-      <c r="AD206" s="5"/>
-      <c r="AE206" s="5"/>
-      <c r="AF206" s="5"/>
-    </row>
-    <row r="207" spans="1:32" ht="18" thickBot="1">
-      <c r="A207" s="3"/>
-      <c r="B207" s="4"/>
-      <c r="C207" s="2"/>
-      <c r="D207" s="1"/>
-      <c r="E207" s="5"/>
-      <c r="F207" s="6"/>
-      <c r="G207" s="5"/>
-      <c r="H207" s="6"/>
-      <c r="I207" s="5"/>
-      <c r="J207" s="6"/>
-      <c r="K207" s="6"/>
-      <c r="L207" s="7"/>
-      <c r="M207" s="5"/>
-      <c r="N207" s="5"/>
-      <c r="O207" s="5"/>
-      <c r="P207" s="5"/>
-      <c r="Q207" s="1"/>
-      <c r="R207" s="1"/>
-      <c r="S207" s="1"/>
-      <c r="T207" s="2"/>
-      <c r="U207" s="5"/>
-      <c r="V207" s="1"/>
-      <c r="W207" s="6"/>
-      <c r="X207" s="7"/>
-      <c r="Y207" s="6"/>
-      <c r="Z207" s="7"/>
-      <c r="AA207" s="7"/>
-      <c r="AB207" s="7"/>
-      <c r="AC207" s="5"/>
-      <c r="AD207" s="5"/>
-      <c r="AE207" s="5"/>
-      <c r="AF207" s="5"/>
-    </row>
-    <row r="208" spans="1:32" ht="18" thickBot="1">
-      <c r="A208" s="3"/>
-      <c r="B208" s="4"/>
-      <c r="C208" s="2"/>
-      <c r="D208" s="1"/>
-      <c r="E208" s="5"/>
-      <c r="F208" s="6"/>
-      <c r="G208" s="5"/>
-      <c r="H208" s="6"/>
-      <c r="I208" s="5"/>
-      <c r="J208" s="6"/>
-      <c r="K208" s="6"/>
-      <c r="L208" s="7"/>
-      <c r="M208" s="5"/>
-      <c r="N208" s="5"/>
-      <c r="O208" s="5"/>
-      <c r="P208" s="5"/>
-      <c r="Q208" s="1"/>
-      <c r="R208" s="1"/>
-      <c r="S208" s="1"/>
-      <c r="T208" s="2"/>
-      <c r="U208" s="5"/>
-      <c r="V208" s="1"/>
-      <c r="W208" s="6"/>
-      <c r="X208" s="7"/>
-      <c r="Y208" s="6"/>
-      <c r="Z208" s="7"/>
-      <c r="AA208" s="7"/>
-      <c r="AB208" s="7"/>
-      <c r="AC208" s="5"/>
-      <c r="AD208" s="5"/>
-      <c r="AE208" s="5"/>
-      <c r="AF208" s="5"/>
-    </row>
-    <row r="209" spans="1:32" ht="18" thickBot="1">
-      <c r="A209" s="3"/>
-      <c r="B209" s="4"/>
-      <c r="C209" s="2"/>
-      <c r="D209" s="1"/>
-      <c r="E209" s="5"/>
-      <c r="F209" s="6"/>
-      <c r="G209" s="5"/>
-      <c r="H209" s="6"/>
-      <c r="I209" s="5"/>
-      <c r="J209" s="6"/>
-      <c r="K209" s="6"/>
-      <c r="L209" s="7"/>
-      <c r="M209" s="5"/>
-      <c r="N209" s="5"/>
-      <c r="O209" s="5"/>
-      <c r="P209" s="5"/>
-      <c r="Q209" s="1"/>
-      <c r="R209" s="1"/>
-      <c r="S209" s="4"/>
-      <c r="T209" s="2"/>
-      <c r="U209" s="5"/>
-      <c r="V209" s="1"/>
-      <c r="W209" s="6"/>
-      <c r="X209" s="7"/>
-      <c r="Y209" s="6"/>
-      <c r="Z209" s="7"/>
-      <c r="AA209" s="7"/>
-      <c r="AB209" s="7"/>
-      <c r="AC209" s="5"/>
-      <c r="AD209" s="5"/>
-      <c r="AE209" s="5"/>
-      <c r="AF209" s="5"/>
-    </row>
-    <row r="210" spans="1:32" ht="18" thickBot="1">
-      <c r="A210" s="2"/>
-      <c r="B210" s="2"/>
-      <c r="C210" s="2"/>
-      <c r="D210" s="2"/>
-      <c r="E210" s="2"/>
-      <c r="F210" s="2"/>
-      <c r="G210" s="2"/>
-      <c r="H210" s="2"/>
-      <c r="I210" s="2"/>
-      <c r="J210" s="2"/>
-      <c r="K210" s="2"/>
-      <c r="L210" s="2"/>
-      <c r="M210" s="2"/>
-      <c r="N210" s="2"/>
-      <c r="O210" s="2"/>
-      <c r="P210" s="2"/>
-      <c r="Q210" s="2"/>
-      <c r="R210" s="2"/>
-      <c r="S210" s="2"/>
-      <c r="T210" s="2"/>
-      <c r="U210" s="2"/>
-      <c r="V210" s="2"/>
-      <c r="W210" s="2"/>
-      <c r="X210" s="2"/>
-      <c r="Y210" s="2"/>
-      <c r="Z210" s="2"/>
-      <c r="AA210" s="2"/>
-      <c r="AB210" s="2"/>
-      <c r="AC210" s="2"/>
-      <c r="AD210" s="2"/>
-      <c r="AE210" s="2"/>
-      <c r="AF210" s="2"/>
-    </row>
-    <row r="211" spans="1:32" ht="18" thickBot="1">
-      <c r="A211" s="2"/>
-      <c r="B211" s="2"/>
-      <c r="C211" s="2"/>
-      <c r="D211" s="2"/>
-      <c r="E211" s="2"/>
-      <c r="F211" s="2"/>
-      <c r="G211" s="2"/>
-      <c r="H211" s="2"/>
-      <c r="I211" s="2"/>
-      <c r="J211" s="2"/>
-      <c r="K211" s="2"/>
-      <c r="L211" s="2"/>
-      <c r="M211" s="2"/>
-      <c r="N211" s="2"/>
-      <c r="O211" s="2"/>
-      <c r="P211" s="2"/>
-      <c r="Q211" s="2"/>
-      <c r="R211" s="2"/>
-      <c r="S211" s="2"/>
-      <c r="T211" s="2"/>
-      <c r="U211" s="2"/>
-      <c r="V211" s="2"/>
-      <c r="W211" s="2"/>
-      <c r="X211" s="2"/>
-      <c r="Y211" s="2"/>
-      <c r="Z211" s="2"/>
-      <c r="AA211" s="2"/>
-      <c r="AB211" s="2"/>
-      <c r="AC211" s="2"/>
-      <c r="AD211" s="2"/>
-      <c r="AE211" s="2"/>
-      <c r="AF211" s="2"/>
-    </row>
-    <row r="212" spans="1:32" ht="18" thickBot="1">
-      <c r="A212" s="2"/>
-      <c r="B212" s="2"/>
-      <c r="C212" s="2"/>
-      <c r="D212" s="2"/>
-      <c r="E212" s="2"/>
-      <c r="F212" s="2"/>
-      <c r="G212" s="2"/>
-      <c r="H212" s="2"/>
-      <c r="I212" s="2"/>
-      <c r="J212" s="2"/>
-      <c r="K212" s="2"/>
-      <c r="L212" s="2"/>
-      <c r="M212" s="2"/>
-      <c r="N212" s="2"/>
-      <c r="O212" s="2"/>
-      <c r="P212" s="2"/>
-      <c r="Q212" s="2"/>
-      <c r="R212" s="2"/>
-      <c r="S212" s="2"/>
-      <c r="T212" s="2"/>
-      <c r="U212" s="2"/>
-      <c r="V212" s="2"/>
-      <c r="W212" s="2"/>
-      <c r="X212" s="2"/>
-      <c r="Y212" s="2"/>
-      <c r="Z212" s="2"/>
-      <c r="AA212" s="2"/>
-      <c r="AB212" s="2"/>
-      <c r="AC212" s="2"/>
-      <c r="AD212" s="2"/>
-      <c r="AE212" s="2"/>
-      <c r="AF212" s="2"/>
-    </row>
-    <row r="213" spans="1:32" ht="18" thickBot="1">
-      <c r="A213" s="2"/>
-      <c r="B213" s="2"/>
-      <c r="C213" s="2"/>
-      <c r="D213" s="2"/>
-      <c r="E213" s="2"/>
-      <c r="F213" s="2"/>
-      <c r="G213" s="2"/>
-      <c r="H213" s="2"/>
-      <c r="I213" s="2"/>
-      <c r="J213" s="2"/>
-      <c r="K213" s="2"/>
-      <c r="L213" s="2"/>
-      <c r="M213" s="2"/>
-      <c r="N213" s="2"/>
-      <c r="O213" s="2"/>
-      <c r="P213" s="2"/>
-      <c r="Q213" s="2"/>
-      <c r="R213" s="2"/>
-      <c r="S213" s="2"/>
-      <c r="T213" s="2"/>
-      <c r="U213" s="2"/>
-      <c r="V213" s="2"/>
-      <c r="W213" s="2"/>
-      <c r="X213" s="2"/>
-      <c r="Y213" s="2"/>
-      <c r="Z213" s="2"/>
-      <c r="AA213" s="2"/>
-      <c r="AB213" s="2"/>
-      <c r="AC213" s="2"/>
-      <c r="AD213" s="2"/>
-      <c r="AE213" s="2"/>
-      <c r="AF213" s="2"/>
-    </row>
-    <row r="214" spans="1:32" ht="18" thickBot="1">
-      <c r="A214" s="2"/>
-      <c r="B214" s="2"/>
-      <c r="C214" s="2"/>
-      <c r="D214" s="2"/>
-      <c r="E214" s="2"/>
-      <c r="F214" s="2"/>
-      <c r="G214" s="2"/>
-      <c r="H214" s="2"/>
-      <c r="I214" s="2"/>
-      <c r="J214" s="2"/>
-      <c r="K214" s="2"/>
-      <c r="L214" s="2"/>
-      <c r="M214" s="2"/>
-      <c r="N214" s="2"/>
-      <c r="O214" s="2"/>
-      <c r="P214" s="2"/>
-      <c r="Q214" s="2"/>
-      <c r="R214" s="2"/>
-      <c r="S214" s="2"/>
-      <c r="T214" s="2"/>
-      <c r="U214" s="2"/>
-      <c r="V214" s="2"/>
-      <c r="W214" s="2"/>
-      <c r="X214" s="2"/>
-      <c r="Y214" s="2"/>
-      <c r="Z214" s="2"/>
-      <c r="AA214" s="2"/>
-      <c r="AB214" s="2"/>
-      <c r="AC214" s="2"/>
-      <c r="AD214" s="2"/>
-      <c r="AE214" s="2"/>
-      <c r="AF214" s="2"/>
-    </row>
-    <row r="215" spans="1:32" ht="18" thickBot="1">
-      <c r="A215" s="2"/>
-      <c r="B215" s="2"/>
-      <c r="C215" s="2"/>
-      <c r="D215" s="2"/>
-      <c r="E215" s="2"/>
-      <c r="F215" s="2"/>
-      <c r="G215" s="2"/>
-      <c r="H215" s="2"/>
-      <c r="I215" s="2"/>
-      <c r="J215" s="2"/>
-      <c r="K215" s="2"/>
-      <c r="L215" s="2"/>
-      <c r="M215" s="2"/>
-      <c r="N215" s="2"/>
-      <c r="O215" s="2"/>
-      <c r="P215" s="2"/>
-      <c r="Q215" s="2"/>
-      <c r="R215" s="2"/>
-      <c r="S215" s="2"/>
-      <c r="T215" s="2"/>
-      <c r="U215" s="2"/>
-      <c r="V215" s="2"/>
-      <c r="W215" s="2"/>
-      <c r="X215" s="2"/>
-      <c r="Y215" s="2"/>
-      <c r="Z215" s="2"/>
-      <c r="AA215" s="2"/>
-      <c r="AB215" s="2"/>
-      <c r="AC215" s="2"/>
-      <c r="AD215" s="2"/>
-      <c r="AE215" s="2"/>
-      <c r="AF215" s="2"/>
-    </row>
-    <row r="216" spans="1:32" ht="18" thickBot="1">
-      <c r="A216" s="2"/>
-      <c r="B216" s="2"/>
-      <c r="C216" s="2"/>
-      <c r="D216" s="2"/>
-      <c r="E216" s="2"/>
-      <c r="F216" s="2"/>
-      <c r="G216" s="2"/>
-      <c r="H216" s="2"/>
-      <c r="I216" s="2"/>
-      <c r="J216" s="2"/>
-      <c r="K216" s="2"/>
-      <c r="L216" s="2"/>
-      <c r="M216" s="2"/>
-      <c r="N216" s="2"/>
-      <c r="O216" s="2"/>
-      <c r="P216" s="2"/>
-      <c r="Q216" s="2"/>
-      <c r="R216" s="2"/>
-      <c r="S216" s="2"/>
-      <c r="T216" s="2"/>
-      <c r="U216" s="2"/>
-      <c r="V216" s="2"/>
-      <c r="W216" s="2"/>
-      <c r="X216" s="2"/>
-      <c r="Y216" s="2"/>
-      <c r="Z216" s="2"/>
-      <c r="AA216" s="2"/>
-      <c r="AB216" s="2"/>
-      <c r="AC216" s="2"/>
-      <c r="AD216" s="2"/>
-      <c r="AE216" s="2"/>
-      <c r="AF216" s="2"/>
-    </row>
-    <row r="217" spans="1:32" ht="18" thickBot="1">
-      <c r="A217" s="2"/>
-      <c r="B217" s="2"/>
-      <c r="C217" s="2"/>
-      <c r="D217" s="2"/>
-      <c r="E217" s="2"/>
-      <c r="F217" s="2"/>
-      <c r="G217" s="2"/>
-      <c r="H217" s="2"/>
-      <c r="I217" s="2"/>
-      <c r="J217" s="2"/>
-      <c r="K217" s="2"/>
-      <c r="L217" s="2"/>
-      <c r="M217" s="2"/>
-      <c r="N217" s="2"/>
-      <c r="O217" s="2"/>
-      <c r="P217" s="2"/>
-      <c r="Q217" s="2"/>
-      <c r="R217" s="2"/>
-      <c r="S217" s="2"/>
-      <c r="T217" s="2"/>
-      <c r="U217" s="2"/>
-      <c r="V217" s="2"/>
-      <c r="W217" s="2"/>
-      <c r="X217" s="2"/>
-      <c r="Y217" s="2"/>
-      <c r="Z217" s="2"/>
-      <c r="AA217" s="2"/>
-      <c r="AB217" s="2"/>
-      <c r="AC217" s="2"/>
-      <c r="AD217" s="2"/>
-      <c r="AE217" s="2"/>
-      <c r="AF217" s="2"/>
-    </row>
-    <row r="218" spans="1:32" ht="18" thickBot="1">
-      <c r="A218" s="2"/>
-      <c r="B218" s="2"/>
-      <c r="C218" s="2"/>
-      <c r="D218" s="2"/>
-      <c r="E218" s="2"/>
-      <c r="F218" s="2"/>
-      <c r="G218" s="2"/>
-      <c r="H218" s="2"/>
-      <c r="I218" s="2"/>
-      <c r="J218" s="2"/>
-      <c r="K218" s="2"/>
-      <c r="L218" s="2"/>
-      <c r="M218" s="2"/>
-      <c r="N218" s="2"/>
-      <c r="O218" s="2"/>
-      <c r="P218" s="2"/>
-      <c r="Q218" s="2"/>
-      <c r="R218" s="2"/>
-      <c r="S218" s="2"/>
-      <c r="T218" s="2"/>
-      <c r="U218" s="2"/>
-      <c r="V218" s="2"/>
-      <c r="W218" s="2"/>
-      <c r="X218" s="2"/>
-      <c r="Y218" s="2"/>
-      <c r="Z218" s="2"/>
-      <c r="AA218" s="2"/>
-      <c r="AB218" s="2"/>
-      <c r="AC218" s="2"/>
-      <c r="AD218" s="2"/>
-      <c r="AE218" s="2"/>
-      <c r="AF218" s="2"/>
-    </row>
-    <row r="219" spans="1:32" ht="18" thickBot="1">
-      <c r="A219" s="2"/>
-      <c r="B219" s="2"/>
-      <c r="C219" s="2"/>
-      <c r="D219" s="2"/>
-      <c r="E219" s="2"/>
-      <c r="F219" s="2"/>
-      <c r="G219" s="2"/>
-      <c r="H219" s="2"/>
-      <c r="I219" s="2"/>
-      <c r="J219" s="2"/>
-      <c r="K219" s="2"/>
-      <c r="L219" s="2"/>
-      <c r="M219" s="2"/>
-      <c r="N219" s="2"/>
-      <c r="O219" s="2"/>
-      <c r="P219" s="2"/>
-      <c r="Q219" s="2"/>
-      <c r="R219" s="2"/>
-      <c r="S219" s="2"/>
-      <c r="T219" s="2"/>
-      <c r="U219" s="2"/>
-      <c r="V219" s="2"/>
-      <c r="W219" s="2"/>
-      <c r="X219" s="2"/>
-      <c r="Y219" s="2"/>
-      <c r="Z219" s="2"/>
-      <c r="AA219" s="2"/>
-      <c r="AB219" s="2"/>
-      <c r="AC219" s="2"/>
-      <c r="AD219" s="2"/>
-      <c r="AE219" s="2"/>
-      <c r="AF219" s="2"/>
-    </row>
-    <row r="220" spans="1:32" ht="18" thickBot="1">
-      <c r="A220" s="2"/>
-      <c r="B220" s="2"/>
-      <c r="C220" s="2"/>
-      <c r="D220" s="2"/>
-      <c r="E220" s="2"/>
-      <c r="F220" s="2"/>
-      <c r="G220" s="2"/>
-      <c r="H220" s="2"/>
-      <c r="I220" s="2"/>
-      <c r="J220" s="2"/>
-      <c r="K220" s="2"/>
-      <c r="L220" s="2"/>
-      <c r="M220" s="2"/>
-      <c r="N220" s="2"/>
-      <c r="O220" s="2"/>
-      <c r="P220" s="2"/>
-      <c r="Q220" s="2"/>
-      <c r="R220" s="2"/>
-      <c r="S220" s="2"/>
-      <c r="T220" s="2"/>
-      <c r="U220" s="2"/>
-      <c r="V220" s="2"/>
-      <c r="W220" s="2"/>
-      <c r="X220" s="2"/>
-      <c r="Y220" s="2"/>
-      <c r="Z220" s="2"/>
-      <c r="AA220" s="2"/>
-      <c r="AB220" s="2"/>
-      <c r="AC220" s="2"/>
-      <c r="AD220" s="2"/>
-      <c r="AE220" s="2"/>
-      <c r="AF220" s="2"/>
-    </row>
-    <row r="221" spans="1:32" ht="18" thickBot="1">
-      <c r="A221" s="2"/>
-      <c r="B221" s="2"/>
-      <c r="C221" s="2"/>
-      <c r="D221" s="2"/>
-      <c r="E221" s="2"/>
-      <c r="F221" s="2"/>
-      <c r="G221" s="2"/>
-      <c r="H221" s="2"/>
-      <c r="I221" s="2"/>
-      <c r="J221" s="2"/>
-      <c r="K221" s="2"/>
-      <c r="L221" s="2"/>
-      <c r="M221" s="2"/>
-      <c r="N221" s="2"/>
-      <c r="O221" s="2"/>
-      <c r="P221" s="2"/>
-      <c r="Q221" s="2"/>
-      <c r="R221" s="2"/>
-      <c r="S221" s="2"/>
-      <c r="T221" s="2"/>
-      <c r="U221" s="2"/>
-      <c r="V221" s="2"/>
-      <c r="W221" s="2"/>
-      <c r="X221" s="2"/>
-      <c r="Y221" s="2"/>
-      <c r="Z221" s="2"/>
-      <c r="AA221" s="2"/>
-      <c r="AB221" s="2"/>
-      <c r="AC221" s="2"/>
-      <c r="AD221" s="2"/>
-      <c r="AE221" s="2"/>
-      <c r="AF221" s="2"/>
-    </row>
-    <row r="222" spans="1:32" ht="18" thickBot="1">
-      <c r="A222" s="2"/>
-      <c r="B222" s="2"/>
-      <c r="C222" s="2"/>
-      <c r="D222" s="2"/>
-      <c r="E222" s="2"/>
-      <c r="F222" s="2"/>
-      <c r="G222" s="2"/>
-      <c r="H222" s="2"/>
-      <c r="I222" s="2"/>
-      <c r="J222" s="2"/>
-      <c r="K222" s="2"/>
-      <c r="L222" s="2"/>
-      <c r="M222" s="2"/>
-      <c r="N222" s="2"/>
-      <c r="O222" s="2"/>
-      <c r="P222" s="2"/>
-      <c r="Q222" s="2"/>
-      <c r="R222" s="2"/>
-      <c r="S222" s="2"/>
-      <c r="T222" s="2"/>
-      <c r="U222" s="2"/>
-      <c r="V222" s="2"/>
-      <c r="W222" s="2"/>
-      <c r="X222" s="2"/>
-      <c r="Y222" s="2"/>
-      <c r="Z222" s="2"/>
-      <c r="AA222" s="2"/>
-      <c r="AB222" s="2"/>
-      <c r="AC222" s="2"/>
-      <c r="AD222" s="2"/>
-      <c r="AE222" s="2"/>
-      <c r="AF222" s="2"/>
-    </row>
-    <row r="223" spans="1:32" ht="18" thickBot="1">
-      <c r="A223" s="2"/>
-      <c r="B223" s="2"/>
-      <c r="C223" s="2"/>
-      <c r="D223" s="2"/>
-      <c r="E223" s="2"/>
-      <c r="F223" s="2"/>
-      <c r="G223" s="2"/>
-      <c r="H223" s="2"/>
-      <c r="I223" s="2"/>
-      <c r="J223" s="2"/>
-      <c r="K223" s="2"/>
-      <c r="L223" s="2"/>
-      <c r="M223" s="2"/>
-      <c r="N223" s="2"/>
-      <c r="O223" s="2"/>
-      <c r="P223" s="2"/>
-      <c r="Q223" s="2"/>
-      <c r="R223" s="2"/>
-      <c r="S223" s="2"/>
-      <c r="T223" s="2"/>
-      <c r="U223" s="2"/>
-      <c r="V223" s="2"/>
-      <c r="W223" s="2"/>
-      <c r="X223" s="2"/>
-      <c r="Y223" s="2"/>
-      <c r="Z223" s="2"/>
-      <c r="AA223" s="2"/>
-      <c r="AB223" s="2"/>
-      <c r="AC223" s="2"/>
-      <c r="AD223" s="2"/>
-      <c r="AE223" s="2"/>
-      <c r="AF223" s="2"/>
-    </row>
-    <row r="224" spans="1:32" ht="18" thickBot="1">
-      <c r="A224" s="2"/>
-      <c r="B224" s="2"/>
-      <c r="C224" s="2"/>
-      <c r="D224" s="2"/>
-      <c r="E224" s="2"/>
-      <c r="F224" s="2"/>
-      <c r="G224" s="2"/>
-      <c r="H224" s="2"/>
-      <c r="I224" s="2"/>
-      <c r="J224" s="2"/>
-      <c r="K224" s="2"/>
-      <c r="L224" s="2"/>
-      <c r="M224" s="2"/>
-      <c r="N224" s="2"/>
-      <c r="O224" s="2"/>
-      <c r="P224" s="2"/>
-      <c r="Q224" s="2"/>
-      <c r="R224" s="2"/>
-      <c r="S224" s="2"/>
-      <c r="T224" s="2"/>
-      <c r="U224" s="2"/>
-      <c r="V224" s="2"/>
-      <c r="W224" s="2"/>
-      <c r="X224" s="2"/>
-      <c r="Y224" s="2"/>
-      <c r="Z224" s="2"/>
-      <c r="AA224" s="2"/>
-      <c r="AB224" s="2"/>
-      <c r="AC224" s="2"/>
-      <c r="AD224" s="2"/>
-      <c r="AE224" s="2"/>
-      <c r="AF224" s="2"/>
+    <row r="205" spans="1:32">
+      <c r="A205" s="8">
+        <v>46048</v>
+      </c>
+      <c r="B205" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C205" s="10"/>
+      <c r="D205" s="9">
+        <v>6869</v>
+      </c>
+      <c r="E205" s="9">
+        <v>0</v>
+      </c>
+      <c r="F205" s="9">
+        <v>0</v>
+      </c>
+      <c r="G205" s="9">
+        <v>0</v>
+      </c>
+      <c r="H205" s="9">
+        <v>0</v>
+      </c>
+      <c r="I205" s="9">
+        <v>62.55</v>
+      </c>
+      <c r="J205" s="9">
+        <v>0</v>
+      </c>
+      <c r="K205" s="9">
+        <v>0</v>
+      </c>
+      <c r="L205" s="9">
+        <v>0</v>
+      </c>
+      <c r="M205" s="9">
+        <v>0</v>
+      </c>
+      <c r="N205" s="11">
+        <v>349976</v>
+      </c>
+      <c r="O205" s="11">
+        <v>349976</v>
+      </c>
+      <c r="P205" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q205" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="R205" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="S205" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="T205" s="10"/>
+      <c r="U205" s="9">
+        <v>0</v>
+      </c>
+      <c r="V205" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W205" s="9">
+        <v>0</v>
+      </c>
+      <c r="X205" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y205" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z205" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA205" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB205" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC205" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD205" s="12">
+        <v>72042766</v>
+      </c>
+      <c r="AE205" s="12">
+        <v>72042766</v>
+      </c>
+      <c r="AF205" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:32">
+      <c r="A206" s="8">
+        <v>46048</v>
+      </c>
+      <c r="B206" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C206" s="10"/>
+      <c r="D206" s="9">
+        <v>2359</v>
+      </c>
+      <c r="E206" s="9">
+        <v>0</v>
+      </c>
+      <c r="F206" s="11">
+        <v>25000</v>
+      </c>
+      <c r="G206" s="9">
+        <v>118.559</v>
+      </c>
+      <c r="H206" s="11">
+        <v>2963990</v>
+      </c>
+      <c r="I206" s="9">
+        <v>113.5</v>
+      </c>
+      <c r="J206" s="11">
+        <v>2837500</v>
+      </c>
+      <c r="K206" s="11">
+        <v>-126490</v>
+      </c>
+      <c r="L206" s="12">
+        <v>-26086425</v>
+      </c>
+      <c r="M206" s="9">
+        <v>0</v>
+      </c>
+      <c r="N206" s="9">
+        <v>0</v>
+      </c>
+      <c r="O206" s="9">
+        <v>0</v>
+      </c>
+      <c r="P206" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q206" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="R206" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="S206" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="T206" s="10"/>
+      <c r="U206" s="9">
+        <v>0</v>
+      </c>
+      <c r="V206" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W206" s="9">
+        <v>188.95</v>
+      </c>
+      <c r="X206" s="12">
+        <v>560075550</v>
+      </c>
+      <c r="Y206" s="9">
+        <v>188.19</v>
+      </c>
+      <c r="Z206" s="12">
+        <v>533989125</v>
+      </c>
+      <c r="AA206" s="12">
+        <v>-23804153</v>
+      </c>
+      <c r="AB206" s="12">
+        <v>-2282272</v>
+      </c>
+      <c r="AC206" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD206" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE206" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF206" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:32">
+      <c r="A207" s="8">
+        <v>46048</v>
+      </c>
+      <c r="B207" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C207" s="10"/>
+      <c r="D207" s="9">
+        <v>6680</v>
+      </c>
+      <c r="E207" s="9">
+        <v>0</v>
+      </c>
+      <c r="F207" s="11">
+        <v>130000</v>
+      </c>
+      <c r="G207" s="9">
+        <v>22.469000000000001</v>
+      </c>
+      <c r="H207" s="11">
+        <v>2921022</v>
+      </c>
+      <c r="I207" s="9">
+        <v>23.06</v>
+      </c>
+      <c r="J207" s="11">
+        <v>2997800</v>
+      </c>
+      <c r="K207" s="11">
+        <v>76778</v>
+      </c>
+      <c r="L207" s="12">
+        <v>12404137</v>
+      </c>
+      <c r="M207" s="9">
+        <v>0</v>
+      </c>
+      <c r="N207" s="9">
+        <v>0</v>
+      </c>
+      <c r="O207" s="9">
+        <v>0</v>
+      </c>
+      <c r="P207" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q207" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="R207" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="S207" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="T207" s="10"/>
+      <c r="U207" s="9">
+        <v>0</v>
+      </c>
+      <c r="V207" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W207" s="9">
+        <v>188.88</v>
+      </c>
+      <c r="X207" s="12">
+        <v>551751845</v>
+      </c>
+      <c r="Y207" s="9">
+        <v>188.19</v>
+      </c>
+      <c r="Z207" s="12">
+        <v>564155982</v>
+      </c>
+      <c r="AA207" s="12">
+        <v>14448851</v>
+      </c>
+      <c r="AB207" s="12">
+        <v>-2044715</v>
+      </c>
+      <c r="AC207" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD207" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE207" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF207" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:32">
+      <c r="A208" s="8">
+        <v>46048</v>
+      </c>
+      <c r="B208" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C208" s="10"/>
+      <c r="D208" s="9">
+        <v>6181</v>
+      </c>
+      <c r="E208" s="9">
+        <v>0</v>
+      </c>
+      <c r="F208" s="9">
+        <v>0</v>
+      </c>
+      <c r="G208" s="9">
+        <v>0</v>
+      </c>
+      <c r="H208" s="9">
+        <v>0</v>
+      </c>
+      <c r="I208" s="9">
+        <v>846.5</v>
+      </c>
+      <c r="J208" s="9">
+        <v>0</v>
+      </c>
+      <c r="K208" s="9">
+        <v>0</v>
+      </c>
+      <c r="L208" s="9">
+        <v>0</v>
+      </c>
+      <c r="M208" s="9">
+        <v>0</v>
+      </c>
+      <c r="N208" s="11">
+        <v>-6374.88</v>
+      </c>
+      <c r="O208" s="9">
+        <v>0</v>
+      </c>
+      <c r="P208" s="11">
+        <v>6374.88</v>
+      </c>
+      <c r="Q208" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="R208" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="S208" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="T208" s="10"/>
+      <c r="U208" s="9">
+        <v>0</v>
+      </c>
+      <c r="V208" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W208" s="9">
+        <v>0</v>
+      </c>
+      <c r="X208" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y208" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z208" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA208" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB208" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC208" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD208" s="12">
+        <v>1362525</v>
+      </c>
+      <c r="AE208" s="12">
+        <v>1362525</v>
+      </c>
+      <c r="AF208" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:32">
+      <c r="A209" s="8">
+        <v>46048</v>
+      </c>
+      <c r="B209" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C209" s="10"/>
+      <c r="D209" s="9">
+        <v>6082</v>
+      </c>
+      <c r="E209" s="9">
+        <v>0</v>
+      </c>
+      <c r="F209" s="9">
+        <v>0</v>
+      </c>
+      <c r="G209" s="9">
+        <v>0</v>
+      </c>
+      <c r="H209" s="9">
+        <v>0</v>
+      </c>
+      <c r="I209" s="9">
+        <v>34.46</v>
+      </c>
+      <c r="J209" s="9">
+        <v>0</v>
+      </c>
+      <c r="K209" s="9">
+        <v>0</v>
+      </c>
+      <c r="L209" s="9">
+        <v>0</v>
+      </c>
+      <c r="M209" s="9">
+        <v>0</v>
+      </c>
+      <c r="N209" s="11">
+        <v>205980</v>
+      </c>
+      <c r="O209" s="11">
+        <v>205980</v>
+      </c>
+      <c r="P209" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q209" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="R209" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="S209" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="T209" s="10"/>
+      <c r="U209" s="9">
+        <v>0</v>
+      </c>
+      <c r="V209" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W209" s="9">
+        <v>0</v>
+      </c>
+      <c r="X209" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y209" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z209" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA209" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB209" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC209" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD209" s="12">
+        <v>49395681</v>
+      </c>
+      <c r="AE209" s="12">
+        <v>49395681</v>
+      </c>
+      <c r="AF209" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:32">
+      <c r="A210" s="8">
+        <v>46048</v>
+      </c>
+      <c r="B210" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C210" s="10"/>
+      <c r="D210" s="9">
+        <v>9988</v>
+      </c>
+      <c r="E210" s="9">
+        <v>0</v>
+      </c>
+      <c r="F210" s="11">
+        <v>70500</v>
+      </c>
+      <c r="G210" s="9">
+        <v>147.79</v>
+      </c>
+      <c r="H210" s="11">
+        <v>10419200</v>
+      </c>
+      <c r="I210" s="9">
+        <v>165</v>
+      </c>
+      <c r="J210" s="11">
+        <v>11632500</v>
+      </c>
+      <c r="K210" s="11">
+        <v>1213300</v>
+      </c>
+      <c r="L210" s="12">
+        <v>254321575</v>
+      </c>
+      <c r="M210" s="9">
+        <v>0</v>
+      </c>
+      <c r="N210" s="9">
+        <v>0</v>
+      </c>
+      <c r="O210" s="9">
+        <v>0</v>
+      </c>
+      <c r="P210" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q210" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="R210" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="S210" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="T210" s="10"/>
+      <c r="U210" s="9">
+        <v>0</v>
+      </c>
+      <c r="V210" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W210" s="9">
+        <v>185.69</v>
+      </c>
+      <c r="X210" s="12">
+        <v>1934798600</v>
+      </c>
+      <c r="Y210" s="9">
+        <v>188.19</v>
+      </c>
+      <c r="Z210" s="12">
+        <v>2189120175</v>
+      </c>
+      <c r="AA210" s="12">
+        <v>228330927</v>
+      </c>
+      <c r="AB210" s="12">
+        <v>25990648</v>
+      </c>
+      <c r="AC210" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD210" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE210" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF210" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:32">
+      <c r="A211" s="8">
+        <v>46048</v>
+      </c>
+      <c r="B211" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C211" s="10"/>
+      <c r="D211" s="9">
+        <v>6861</v>
+      </c>
+      <c r="E211" s="9">
+        <v>0</v>
+      </c>
+      <c r="F211" s="11">
+        <v>1900</v>
+      </c>
+      <c r="G211" s="11">
+        <v>55916.79</v>
+      </c>
+      <c r="H211" s="11">
+        <v>106241900</v>
+      </c>
+      <c r="I211" s="11">
+        <v>58390</v>
+      </c>
+      <c r="J211" s="11">
+        <v>110941000</v>
+      </c>
+      <c r="K211" s="11">
+        <v>4699100</v>
+      </c>
+      <c r="L211" s="12">
+        <v>70533092</v>
+      </c>
+      <c r="M211" s="9">
+        <v>0</v>
+      </c>
+      <c r="N211" s="9">
+        <v>0</v>
+      </c>
+      <c r="O211" s="9">
+        <v>0</v>
+      </c>
+      <c r="P211" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q211" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="R211" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="S211" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="T211" s="10"/>
+      <c r="U211" s="9">
+        <v>0</v>
+      </c>
+      <c r="V211" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W211" s="9">
+        <v>924.45</v>
+      </c>
+      <c r="X211" s="12">
+        <v>982163868</v>
+      </c>
+      <c r="Y211" s="9">
+        <v>948.88</v>
+      </c>
+      <c r="Z211" s="12">
+        <v>1052696960</v>
+      </c>
+      <c r="AA211" s="12">
+        <v>44588820</v>
+      </c>
+      <c r="AB211" s="12">
+        <v>25944272</v>
+      </c>
+      <c r="AC211" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD211" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE211" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF211" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:32">
+      <c r="A212" s="8">
+        <v>46048</v>
+      </c>
+      <c r="B212" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C212" s="10"/>
+      <c r="D212" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E212" s="9">
+        <v>0</v>
+      </c>
+      <c r="F212" s="9">
+        <v>0</v>
+      </c>
+      <c r="G212" s="9">
+        <v>0</v>
+      </c>
+      <c r="H212" s="9">
+        <v>0</v>
+      </c>
+      <c r="I212" s="11">
+        <v>17450</v>
+      </c>
+      <c r="J212" s="9">
+        <v>0</v>
+      </c>
+      <c r="K212" s="9">
+        <v>0</v>
+      </c>
+      <c r="L212" s="9">
+        <v>0</v>
+      </c>
+      <c r="M212" s="9">
+        <v>0</v>
+      </c>
+      <c r="N212" s="11">
+        <v>4480700</v>
+      </c>
+      <c r="O212" s="11">
+        <v>4480700</v>
+      </c>
+      <c r="P212" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q212" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="R212" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="S212" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="T212" s="10"/>
+      <c r="U212" s="9">
+        <v>0</v>
+      </c>
+      <c r="V212" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W212" s="9">
+        <v>0</v>
+      </c>
+      <c r="X212" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y212" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z212" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA212" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB212" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC212" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD212" s="12">
+        <v>37760160</v>
+      </c>
+      <c r="AE212" s="12">
+        <v>37760160</v>
+      </c>
+      <c r="AF212" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:32">
+      <c r="A213" s="8">
+        <v>46048</v>
+      </c>
+      <c r="B213" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C213" s="10"/>
+      <c r="D213" s="9">
+        <v>9984</v>
+      </c>
+      <c r="E213" s="9">
+        <v>0</v>
+      </c>
+      <c r="F213" s="11">
+        <v>23000</v>
+      </c>
+      <c r="G213" s="11">
+        <v>4066.73</v>
+      </c>
+      <c r="H213" s="11">
+        <v>93534900</v>
+      </c>
+      <c r="I213" s="11">
+        <v>4065</v>
+      </c>
+      <c r="J213" s="11">
+        <v>93495000</v>
+      </c>
+      <c r="K213" s="11">
+        <v>-39900</v>
+      </c>
+      <c r="L213" s="12">
+        <v>20535801</v>
+      </c>
+      <c r="M213" s="9">
+        <v>0</v>
+      </c>
+      <c r="N213" s="9">
+        <v>0</v>
+      </c>
+      <c r="O213" s="9">
+        <v>0</v>
+      </c>
+      <c r="P213" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q213" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="R213" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="S213" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="T213" s="10"/>
+      <c r="U213" s="9">
+        <v>0</v>
+      </c>
+      <c r="V213" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W213" s="9">
+        <v>926.51</v>
+      </c>
+      <c r="X213" s="12">
+        <v>866619555</v>
+      </c>
+      <c r="Y213" s="9">
+        <v>948.88</v>
+      </c>
+      <c r="Z213" s="12">
+        <v>887155356</v>
+      </c>
+      <c r="AA213" s="12">
+        <v>-378603</v>
+      </c>
+      <c r="AB213" s="12">
+        <v>20914404</v>
+      </c>
+      <c r="AC213" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD213" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE213" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF213" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:32">
+      <c r="A214" s="8">
+        <v>46048</v>
+      </c>
+      <c r="B214" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C214" s="10"/>
+      <c r="D214" s="9">
+        <v>6954</v>
+      </c>
+      <c r="E214" s="9">
+        <v>0</v>
+      </c>
+      <c r="F214" s="11">
+        <v>10000</v>
+      </c>
+      <c r="G214" s="11">
+        <v>6568.27</v>
+      </c>
+      <c r="H214" s="11">
+        <v>65682650</v>
+      </c>
+      <c r="I214" s="11">
+        <v>6394</v>
+      </c>
+      <c r="J214" s="11">
+        <v>63940000</v>
+      </c>
+      <c r="K214" s="11">
+        <v>-1742650</v>
+      </c>
+      <c r="L214" s="12">
+        <v>-2177430</v>
+      </c>
+      <c r="M214" s="9">
+        <v>0</v>
+      </c>
+      <c r="N214" s="9">
+        <v>0</v>
+      </c>
+      <c r="O214" s="9">
+        <v>0</v>
+      </c>
+      <c r="P214" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q214" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="R214" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="S214" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="T214" s="10"/>
+      <c r="U214" s="9">
+        <v>0</v>
+      </c>
+      <c r="V214" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W214" s="9">
+        <v>927.01</v>
+      </c>
+      <c r="X214" s="12">
+        <v>608891302</v>
+      </c>
+      <c r="Y214" s="9">
+        <v>948.88</v>
+      </c>
+      <c r="Z214" s="12">
+        <v>606713872</v>
+      </c>
+      <c r="AA214" s="12">
+        <v>-16535657</v>
+      </c>
+      <c r="AB214" s="12">
+        <v>14358227</v>
+      </c>
+      <c r="AC214" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD214" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE214" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF214" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:32">
+      <c r="A215" s="8">
+        <v>46048</v>
+      </c>
+      <c r="B215" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C215" s="10"/>
+      <c r="D215" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E215" s="9">
+        <v>0</v>
+      </c>
+      <c r="F215" s="11">
+        <v>38000</v>
+      </c>
+      <c r="G215" s="9">
+        <v>12.58</v>
+      </c>
+      <c r="H215" s="11">
+        <v>478066.6</v>
+      </c>
+      <c r="I215" s="9">
+        <v>12.71</v>
+      </c>
+      <c r="J215" s="11">
+        <v>482980</v>
+      </c>
+      <c r="K215" s="11">
+        <v>4913.3999999999996</v>
+      </c>
+      <c r="L215" s="12">
+        <v>6635261</v>
+      </c>
+      <c r="M215" s="9">
+        <v>0</v>
+      </c>
+      <c r="N215" s="9">
+        <v>0</v>
+      </c>
+      <c r="O215" s="9">
+        <v>0</v>
+      </c>
+      <c r="P215" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q215" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R215" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S215" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="T215" s="10"/>
+      <c r="U215" s="9">
+        <v>0</v>
+      </c>
+      <c r="V215" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W215" s="11">
+        <v>1468.39</v>
+      </c>
+      <c r="X215" s="12">
+        <v>701992995</v>
+      </c>
+      <c r="Y215" s="11">
+        <v>1467.2</v>
+      </c>
+      <c r="Z215" s="12">
+        <v>708628256</v>
+      </c>
+      <c r="AA215" s="12">
+        <v>7208940</v>
+      </c>
+      <c r="AB215" s="12">
+        <v>-573680</v>
+      </c>
+      <c r="AC215" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD215" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE215" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF215" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:32">
+      <c r="A216" s="8">
+        <v>46048</v>
+      </c>
+      <c r="B216" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C216" s="10"/>
+      <c r="D216" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E216" s="9">
+        <v>0</v>
+      </c>
+      <c r="F216" s="11">
+        <v>10000</v>
+      </c>
+      <c r="G216" s="9">
+        <v>48.203000000000003</v>
+      </c>
+      <c r="H216" s="11">
+        <v>482030</v>
+      </c>
+      <c r="I216" s="9">
+        <v>51.06</v>
+      </c>
+      <c r="J216" s="11">
+        <v>510600</v>
+      </c>
+      <c r="K216" s="11">
+        <v>28570</v>
+      </c>
+      <c r="L216" s="12">
+        <v>47461249</v>
+      </c>
+      <c r="M216" s="9">
+        <v>0</v>
+      </c>
+      <c r="N216" s="9">
+        <v>0</v>
+      </c>
+      <c r="O216" s="9">
+        <v>0</v>
+      </c>
+      <c r="P216" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q216" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R216" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S216" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="T216" s="10"/>
+      <c r="U216" s="9">
+        <v>0</v>
+      </c>
+      <c r="V216" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W216" s="11">
+        <v>1455.7</v>
+      </c>
+      <c r="X216" s="12">
+        <v>701691071</v>
+      </c>
+      <c r="Y216" s="11">
+        <v>1467.2</v>
+      </c>
+      <c r="Z216" s="12">
+        <v>749152320</v>
+      </c>
+      <c r="AA216" s="12">
+        <v>41917904</v>
+      </c>
+      <c r="AB216" s="12">
+        <v>5543345</v>
+      </c>
+      <c r="AC216" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD216" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE216" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF216" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:32">
+      <c r="A217" s="8">
+        <v>46048</v>
+      </c>
+      <c r="B217" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C217" s="10"/>
+      <c r="D217" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E217" s="9">
+        <v>0</v>
+      </c>
+      <c r="F217" s="11">
+        <v>20000</v>
+      </c>
+      <c r="G217" s="9">
+        <v>34.24</v>
+      </c>
+      <c r="H217" s="11">
+        <v>684800</v>
+      </c>
+      <c r="I217" s="9">
+        <v>34.75</v>
+      </c>
+      <c r="J217" s="11">
+        <v>695000</v>
+      </c>
+      <c r="K217" s="11">
+        <v>10200</v>
+      </c>
+      <c r="L217" s="12">
+        <v>8254400</v>
+      </c>
+      <c r="M217" s="9">
+        <v>0</v>
+      </c>
+      <c r="N217" s="9">
+        <v>0</v>
+      </c>
+      <c r="O217" s="9">
+        <v>0</v>
+      </c>
+      <c r="P217" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q217" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R217" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S217" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="T217" s="10"/>
+      <c r="U217" s="9">
+        <v>0</v>
+      </c>
+      <c r="V217" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W217" s="11">
+        <v>1477</v>
+      </c>
+      <c r="X217" s="12">
+        <v>1011449600</v>
+      </c>
+      <c r="Y217" s="11">
+        <v>1467.2</v>
+      </c>
+      <c r="Z217" s="12">
+        <v>1019704000</v>
+      </c>
+      <c r="AA217" s="12">
+        <v>14965440</v>
+      </c>
+      <c r="AB217" s="12">
+        <v>-6711040</v>
+      </c>
+      <c r="AC217" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD217" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE217" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF217" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:32">
+      <c r="A218" s="8">
+        <v>46048</v>
+      </c>
+      <c r="B218" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C218" s="10"/>
+      <c r="D218" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E218" s="9">
+        <v>0</v>
+      </c>
+      <c r="F218" s="11">
+        <v>3000</v>
+      </c>
+      <c r="G218" s="9">
+        <v>247.65</v>
+      </c>
+      <c r="H218" s="11">
+        <v>742950</v>
+      </c>
+      <c r="I218" s="9">
+        <v>248.18</v>
+      </c>
+      <c r="J218" s="11">
+        <v>744540</v>
+      </c>
+      <c r="K218" s="11">
+        <v>1590</v>
+      </c>
+      <c r="L218" s="12">
+        <v>-4948062</v>
+      </c>
+      <c r="M218" s="9">
+        <v>0</v>
+      </c>
+      <c r="N218" s="9">
+        <v>0</v>
+      </c>
+      <c r="O218" s="9">
+        <v>0</v>
+      </c>
+      <c r="P218" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q218" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R218" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S218" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="T218" s="10"/>
+      <c r="U218" s="9">
+        <v>0</v>
+      </c>
+      <c r="V218" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W218" s="11">
+        <v>1477</v>
+      </c>
+      <c r="X218" s="12">
+        <v>1097337150</v>
+      </c>
+      <c r="Y218" s="11">
+        <v>1467.2</v>
+      </c>
+      <c r="Z218" s="12">
+        <v>1092389088</v>
+      </c>
+      <c r="AA218" s="12">
+        <v>2332848</v>
+      </c>
+      <c r="AB218" s="12">
+        <v>-7280910</v>
+      </c>
+      <c r="AC218" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD218" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE218" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF218" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:32">
+      <c r="A219" s="8">
+        <v>46048</v>
+      </c>
+      <c r="B219" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C219" s="10"/>
+      <c r="D219" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E219" s="9">
+        <v>0</v>
+      </c>
+      <c r="F219" s="11">
+        <v>83000</v>
+      </c>
+      <c r="G219" s="9">
+        <v>12.374000000000001</v>
+      </c>
+      <c r="H219" s="11">
+        <v>1027042</v>
+      </c>
+      <c r="I219" s="9">
+        <v>9.83</v>
+      </c>
+      <c r="J219" s="11">
+        <v>815890</v>
+      </c>
+      <c r="K219" s="11">
+        <v>-211152</v>
+      </c>
+      <c r="L219" s="12">
+        <v>-287720811</v>
+      </c>
+      <c r="M219" s="9">
+        <v>0</v>
+      </c>
+      <c r="N219" s="9">
+        <v>0</v>
+      </c>
+      <c r="O219" s="9">
+        <v>0</v>
+      </c>
+      <c r="P219" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q219" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R219" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S219" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="T219" s="10"/>
+      <c r="U219" s="9">
+        <v>0</v>
+      </c>
+      <c r="V219" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W219" s="11">
+        <v>1445.69</v>
+      </c>
+      <c r="X219" s="12">
+        <v>1484794619</v>
+      </c>
+      <c r="Y219" s="11">
+        <v>1467.2</v>
+      </c>
+      <c r="Z219" s="12">
+        <v>1197073808</v>
+      </c>
+      <c r="AA219" s="12">
+        <v>-309802214</v>
+      </c>
+      <c r="AB219" s="12">
+        <v>22081403</v>
+      </c>
+      <c r="AC219" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD219" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE219" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF219" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:32">
+      <c r="A220" s="8">
+        <v>46048</v>
+      </c>
+      <c r="B220" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C220" s="10"/>
+      <c r="D220" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E220" s="9">
+        <v>0</v>
+      </c>
+      <c r="F220" s="11">
+        <v>10000</v>
+      </c>
+      <c r="G220" s="9">
+        <v>44.158999999999999</v>
+      </c>
+      <c r="H220" s="11">
+        <v>441591</v>
+      </c>
+      <c r="I220" s="9">
+        <v>44.63</v>
+      </c>
+      <c r="J220" s="11">
+        <v>446300</v>
+      </c>
+      <c r="K220" s="11">
+        <v>4709</v>
+      </c>
+      <c r="L220" s="12">
+        <v>6379136</v>
+      </c>
+      <c r="M220" s="9">
+        <v>0</v>
+      </c>
+      <c r="N220" s="9">
+        <v>0</v>
+      </c>
+      <c r="O220" s="9">
+        <v>0</v>
+      </c>
+      <c r="P220" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q220" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R220" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S220" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="T220" s="10"/>
+      <c r="U220" s="9">
+        <v>0</v>
+      </c>
+      <c r="V220" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W220" s="11">
+        <v>1468.39</v>
+      </c>
+      <c r="X220" s="12">
+        <v>648432224</v>
+      </c>
+      <c r="Y220" s="11">
+        <v>1467.2</v>
+      </c>
+      <c r="Z220" s="12">
+        <v>654811360</v>
+      </c>
+      <c r="AA220" s="12">
+        <v>6909044</v>
+      </c>
+      <c r="AB220" s="12">
+        <v>-529909</v>
+      </c>
+      <c r="AC220" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD220" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE220" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF220" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:32">
+      <c r="A221" s="8">
+        <v>46048</v>
+      </c>
+      <c r="B221" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C221" s="10"/>
+      <c r="D221" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E221" s="9">
+        <v>0</v>
+      </c>
+      <c r="F221" s="11">
+        <v>1000</v>
+      </c>
+      <c r="G221" s="9">
+        <v>681.92</v>
+      </c>
+      <c r="H221" s="11">
+        <v>681920</v>
+      </c>
+      <c r="I221" s="9">
+        <v>688.32</v>
+      </c>
+      <c r="J221" s="11">
+        <v>688320</v>
+      </c>
+      <c r="K221" s="11">
+        <v>6400</v>
+      </c>
+      <c r="L221" s="12">
+        <v>31416096</v>
+      </c>
+      <c r="M221" s="11">
+        <v>11310.3</v>
+      </c>
+      <c r="N221" s="11">
+        <v>20010.3</v>
+      </c>
+      <c r="O221" s="11">
+        <v>20010.3</v>
+      </c>
+      <c r="P221" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q221" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R221" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S221" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="T221" s="10"/>
+      <c r="U221" s="9">
+        <v>0</v>
+      </c>
+      <c r="V221" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="W221" s="11">
+        <v>1434.9</v>
+      </c>
+      <c r="X221" s="12">
+        <v>978487008</v>
+      </c>
+      <c r="Y221" s="11">
+        <v>1467.2</v>
+      </c>
+      <c r="Z221" s="12">
+        <v>1009903104</v>
+      </c>
+      <c r="AA221" s="12">
+        <v>9390080</v>
+      </c>
+      <c r="AB221" s="12">
+        <v>22026016</v>
+      </c>
+      <c r="AC221" s="12">
+        <v>50874524</v>
+      </c>
+      <c r="AD221" s="12">
+        <v>135496504</v>
+      </c>
+      <c r="AE221" s="12">
+        <v>135496504</v>
+      </c>
+      <c r="AF221" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:32">
+      <c r="A222" s="8">
+        <v>46048</v>
+      </c>
+      <c r="B222" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C222" s="10"/>
+      <c r="D222" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E222" s="9">
+        <v>0</v>
+      </c>
+      <c r="F222" s="11">
+        <v>4200</v>
+      </c>
+      <c r="G222" s="9">
+        <v>396.31</v>
+      </c>
+      <c r="H222" s="11">
+        <v>1664502</v>
+      </c>
+      <c r="I222" s="9">
+        <v>468.18</v>
+      </c>
+      <c r="J222" s="11">
+        <v>1966356</v>
+      </c>
+      <c r="K222" s="11">
+        <v>301854</v>
+      </c>
+      <c r="L222" s="12">
+        <v>496643604</v>
+      </c>
+      <c r="M222" s="9">
+        <v>0</v>
+      </c>
+      <c r="N222" s="9">
+        <v>0</v>
+      </c>
+      <c r="O222" s="9">
+        <v>0</v>
+      </c>
+      <c r="P222" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q222" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R222" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S222" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="T222" s="10"/>
+      <c r="U222" s="9">
+        <v>0</v>
+      </c>
+      <c r="V222" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="W222" s="11">
+        <v>1434.89</v>
+      </c>
+      <c r="X222" s="12">
+        <v>2388393919</v>
+      </c>
+      <c r="Y222" s="11">
+        <v>1467.2</v>
+      </c>
+      <c r="Z222" s="12">
+        <v>2885037523</v>
+      </c>
+      <c r="AA222" s="12">
+        <v>442880188</v>
+      </c>
+      <c r="AB222" s="12">
+        <v>53763415</v>
+      </c>
+      <c r="AC222" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD222" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE222" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF222" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:32">
+      <c r="A223" s="8">
+        <v>46048</v>
+      </c>
+      <c r="B223" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C223" s="10"/>
+      <c r="D223" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E223" s="9">
+        <v>0</v>
+      </c>
+      <c r="F223" s="11">
+        <v>24000</v>
+      </c>
+      <c r="G223" s="9">
+        <v>17.655000000000001</v>
+      </c>
+      <c r="H223" s="11">
+        <v>423736.8</v>
+      </c>
+      <c r="I223" s="9">
+        <v>17.27</v>
+      </c>
+      <c r="J223" s="11">
+        <v>414480</v>
+      </c>
+      <c r="K223" s="11">
+        <v>-9256.7999999999993</v>
+      </c>
+      <c r="L223" s="12">
+        <v>-12267992</v>
+      </c>
+      <c r="M223" s="9">
+        <v>0</v>
+      </c>
+      <c r="N223" s="9">
+        <v>0</v>
+      </c>
+      <c r="O223" s="9">
+        <v>0</v>
+      </c>
+      <c r="P223" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q223" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R223" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S223" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="T223" s="10"/>
+      <c r="U223" s="9">
+        <v>0</v>
+      </c>
+      <c r="V223" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W223" s="11">
+        <v>1464.09</v>
+      </c>
+      <c r="X223" s="12">
+        <v>620393048</v>
+      </c>
+      <c r="Y223" s="11">
+        <v>1467.2</v>
+      </c>
+      <c r="Z223" s="12">
+        <v>608125056</v>
+      </c>
+      <c r="AA223" s="12">
+        <v>-13581576</v>
+      </c>
+      <c r="AB223" s="12">
+        <v>1313584</v>
+      </c>
+      <c r="AC223" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD223" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE223" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF223" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:32">
+      <c r="A224" s="8">
+        <v>46048</v>
+      </c>
+      <c r="B224" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C224" s="10"/>
+      <c r="D224" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E224" s="9">
+        <v>0</v>
+      </c>
+      <c r="F224" s="11">
+        <v>1400</v>
+      </c>
+      <c r="G224" s="9">
+        <v>432.53800000000001</v>
+      </c>
+      <c r="H224" s="11">
+        <v>605554.04</v>
+      </c>
+      <c r="I224" s="9">
+        <v>444.48</v>
+      </c>
+      <c r="J224" s="11">
+        <v>622272</v>
+      </c>
+      <c r="K224" s="11">
+        <v>16717.96</v>
+      </c>
+      <c r="L224" s="12">
+        <v>36881893</v>
+      </c>
+      <c r="M224" s="9">
+        <v>0</v>
+      </c>
+      <c r="N224" s="9">
+        <v>0</v>
+      </c>
+      <c r="O224" s="9">
+        <v>0</v>
+      </c>
+      <c r="P224" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q224" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R224" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S224" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="T224" s="10"/>
+      <c r="U224" s="9">
+        <v>0</v>
+      </c>
+      <c r="V224" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W224" s="11">
+        <v>1446.79</v>
+      </c>
+      <c r="X224" s="12">
+        <v>876115585</v>
+      </c>
+      <c r="Y224" s="11">
+        <v>1467.2</v>
+      </c>
+      <c r="Z224" s="12">
+        <v>912997478</v>
+      </c>
+      <c r="AA224" s="12">
+        <v>24528590</v>
+      </c>
+      <c r="AB224" s="12">
+        <v>12353302</v>
+      </c>
+      <c r="AC224" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD224" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE224" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF224" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="225" spans="1:32" ht="18" thickBot="1">
-      <c r="A225" s="2"/>
-      <c r="B225" s="2"/>
-      <c r="C225" s="2"/>
-      <c r="D225" s="2"/>
-      <c r="E225" s="2"/>
-      <c r="F225" s="2"/>
-      <c r="G225" s="2"/>
-      <c r="H225" s="2"/>
-      <c r="I225" s="2"/>
-      <c r="J225" s="2"/>
-      <c r="K225" s="2"/>
-      <c r="L225" s="2"/>
-      <c r="M225" s="2"/>
-      <c r="N225" s="2"/>
-      <c r="O225" s="2"/>
-      <c r="P225" s="2"/>
-      <c r="Q225" s="2"/>
-      <c r="R225" s="2"/>
-      <c r="S225" s="2"/>
-      <c r="T225" s="2"/>
-      <c r="U225" s="2"/>
-      <c r="V225" s="2"/>
-      <c r="W225" s="2"/>
-      <c r="X225" s="2"/>
-      <c r="Y225" s="2"/>
-      <c r="Z225" s="2"/>
-      <c r="AA225" s="2"/>
-      <c r="AB225" s="2"/>
-      <c r="AC225" s="2"/>
-      <c r="AD225" s="2"/>
-      <c r="AE225" s="2"/>
-      <c r="AF225" s="2"/>
+      <c r="A225" s="8">
+        <v>46048</v>
+      </c>
+      <c r="B225" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C225" s="10"/>
+      <c r="D225" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E225" s="9">
+        <v>0</v>
+      </c>
+      <c r="F225" s="11">
+        <v>3500</v>
+      </c>
+      <c r="G225" s="9">
+        <v>169.042</v>
+      </c>
+      <c r="H225" s="11">
+        <v>591649.80000000005</v>
+      </c>
+      <c r="I225" s="9">
+        <v>159.19999999999999</v>
+      </c>
+      <c r="J225" s="11">
+        <v>557200</v>
+      </c>
+      <c r="K225" s="11">
+        <v>-34449.800000000003</v>
+      </c>
+      <c r="L225" s="12">
+        <v>-38475090</v>
+      </c>
+      <c r="M225" s="9">
+        <v>0</v>
+      </c>
+      <c r="N225" s="9">
+        <v>0</v>
+      </c>
+      <c r="O225" s="9">
+        <v>0</v>
+      </c>
+      <c r="P225" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q225" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R225" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S225" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="T225" s="10"/>
+      <c r="U225" s="9">
+        <v>0</v>
+      </c>
+      <c r="V225" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W225" s="11">
+        <v>1446.79</v>
+      </c>
+      <c r="X225" s="12">
+        <v>855998930</v>
+      </c>
+      <c r="Y225" s="11">
+        <v>1467.2</v>
+      </c>
+      <c r="Z225" s="12">
+        <v>817523840</v>
+      </c>
+      <c r="AA225" s="12">
+        <v>-50544746</v>
+      </c>
+      <c r="AB225" s="12">
+        <v>12069656</v>
+      </c>
+      <c r="AC225" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD225" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE225" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF225" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="226" spans="1:32" ht="18" thickBot="1">
       <c r="A226" s="2"/>

</xml_diff>

<commit_message>
Update 2026_멀티.xlsx (2026-01-29 15:48:15)
</commit_message>
<xml_diff>
--- a/2026_멀티.xlsx
+++ b/2026_멀티.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyejinha/Desktop/Workspace/Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3F3C77-BB96-A54B-A54B-283757F272A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE413AF-2E1D-1748-AE52-2C0B66A8FB8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -696,7 +696,7 @@
   <dimension ref="A1:AF1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A261" workbookViewId="0">
-      <selection activeCell="A268" sqref="A268:AF288"/>
+      <selection activeCell="B292" sqref="B292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>

</xml_diff>

<commit_message>
Update 2026_멀티.xlsx (2026-02-20 18:23:45)
</commit_message>
<xml_diff>
--- a/2026_멀티.xlsx
+++ b/2026_멀티.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\다른 컴퓨터\내 Mac\Workspace\Team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F19A72-92AE-4395-810F-5B3EA351731D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091DB785-CD97-4DAB-A5DE-6370372E7140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3923" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4097" uniqueCount="125">
   <si>
     <t>기준일자</t>
   </si>
@@ -790,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A530" workbookViewId="0">
-      <selection activeCell="D544" sqref="D544"/>
+    <sheetView tabSelected="1" topLeftCell="A709" workbookViewId="0">
+      <selection activeCell="F730" sqref="F730"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -66129,1058 +66129,2896 @@
       </c>
     </row>
     <row r="699" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A699" s="2"/>
-      <c r="B699" s="2"/>
+      <c r="A699" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B699" s="4" t="s">
+        <v>122</v>
+      </c>
       <c r="C699" s="2"/>
-      <c r="D699" s="2"/>
-      <c r="E699" s="2"/>
-      <c r="F699" s="2"/>
-      <c r="G699" s="2"/>
-      <c r="H699" s="2"/>
-      <c r="I699" s="2"/>
-      <c r="J699" s="2"/>
-      <c r="K699" s="2"/>
-      <c r="L699" s="2"/>
-      <c r="M699" s="2"/>
-      <c r="N699" s="2"/>
-      <c r="O699" s="2"/>
-      <c r="P699" s="2"/>
-      <c r="Q699" s="2"/>
-      <c r="R699" s="2"/>
-      <c r="S699" s="2"/>
+      <c r="D699" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E699" s="5">
+        <v>0</v>
+      </c>
+      <c r="F699" s="6">
+        <v>6500</v>
+      </c>
+      <c r="G699" s="5">
+        <v>117.809</v>
+      </c>
+      <c r="H699" s="6">
+        <v>765763.05</v>
+      </c>
+      <c r="I699" s="5">
+        <v>119.03</v>
+      </c>
+      <c r="J699" s="6">
+        <v>773695</v>
+      </c>
+      <c r="K699" s="6">
+        <v>7931.95</v>
+      </c>
+      <c r="L699" s="7">
+        <v>2793475</v>
+      </c>
+      <c r="M699" s="5">
+        <v>0</v>
+      </c>
+      <c r="N699" s="5">
+        <v>0</v>
+      </c>
+      <c r="O699" s="5">
+        <v>0</v>
+      </c>
+      <c r="P699" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q699" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R699" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S699" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="T699" s="2"/>
-      <c r="U699" s="2"/>
-      <c r="V699" s="2"/>
-      <c r="W699" s="2"/>
-      <c r="X699" s="2"/>
-      <c r="Y699" s="2"/>
-      <c r="Z699" s="2"/>
-      <c r="AA699" s="2"/>
-      <c r="AB699" s="2"/>
-      <c r="AC699" s="2"/>
-      <c r="AD699" s="2"/>
-      <c r="AE699" s="2"/>
-      <c r="AF699" s="2"/>
+      <c r="U699" s="5">
+        <v>0</v>
+      </c>
+      <c r="V699" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W699" s="6">
+        <v>1454.39</v>
+      </c>
+      <c r="X699" s="7">
+        <v>1113725779</v>
+      </c>
+      <c r="Y699" s="6">
+        <v>1443.1</v>
+      </c>
+      <c r="Z699" s="7">
+        <v>1116519254</v>
+      </c>
+      <c r="AA699" s="7">
+        <v>11446597</v>
+      </c>
+      <c r="AB699" s="7">
+        <v>-8653122</v>
+      </c>
+      <c r="AC699" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD699" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE699" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF699" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="700" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A700" s="2"/>
-      <c r="B700" s="2"/>
+      <c r="A700" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B700" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="C700" s="2"/>
-      <c r="D700" s="2"/>
-      <c r="E700" s="2"/>
-      <c r="F700" s="2"/>
-      <c r="G700" s="2"/>
-      <c r="H700" s="2"/>
-      <c r="I700" s="2"/>
-      <c r="J700" s="2"/>
-      <c r="K700" s="2"/>
-      <c r="L700" s="2"/>
-      <c r="M700" s="2"/>
-      <c r="N700" s="2"/>
-      <c r="O700" s="2"/>
-      <c r="P700" s="2"/>
-      <c r="Q700" s="2"/>
-      <c r="R700" s="2"/>
-      <c r="S700" s="2"/>
+      <c r="D700" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E700" s="5">
+        <v>0</v>
+      </c>
+      <c r="F700" s="6">
+        <v>38000</v>
+      </c>
+      <c r="G700" s="5">
+        <v>12.58</v>
+      </c>
+      <c r="H700" s="6">
+        <v>478066.6</v>
+      </c>
+      <c r="I700" s="5">
+        <v>12.34</v>
+      </c>
+      <c r="J700" s="6">
+        <v>468920</v>
+      </c>
+      <c r="K700" s="6">
+        <v>-9146.6</v>
+      </c>
+      <c r="L700" s="7">
+        <v>-25294543</v>
+      </c>
+      <c r="M700" s="5">
+        <v>0</v>
+      </c>
+      <c r="N700" s="5">
+        <v>0</v>
+      </c>
+      <c r="O700" s="5">
+        <v>0</v>
+      </c>
+      <c r="P700" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q700" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R700" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S700" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="T700" s="2"/>
-      <c r="U700" s="2"/>
-      <c r="V700" s="2"/>
-      <c r="W700" s="2"/>
-      <c r="X700" s="2"/>
-      <c r="Y700" s="2"/>
-      <c r="Z700" s="2"/>
-      <c r="AA700" s="2"/>
-      <c r="AB700" s="2"/>
-      <c r="AC700" s="2"/>
-      <c r="AD700" s="2"/>
-      <c r="AE700" s="2"/>
-      <c r="AF700" s="2"/>
+      <c r="U700" s="5">
+        <v>0</v>
+      </c>
+      <c r="V700" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W700" s="6">
+        <v>1468.39</v>
+      </c>
+      <c r="X700" s="7">
+        <v>701992995</v>
+      </c>
+      <c r="Y700" s="6">
+        <v>1443.1</v>
+      </c>
+      <c r="Z700" s="7">
+        <v>676698452</v>
+      </c>
+      <c r="AA700" s="7">
+        <v>-13199458</v>
+      </c>
+      <c r="AB700" s="7">
+        <v>-12095085</v>
+      </c>
+      <c r="AC700" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD700" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE700" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF700" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="701" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A701" s="2"/>
-      <c r="B701" s="2"/>
+      <c r="A701" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B701" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="C701" s="2"/>
-      <c r="D701" s="2"/>
-      <c r="E701" s="2"/>
-      <c r="F701" s="2"/>
-      <c r="G701" s="2"/>
-      <c r="H701" s="2"/>
-      <c r="I701" s="2"/>
-      <c r="J701" s="2"/>
-      <c r="K701" s="2"/>
-      <c r="L701" s="2"/>
-      <c r="M701" s="2"/>
-      <c r="N701" s="2"/>
-      <c r="O701" s="2"/>
-      <c r="P701" s="2"/>
-      <c r="Q701" s="2"/>
-      <c r="R701" s="2"/>
-      <c r="S701" s="2"/>
+      <c r="D701" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E701" s="5">
+        <v>0</v>
+      </c>
+      <c r="F701" s="6">
+        <v>10000</v>
+      </c>
+      <c r="G701" s="5">
+        <v>48.203000000000003</v>
+      </c>
+      <c r="H701" s="6">
+        <v>482030</v>
+      </c>
+      <c r="I701" s="5">
+        <v>55.33</v>
+      </c>
+      <c r="J701" s="6">
+        <v>553300</v>
+      </c>
+      <c r="K701" s="6">
+        <v>71270</v>
+      </c>
+      <c r="L701" s="7">
+        <v>96776159</v>
+      </c>
+      <c r="M701" s="5">
+        <v>0</v>
+      </c>
+      <c r="N701" s="5">
+        <v>0</v>
+      </c>
+      <c r="O701" s="5">
+        <v>0</v>
+      </c>
+      <c r="P701" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q701" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R701" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S701" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="T701" s="2"/>
-      <c r="U701" s="2"/>
-      <c r="V701" s="2"/>
-      <c r="W701" s="2"/>
-      <c r="X701" s="2"/>
-      <c r="Y701" s="2"/>
-      <c r="Z701" s="2"/>
-      <c r="AA701" s="2"/>
-      <c r="AB701" s="2"/>
-      <c r="AC701" s="2"/>
-      <c r="AD701" s="2"/>
-      <c r="AE701" s="2"/>
-      <c r="AF701" s="2"/>
-    </row>
-    <row r="702" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A702" s="2"/>
-      <c r="B702" s="2"/>
+      <c r="U701" s="5">
+        <v>0</v>
+      </c>
+      <c r="V701" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W701" s="6">
+        <v>1455.7</v>
+      </c>
+      <c r="X701" s="7">
+        <v>701691071</v>
+      </c>
+      <c r="Y701" s="6">
+        <v>1443.1</v>
+      </c>
+      <c r="Z701" s="7">
+        <v>798467230</v>
+      </c>
+      <c r="AA701" s="7">
+        <v>102849737</v>
+      </c>
+      <c r="AB701" s="7">
+        <v>-6073578</v>
+      </c>
+      <c r="AC701" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD701" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE701" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF701" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="702" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A702" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B702" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="C702" s="2"/>
-      <c r="D702" s="2"/>
-      <c r="E702" s="2"/>
-      <c r="F702" s="2"/>
-      <c r="G702" s="2"/>
-      <c r="H702" s="2"/>
+      <c r="D702" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E702" s="5">
+        <v>0</v>
+      </c>
+      <c r="F702" s="5">
+        <v>0</v>
+      </c>
+      <c r="G702" s="5">
+        <v>0</v>
+      </c>
+      <c r="H702" s="5">
+        <v>0</v>
+      </c>
       <c r="I702" s="2"/>
-      <c r="J702" s="2"/>
-      <c r="K702" s="2"/>
-      <c r="L702" s="2"/>
-      <c r="M702" s="2"/>
-      <c r="N702" s="2"/>
-      <c r="O702" s="2"/>
-      <c r="P702" s="2"/>
-      <c r="Q702" s="2"/>
-      <c r="R702" s="2"/>
-      <c r="S702" s="2"/>
+      <c r="J702" s="5">
+        <v>0</v>
+      </c>
+      <c r="K702" s="5">
+        <v>0</v>
+      </c>
+      <c r="L702" s="5">
+        <v>0</v>
+      </c>
+      <c r="M702" s="5">
+        <v>0</v>
+      </c>
+      <c r="N702" s="6">
+        <v>-57372.9</v>
+      </c>
+      <c r="O702" s="5">
+        <v>0</v>
+      </c>
+      <c r="P702" s="6">
+        <v>57372.9</v>
+      </c>
+      <c r="Q702" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R702" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S702" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="T702" s="2"/>
-      <c r="U702" s="2"/>
-      <c r="V702" s="2"/>
-      <c r="W702" s="2"/>
-      <c r="X702" s="2"/>
-      <c r="Y702" s="2"/>
-      <c r="Z702" s="2"/>
-      <c r="AA702" s="2"/>
-      <c r="AB702" s="2"/>
-      <c r="AC702" s="2"/>
-      <c r="AD702" s="2"/>
-      <c r="AE702" s="2"/>
-      <c r="AF702" s="2"/>
+      <c r="U702" s="5">
+        <v>0</v>
+      </c>
+      <c r="V702" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W702" s="5">
+        <v>0</v>
+      </c>
+      <c r="X702" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y702" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z702" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA702" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB702" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC702" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD702" s="7">
+        <v>-70979771</v>
+      </c>
+      <c r="AE702" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF702" s="7">
+        <v>70979771</v>
+      </c>
     </row>
     <row r="703" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A703" s="2"/>
-      <c r="B703" s="2"/>
+      <c r="A703" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B703" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="C703" s="2"/>
-      <c r="D703" s="2"/>
-      <c r="E703" s="2"/>
-      <c r="F703" s="2"/>
-      <c r="G703" s="2"/>
-      <c r="H703" s="2"/>
+      <c r="D703" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E703" s="5">
+        <v>0</v>
+      </c>
+      <c r="F703" s="5">
+        <v>0</v>
+      </c>
+      <c r="G703" s="5">
+        <v>0</v>
+      </c>
+      <c r="H703" s="5">
+        <v>0</v>
+      </c>
       <c r="I703" s="2"/>
-      <c r="J703" s="2"/>
-      <c r="K703" s="2"/>
-      <c r="L703" s="2"/>
-      <c r="M703" s="2"/>
-      <c r="N703" s="2"/>
-      <c r="O703" s="2"/>
-      <c r="P703" s="2"/>
-      <c r="Q703" s="2"/>
-      <c r="R703" s="2"/>
-      <c r="S703" s="2"/>
+      <c r="J703" s="5">
+        <v>0</v>
+      </c>
+      <c r="K703" s="5">
+        <v>0</v>
+      </c>
+      <c r="L703" s="5">
+        <v>0</v>
+      </c>
+      <c r="M703" s="5">
+        <v>0</v>
+      </c>
+      <c r="N703" s="6">
+        <v>-136827</v>
+      </c>
+      <c r="O703" s="5">
+        <v>0</v>
+      </c>
+      <c r="P703" s="6">
+        <v>136827</v>
+      </c>
+      <c r="Q703" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R703" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S703" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="T703" s="2"/>
-      <c r="U703" s="2"/>
-      <c r="V703" s="2"/>
-      <c r="W703" s="2"/>
-      <c r="X703" s="2"/>
-      <c r="Y703" s="2"/>
-      <c r="Z703" s="2"/>
-      <c r="AA703" s="2"/>
-      <c r="AB703" s="2"/>
-      <c r="AC703" s="2"/>
-      <c r="AD703" s="2"/>
-      <c r="AE703" s="2"/>
-      <c r="AF703" s="2"/>
+      <c r="U703" s="5">
+        <v>0</v>
+      </c>
+      <c r="V703" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W703" s="5">
+        <v>0</v>
+      </c>
+      <c r="X703" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y703" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z703" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA703" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB703" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC703" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD703" s="7">
+        <v>-187208997</v>
+      </c>
+      <c r="AE703" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF703" s="7">
+        <v>187208997</v>
+      </c>
     </row>
     <row r="704" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A704" s="2"/>
-      <c r="B704" s="2"/>
+      <c r="A704" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B704" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="C704" s="2"/>
-      <c r="D704" s="2"/>
-      <c r="E704" s="2"/>
-      <c r="F704" s="2"/>
-      <c r="G704" s="2"/>
-      <c r="H704" s="2"/>
-      <c r="I704" s="2"/>
-      <c r="J704" s="2"/>
-      <c r="K704" s="2"/>
-      <c r="L704" s="2"/>
-      <c r="M704" s="2"/>
-      <c r="N704" s="2"/>
-      <c r="O704" s="2"/>
-      <c r="P704" s="2"/>
-      <c r="Q704" s="2"/>
-      <c r="R704" s="2"/>
-      <c r="S704" s="2"/>
+      <c r="D704" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E704" s="5">
+        <v>0</v>
+      </c>
+      <c r="F704" s="6">
+        <v>20000</v>
+      </c>
+      <c r="G704" s="5">
+        <v>34.24</v>
+      </c>
+      <c r="H704" s="6">
+        <v>684800</v>
+      </c>
+      <c r="I704" s="5">
+        <v>35.03</v>
+      </c>
+      <c r="J704" s="6">
+        <v>700600</v>
+      </c>
+      <c r="K704" s="6">
+        <v>15800</v>
+      </c>
+      <c r="L704" s="7">
+        <v>-413740</v>
+      </c>
+      <c r="M704" s="5">
+        <v>0</v>
+      </c>
+      <c r="N704" s="5">
+        <v>0</v>
+      </c>
+      <c r="O704" s="5">
+        <v>0</v>
+      </c>
+      <c r="P704" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q704" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R704" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S704" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="T704" s="2"/>
-      <c r="U704" s="2"/>
-      <c r="V704" s="2"/>
-      <c r="W704" s="2"/>
-      <c r="X704" s="2"/>
-      <c r="Y704" s="2"/>
-      <c r="Z704" s="2"/>
-      <c r="AA704" s="2"/>
-      <c r="AB704" s="2"/>
-      <c r="AC704" s="2"/>
-      <c r="AD704" s="2"/>
-      <c r="AE704" s="2"/>
-      <c r="AF704" s="2"/>
+      <c r="U704" s="5">
+        <v>0</v>
+      </c>
+      <c r="V704" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W704" s="6">
+        <v>1477</v>
+      </c>
+      <c r="X704" s="7">
+        <v>1011449600</v>
+      </c>
+      <c r="Y704" s="6">
+        <v>1443.1</v>
+      </c>
+      <c r="Z704" s="7">
+        <v>1011035860</v>
+      </c>
+      <c r="AA704" s="7">
+        <v>22800980</v>
+      </c>
+      <c r="AB704" s="7">
+        <v>-23214720</v>
+      </c>
+      <c r="AC704" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD704" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE704" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF704" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="705" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A705" s="2"/>
-      <c r="B705" s="2"/>
+      <c r="A705" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B705" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="C705" s="2"/>
-      <c r="D705" s="2"/>
-      <c r="E705" s="2"/>
-      <c r="F705" s="2"/>
-      <c r="G705" s="2"/>
-      <c r="H705" s="2"/>
-      <c r="I705" s="2"/>
-      <c r="J705" s="2"/>
-      <c r="K705" s="2"/>
-      <c r="L705" s="2"/>
-      <c r="M705" s="2"/>
-      <c r="N705" s="2"/>
-      <c r="O705" s="2"/>
-      <c r="P705" s="2"/>
-      <c r="Q705" s="2"/>
-      <c r="R705" s="2"/>
-      <c r="S705" s="2"/>
+      <c r="D705" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E705" s="5">
+        <v>0</v>
+      </c>
+      <c r="F705" s="6">
+        <v>2500</v>
+      </c>
+      <c r="G705" s="5">
+        <v>251.01</v>
+      </c>
+      <c r="H705" s="6">
+        <v>627525.9</v>
+      </c>
+      <c r="I705" s="5">
+        <v>260.58</v>
+      </c>
+      <c r="J705" s="6">
+        <v>651450</v>
+      </c>
+      <c r="K705" s="6">
+        <v>23924.1</v>
+      </c>
+      <c r="L705" s="7">
+        <v>20472377</v>
+      </c>
+      <c r="M705" s="5">
+        <v>0</v>
+      </c>
+      <c r="N705" s="6">
+        <v>26490.1</v>
+      </c>
+      <c r="O705" s="6">
+        <v>26490.1</v>
+      </c>
+      <c r="P705" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q705" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R705" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S705" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="T705" s="2"/>
-      <c r="U705" s="2"/>
-      <c r="V705" s="2"/>
-      <c r="W705" s="2"/>
-      <c r="X705" s="2"/>
-      <c r="Y705" s="2"/>
-      <c r="Z705" s="2"/>
-      <c r="AA705" s="2"/>
-      <c r="AB705" s="2"/>
-      <c r="AC705" s="2"/>
-      <c r="AD705" s="2"/>
-      <c r="AE705" s="2"/>
-      <c r="AF705" s="2"/>
+      <c r="U705" s="5">
+        <v>0</v>
+      </c>
+      <c r="V705" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W705" s="6">
+        <v>1465.49</v>
+      </c>
+      <c r="X705" s="7">
+        <v>919635118</v>
+      </c>
+      <c r="Y705" s="6">
+        <v>1443.1</v>
+      </c>
+      <c r="Z705" s="7">
+        <v>940107495</v>
+      </c>
+      <c r="AA705" s="7">
+        <v>34524868</v>
+      </c>
+      <c r="AB705" s="7">
+        <v>-14052492</v>
+      </c>
+      <c r="AC705" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD705" s="7">
+        <v>31565751</v>
+      </c>
+      <c r="AE705" s="7">
+        <v>31565751</v>
+      </c>
+      <c r="AF705" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="706" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A706" s="2"/>
-      <c r="B706" s="2"/>
+      <c r="A706" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B706" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="C706" s="2"/>
-      <c r="D706" s="2"/>
-      <c r="E706" s="2"/>
-      <c r="F706" s="2"/>
-      <c r="G706" s="2"/>
-      <c r="H706" s="2"/>
-      <c r="I706" s="2"/>
-      <c r="J706" s="2"/>
-      <c r="K706" s="2"/>
-      <c r="L706" s="2"/>
-      <c r="M706" s="2"/>
-      <c r="N706" s="2"/>
-      <c r="O706" s="2"/>
-      <c r="P706" s="2"/>
-      <c r="Q706" s="2"/>
-      <c r="R706" s="2"/>
-      <c r="S706" s="2"/>
+      <c r="D706" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E706" s="5">
+        <v>0</v>
+      </c>
+      <c r="F706" s="6">
+        <v>1550</v>
+      </c>
+      <c r="G706" s="5">
+        <v>192.399</v>
+      </c>
+      <c r="H706" s="6">
+        <v>298219.38</v>
+      </c>
+      <c r="I706" s="5">
+        <v>192.64</v>
+      </c>
+      <c r="J706" s="6">
+        <v>298592</v>
+      </c>
+      <c r="K706" s="5">
+        <v>372.62</v>
+      </c>
+      <c r="L706" s="7">
+        <v>-3816275</v>
+      </c>
+      <c r="M706" s="5">
+        <v>0</v>
+      </c>
+      <c r="N706" s="5">
+        <v>0</v>
+      </c>
+      <c r="O706" s="5">
+        <v>0</v>
+      </c>
+      <c r="P706" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q706" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R706" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S706" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="T706" s="2"/>
-      <c r="U706" s="2"/>
-      <c r="V706" s="2"/>
-      <c r="W706" s="2"/>
-      <c r="X706" s="2"/>
-      <c r="Y706" s="2"/>
-      <c r="Z706" s="2"/>
-      <c r="AA706" s="2"/>
-      <c r="AB706" s="2"/>
-      <c r="AC706" s="2"/>
-      <c r="AD706" s="2"/>
-      <c r="AE706" s="2"/>
-      <c r="AF706" s="2"/>
+      <c r="U706" s="5">
+        <v>0</v>
+      </c>
+      <c r="V706" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W706" s="6">
+        <v>1457.69</v>
+      </c>
+      <c r="X706" s="7">
+        <v>434714390</v>
+      </c>
+      <c r="Y706" s="6">
+        <v>1443.1</v>
+      </c>
+      <c r="Z706" s="7">
+        <v>430898115</v>
+      </c>
+      <c r="AA706" s="7">
+        <v>537727</v>
+      </c>
+      <c r="AB706" s="7">
+        <v>-4354003</v>
+      </c>
+      <c r="AC706" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD706" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE706" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF706" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="707" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A707" s="2"/>
-      <c r="B707" s="2"/>
+      <c r="A707" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B707" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="C707" s="2"/>
-      <c r="D707" s="2"/>
-      <c r="E707" s="2"/>
-      <c r="F707" s="2"/>
-      <c r="G707" s="2"/>
-      <c r="H707" s="2"/>
-      <c r="I707" s="2"/>
-      <c r="J707" s="2"/>
-      <c r="K707" s="2"/>
-      <c r="L707" s="2"/>
-      <c r="M707" s="2"/>
-      <c r="N707" s="2"/>
-      <c r="O707" s="2"/>
-      <c r="P707" s="2"/>
-      <c r="Q707" s="2"/>
-      <c r="R707" s="2"/>
-      <c r="S707" s="2"/>
+      <c r="D707" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E707" s="5">
+        <v>0</v>
+      </c>
+      <c r="F707" s="6">
+        <v>35000</v>
+      </c>
+      <c r="G707" s="5">
+        <v>8.0350000000000001</v>
+      </c>
+      <c r="H707" s="6">
+        <v>281256.5</v>
+      </c>
+      <c r="I707" s="5">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="J707" s="6">
+        <v>292950</v>
+      </c>
+      <c r="K707" s="6">
+        <v>11693.5</v>
+      </c>
+      <c r="L707" s="7">
+        <v>10912253</v>
+      </c>
+      <c r="M707" s="5">
+        <v>0</v>
+      </c>
+      <c r="N707" s="5">
+        <v>0</v>
+      </c>
+      <c r="O707" s="5">
+        <v>0</v>
+      </c>
+      <c r="P707" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q707" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R707" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S707" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="T707" s="2"/>
-      <c r="U707" s="2"/>
-      <c r="V707" s="2"/>
-      <c r="W707" s="2"/>
-      <c r="X707" s="2"/>
-      <c r="Y707" s="2"/>
-      <c r="Z707" s="2"/>
-      <c r="AA707" s="2"/>
-      <c r="AB707" s="2"/>
-      <c r="AC707" s="2"/>
-      <c r="AD707" s="2"/>
-      <c r="AE707" s="2"/>
-      <c r="AF707" s="2"/>
+      <c r="U707" s="5">
+        <v>0</v>
+      </c>
+      <c r="V707" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W707" s="6">
+        <v>1464.29</v>
+      </c>
+      <c r="X707" s="7">
+        <v>411843892</v>
+      </c>
+      <c r="Y707" s="6">
+        <v>1443.1</v>
+      </c>
+      <c r="Z707" s="7">
+        <v>422756145</v>
+      </c>
+      <c r="AA707" s="7">
+        <v>16874889</v>
+      </c>
+      <c r="AB707" s="7">
+        <v>-5962637</v>
+      </c>
+      <c r="AC707" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD707" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE707" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF707" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="708" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A708" s="2"/>
-      <c r="B708" s="2"/>
+      <c r="A708" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B708" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="C708" s="2"/>
-      <c r="D708" s="2"/>
-      <c r="E708" s="2"/>
-      <c r="F708" s="2"/>
-      <c r="G708" s="2"/>
-      <c r="H708" s="2"/>
+      <c r="D708" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E708" s="5">
+        <v>0</v>
+      </c>
+      <c r="F708" s="5">
+        <v>0</v>
+      </c>
+      <c r="G708" s="5">
+        <v>0</v>
+      </c>
+      <c r="H708" s="5">
+        <v>0</v>
+      </c>
       <c r="I708" s="2"/>
-      <c r="J708" s="2"/>
-      <c r="K708" s="2"/>
-      <c r="L708" s="2"/>
-      <c r="M708" s="2"/>
-      <c r="N708" s="2"/>
-      <c r="O708" s="2"/>
-      <c r="P708" s="2"/>
-      <c r="Q708" s="2"/>
-      <c r="R708" s="2"/>
-      <c r="S708" s="2"/>
+      <c r="J708" s="5">
+        <v>0</v>
+      </c>
+      <c r="K708" s="5">
+        <v>0</v>
+      </c>
+      <c r="L708" s="5">
+        <v>0</v>
+      </c>
+      <c r="M708" s="5">
+        <v>0</v>
+      </c>
+      <c r="N708" s="6">
+        <v>-276165.90000000002</v>
+      </c>
+      <c r="O708" s="5">
+        <v>0</v>
+      </c>
+      <c r="P708" s="6">
+        <v>276165.90000000002</v>
+      </c>
+      <c r="Q708" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R708" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S708" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="T708" s="2"/>
-      <c r="U708" s="2"/>
-      <c r="V708" s="2"/>
-      <c r="W708" s="2"/>
-      <c r="X708" s="2"/>
-      <c r="Y708" s="2"/>
-      <c r="Z708" s="2"/>
-      <c r="AA708" s="2"/>
-      <c r="AB708" s="2"/>
-      <c r="AC708" s="2"/>
-      <c r="AD708" s="2"/>
-      <c r="AE708" s="2"/>
-      <c r="AF708" s="2"/>
+      <c r="U708" s="5">
+        <v>0</v>
+      </c>
+      <c r="V708" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W708" s="5">
+        <v>0</v>
+      </c>
+      <c r="X708" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y708" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z708" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA708" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB708" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC708" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD708" s="7">
+        <v>-413294425</v>
+      </c>
+      <c r="AE708" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF708" s="7">
+        <v>413294425</v>
+      </c>
     </row>
     <row r="709" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A709" s="2"/>
-      <c r="B709" s="2"/>
+      <c r="A709" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B709" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="C709" s="2"/>
-      <c r="D709" s="2"/>
-      <c r="E709" s="2"/>
-      <c r="F709" s="2"/>
-      <c r="G709" s="2"/>
-      <c r="H709" s="2"/>
-      <c r="I709" s="2"/>
-      <c r="J709" s="2"/>
-      <c r="K709" s="2"/>
-      <c r="L709" s="2"/>
-      <c r="M709" s="2"/>
-      <c r="N709" s="2"/>
-      <c r="O709" s="2"/>
-      <c r="P709" s="2"/>
-      <c r="Q709" s="2"/>
-      <c r="R709" s="2"/>
-      <c r="S709" s="2"/>
+      <c r="D709" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E709" s="5">
+        <v>0</v>
+      </c>
+      <c r="F709" s="6">
+        <v>1500</v>
+      </c>
+      <c r="G709" s="5">
+        <v>191.75399999999999</v>
+      </c>
+      <c r="H709" s="6">
+        <v>287631.15000000002</v>
+      </c>
+      <c r="I709" s="5">
+        <v>187.9</v>
+      </c>
+      <c r="J709" s="6">
+        <v>281850</v>
+      </c>
+      <c r="K709" s="6">
+        <v>-5781.15</v>
+      </c>
+      <c r="L709" s="7">
+        <v>-3711916</v>
+      </c>
+      <c r="M709" s="5">
+        <v>0</v>
+      </c>
+      <c r="N709" s="6">
+        <v>-17520.8</v>
+      </c>
+      <c r="O709" s="5">
+        <v>0</v>
+      </c>
+      <c r="P709" s="6">
+        <v>17520.8</v>
+      </c>
+      <c r="Q709" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R709" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S709" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="T709" s="2"/>
-      <c r="U709" s="2"/>
-      <c r="V709" s="2"/>
-      <c r="W709" s="2"/>
-      <c r="X709" s="2"/>
-      <c r="Y709" s="2"/>
-      <c r="Z709" s="2"/>
-      <c r="AA709" s="2"/>
-      <c r="AB709" s="2"/>
-      <c r="AC709" s="2"/>
-      <c r="AD709" s="2"/>
-      <c r="AE709" s="2"/>
-      <c r="AF709" s="2"/>
+      <c r="U709" s="5">
+        <v>0</v>
+      </c>
+      <c r="V709" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W709" s="6">
+        <v>1426.99</v>
+      </c>
+      <c r="X709" s="7">
+        <v>410449651</v>
+      </c>
+      <c r="Y709" s="6">
+        <v>1443.1</v>
+      </c>
+      <c r="Z709" s="7">
+        <v>406737735</v>
+      </c>
+      <c r="AA709" s="7">
+        <v>-8342777</v>
+      </c>
+      <c r="AB709" s="7">
+        <v>4630861</v>
+      </c>
+      <c r="AC709" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD709" s="7">
+        <v>-4466002</v>
+      </c>
+      <c r="AE709" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF709" s="7">
+        <v>4466002</v>
+      </c>
     </row>
     <row r="710" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A710" s="2"/>
-      <c r="B710" s="2"/>
+      <c r="A710" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B710" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="C710" s="2"/>
-      <c r="D710" s="2"/>
-      <c r="E710" s="2"/>
-      <c r="F710" s="2"/>
-      <c r="G710" s="2"/>
-      <c r="H710" s="2"/>
-      <c r="I710" s="2"/>
-      <c r="J710" s="2"/>
-      <c r="K710" s="2"/>
-      <c r="L710" s="2"/>
-      <c r="M710" s="2"/>
-      <c r="N710" s="2"/>
-      <c r="O710" s="2"/>
-      <c r="P710" s="2"/>
-      <c r="Q710" s="2"/>
-      <c r="R710" s="2"/>
-      <c r="S710" s="2"/>
+      <c r="D710" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E710" s="5">
+        <v>0</v>
+      </c>
+      <c r="F710" s="6">
+        <v>20000</v>
+      </c>
+      <c r="G710" s="5">
+        <v>45.33</v>
+      </c>
+      <c r="H710" s="6">
+        <v>906615</v>
+      </c>
+      <c r="I710" s="5">
+        <v>51.53</v>
+      </c>
+      <c r="J710" s="6">
+        <v>1030600</v>
+      </c>
+      <c r="K710" s="6">
+        <v>123985</v>
+      </c>
+      <c r="L710" s="7">
+        <v>155101849</v>
+      </c>
+      <c r="M710" s="5">
+        <v>0</v>
+      </c>
+      <c r="N710" s="5">
+        <v>0</v>
+      </c>
+      <c r="O710" s="5">
+        <v>0</v>
+      </c>
+      <c r="P710" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q710" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R710" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S710" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="T710" s="2"/>
-      <c r="U710" s="2"/>
-      <c r="V710" s="2"/>
-      <c r="W710" s="2"/>
-      <c r="X710" s="2"/>
-      <c r="Y710" s="2"/>
-      <c r="Z710" s="2"/>
-      <c r="AA710" s="2"/>
-      <c r="AB710" s="2"/>
-      <c r="AC710" s="2"/>
-      <c r="AD710" s="2"/>
-      <c r="AE710" s="2"/>
-      <c r="AF710" s="2"/>
+      <c r="U710" s="5">
+        <v>0</v>
+      </c>
+      <c r="V710" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W710" s="6">
+        <v>1469.37</v>
+      </c>
+      <c r="X710" s="7">
+        <v>1332157011</v>
+      </c>
+      <c r="Y710" s="6">
+        <v>1443.1</v>
+      </c>
+      <c r="Z710" s="7">
+        <v>1487258860</v>
+      </c>
+      <c r="AA710" s="7">
+        <v>178922753</v>
+      </c>
+      <c r="AB710" s="7">
+        <v>-23820905</v>
+      </c>
+      <c r="AC710" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD710" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE710" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF710" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="711" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A711" s="2"/>
-      <c r="B711" s="2"/>
+      <c r="A711" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B711" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="C711" s="2"/>
-      <c r="D711" s="2"/>
-      <c r="E711" s="2"/>
-      <c r="F711" s="2"/>
-      <c r="G711" s="2"/>
-      <c r="H711" s="2"/>
+      <c r="D711" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E711" s="5">
+        <v>0</v>
+      </c>
+      <c r="F711" s="5">
+        <v>0</v>
+      </c>
+      <c r="G711" s="5">
+        <v>0</v>
+      </c>
+      <c r="H711" s="5">
+        <v>0</v>
+      </c>
       <c r="I711" s="2"/>
-      <c r="J711" s="2"/>
-      <c r="K711" s="2"/>
-      <c r="L711" s="2"/>
-      <c r="M711" s="2"/>
-      <c r="N711" s="2"/>
-      <c r="O711" s="2"/>
-      <c r="P711" s="2"/>
-      <c r="Q711" s="2"/>
-      <c r="R711" s="2"/>
-      <c r="S711" s="2"/>
+      <c r="J711" s="5">
+        <v>0</v>
+      </c>
+      <c r="K711" s="5">
+        <v>0</v>
+      </c>
+      <c r="L711" s="5">
+        <v>0</v>
+      </c>
+      <c r="M711" s="5">
+        <v>0</v>
+      </c>
+      <c r="N711" s="6">
+        <v>20374.7</v>
+      </c>
+      <c r="O711" s="6">
+        <v>20374.7</v>
+      </c>
+      <c r="P711" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q711" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R711" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S711" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="T711" s="2"/>
-      <c r="U711" s="2"/>
-      <c r="V711" s="2"/>
-      <c r="W711" s="2"/>
-      <c r="X711" s="2"/>
-      <c r="Y711" s="2"/>
-      <c r="Z711" s="2"/>
-      <c r="AA711" s="2"/>
-      <c r="AB711" s="2"/>
-      <c r="AC711" s="2"/>
-      <c r="AD711" s="2"/>
-      <c r="AE711" s="2"/>
-      <c r="AF711" s="2"/>
+      <c r="U711" s="5">
+        <v>0</v>
+      </c>
+      <c r="V711" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W711" s="5">
+        <v>0</v>
+      </c>
+      <c r="X711" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y711" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z711" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA711" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB711" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC711" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD711" s="7">
+        <v>149323927</v>
+      </c>
+      <c r="AE711" s="7">
+        <v>149323927</v>
+      </c>
+      <c r="AF711" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="712" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A712" s="2"/>
-      <c r="B712" s="2"/>
+      <c r="A712" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B712" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="C712" s="2"/>
-      <c r="D712" s="2"/>
-      <c r="E712" s="2"/>
-      <c r="F712" s="2"/>
-      <c r="G712" s="2"/>
-      <c r="H712" s="2"/>
-      <c r="I712" s="2"/>
-      <c r="J712" s="2"/>
-      <c r="K712" s="2"/>
-      <c r="L712" s="2"/>
-      <c r="M712" s="2"/>
-      <c r="N712" s="2"/>
-      <c r="O712" s="2"/>
-      <c r="P712" s="2"/>
-      <c r="Q712" s="2"/>
-      <c r="R712" s="2"/>
-      <c r="S712" s="2"/>
+      <c r="D712" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E712" s="5">
+        <v>0</v>
+      </c>
+      <c r="F712" s="5">
+        <v>700</v>
+      </c>
+      <c r="G712" s="5">
+        <v>396.31</v>
+      </c>
+      <c r="H712" s="6">
+        <v>277417</v>
+      </c>
+      <c r="I712" s="5">
+        <v>459.56</v>
+      </c>
+      <c r="J712" s="6">
+        <v>321692</v>
+      </c>
+      <c r="K712" s="6">
+        <v>44275</v>
+      </c>
+      <c r="L712" s="7">
+        <v>66168072</v>
+      </c>
+      <c r="M712" s="5">
+        <v>0</v>
+      </c>
+      <c r="N712" s="6">
+        <v>208082</v>
+      </c>
+      <c r="O712" s="6">
+        <v>208082</v>
+      </c>
+      <c r="P712" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q712" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R712" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S712" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="T712" s="2"/>
-      <c r="U712" s="2"/>
-      <c r="V712" s="2"/>
-      <c r="W712" s="2"/>
-      <c r="X712" s="2"/>
-      <c r="Y712" s="2"/>
-      <c r="Z712" s="2"/>
-      <c r="AA712" s="2"/>
-      <c r="AB712" s="2"/>
-      <c r="AC712" s="2"/>
-      <c r="AD712" s="2"/>
-      <c r="AE712" s="2"/>
-      <c r="AF712" s="2"/>
+      <c r="U712" s="5">
+        <v>0</v>
+      </c>
+      <c r="V712" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W712" s="6">
+        <v>1434.89</v>
+      </c>
+      <c r="X712" s="7">
+        <v>398065653</v>
+      </c>
+      <c r="Y712" s="6">
+        <v>1443.1</v>
+      </c>
+      <c r="Z712" s="7">
+        <v>464233725</v>
+      </c>
+      <c r="AA712" s="7">
+        <v>63893252</v>
+      </c>
+      <c r="AB712" s="7">
+        <v>2274819</v>
+      </c>
+      <c r="AC712" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD712" s="7">
+        <v>337072659</v>
+      </c>
+      <c r="AE712" s="7">
+        <v>337072659</v>
+      </c>
+      <c r="AF712" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="713" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A713" s="2"/>
-      <c r="B713" s="2"/>
+      <c r="A713" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B713" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="C713" s="2"/>
-      <c r="D713" s="2"/>
-      <c r="E713" s="2"/>
-      <c r="F713" s="2"/>
-      <c r="G713" s="2"/>
-      <c r="H713" s="2"/>
-      <c r="I713" s="2"/>
-      <c r="J713" s="2"/>
-      <c r="K713" s="2"/>
-      <c r="L713" s="2"/>
-      <c r="M713" s="2"/>
-      <c r="N713" s="2"/>
-      <c r="O713" s="2"/>
-      <c r="P713" s="2"/>
-      <c r="Q713" s="2"/>
-      <c r="R713" s="2"/>
-      <c r="S713" s="2"/>
+      <c r="D713" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E713" s="5">
+        <v>0</v>
+      </c>
+      <c r="F713" s="6">
+        <v>5000</v>
+      </c>
+      <c r="G713" s="5">
+        <v>87.436000000000007</v>
+      </c>
+      <c r="H713" s="6">
+        <v>437184.5</v>
+      </c>
+      <c r="I713" s="5">
+        <v>87.67</v>
+      </c>
+      <c r="J713" s="6">
+        <v>438350</v>
+      </c>
+      <c r="K713" s="6">
+        <v>1165.5</v>
+      </c>
+      <c r="L713" s="7">
+        <v>-10209485</v>
+      </c>
+      <c r="M713" s="5">
+        <v>0</v>
+      </c>
+      <c r="N713" s="5">
+        <v>0</v>
+      </c>
+      <c r="O713" s="5">
+        <v>0</v>
+      </c>
+      <c r="P713" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q713" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R713" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S713" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="T713" s="2"/>
-      <c r="U713" s="2"/>
-      <c r="V713" s="2"/>
-      <c r="W713" s="2"/>
-      <c r="X713" s="2"/>
-      <c r="Y713" s="2"/>
-      <c r="Z713" s="2"/>
-      <c r="AA713" s="2"/>
-      <c r="AB713" s="2"/>
-      <c r="AC713" s="2"/>
-      <c r="AD713" s="2"/>
-      <c r="AE713" s="2"/>
-      <c r="AF713" s="2"/>
+      <c r="U713" s="5">
+        <v>0</v>
+      </c>
+      <c r="V713" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W713" s="6">
+        <v>1470.29</v>
+      </c>
+      <c r="X713" s="7">
+        <v>642792370</v>
+      </c>
+      <c r="Y713" s="6">
+        <v>1443.1</v>
+      </c>
+      <c r="Z713" s="7">
+        <v>632582885</v>
+      </c>
+      <c r="AA713" s="7">
+        <v>1681933</v>
+      </c>
+      <c r="AB713" s="7">
+        <v>-11891419</v>
+      </c>
+      <c r="AC713" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD713" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE713" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF713" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="714" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A714" s="2"/>
-      <c r="B714" s="2"/>
+      <c r="A714" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B714" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="C714" s="2"/>
-      <c r="D714" s="2"/>
-      <c r="E714" s="2"/>
-      <c r="F714" s="2"/>
-      <c r="G714" s="2"/>
-      <c r="H714" s="2"/>
+      <c r="D714" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E714" s="5">
+        <v>0</v>
+      </c>
+      <c r="F714" s="5">
+        <v>0</v>
+      </c>
+      <c r="G714" s="5">
+        <v>0</v>
+      </c>
+      <c r="H714" s="5">
+        <v>0</v>
+      </c>
       <c r="I714" s="2"/>
-      <c r="J714" s="2"/>
-      <c r="K714" s="2"/>
-      <c r="L714" s="2"/>
-      <c r="M714" s="2"/>
-      <c r="N714" s="2"/>
-      <c r="O714" s="2"/>
-      <c r="P714" s="2"/>
-      <c r="Q714" s="2"/>
-      <c r="R714" s="2"/>
-      <c r="S714" s="2"/>
+      <c r="J714" s="5">
+        <v>0</v>
+      </c>
+      <c r="K714" s="5">
+        <v>0</v>
+      </c>
+      <c r="L714" s="5">
+        <v>0</v>
+      </c>
+      <c r="M714" s="5">
+        <v>0</v>
+      </c>
+      <c r="N714" s="6">
+        <v>-59856</v>
+      </c>
+      <c r="O714" s="5">
+        <v>0</v>
+      </c>
+      <c r="P714" s="6">
+        <v>59856</v>
+      </c>
+      <c r="Q714" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R714" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S714" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="T714" s="2"/>
-      <c r="U714" s="2"/>
-      <c r="V714" s="2"/>
-      <c r="W714" s="2"/>
-      <c r="X714" s="2"/>
-      <c r="Y714" s="2"/>
-      <c r="Z714" s="2"/>
-      <c r="AA714" s="2"/>
-      <c r="AB714" s="2"/>
-      <c r="AC714" s="2"/>
-      <c r="AD714" s="2"/>
-      <c r="AE714" s="2"/>
-      <c r="AF714" s="2"/>
+      <c r="U714" s="5">
+        <v>0</v>
+      </c>
+      <c r="V714" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W714" s="5">
+        <v>0</v>
+      </c>
+      <c r="X714" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y714" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z714" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA714" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB714" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC714" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD714" s="7">
+        <v>-91164813</v>
+      </c>
+      <c r="AE714" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF714" s="7">
+        <v>91164813</v>
+      </c>
     </row>
     <row r="715" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A715" s="2"/>
-      <c r="B715" s="2"/>
+      <c r="A715" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B715" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="C715" s="2"/>
-      <c r="D715" s="2"/>
-      <c r="E715" s="2"/>
-      <c r="F715" s="2"/>
-      <c r="G715" s="2"/>
-      <c r="H715" s="2"/>
-      <c r="I715" s="2"/>
-      <c r="J715" s="2"/>
-      <c r="K715" s="2"/>
-      <c r="L715" s="2"/>
-      <c r="M715" s="2"/>
-      <c r="N715" s="2"/>
-      <c r="O715" s="2"/>
-      <c r="P715" s="2"/>
-      <c r="Q715" s="2"/>
-      <c r="R715" s="2"/>
-      <c r="S715" s="2"/>
+      <c r="D715" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E715" s="5">
+        <v>0</v>
+      </c>
+      <c r="F715" s="5">
+        <v>400</v>
+      </c>
+      <c r="G715" s="5">
+        <v>432.53800000000001</v>
+      </c>
+      <c r="H715" s="6">
+        <v>173015.44</v>
+      </c>
+      <c r="I715" s="5">
+        <v>411.71</v>
+      </c>
+      <c r="J715" s="6">
+        <v>164684</v>
+      </c>
+      <c r="K715" s="6">
+        <v>-8331.44</v>
+      </c>
+      <c r="L715" s="7">
+        <v>-12663259</v>
+      </c>
+      <c r="M715" s="5">
+        <v>0</v>
+      </c>
+      <c r="N715" s="6">
+        <v>-16338.7</v>
+      </c>
+      <c r="O715" s="5">
+        <v>0</v>
+      </c>
+      <c r="P715" s="6">
+        <v>16338.7</v>
+      </c>
+      <c r="Q715" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R715" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S715" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="T715" s="2"/>
-      <c r="U715" s="2"/>
-      <c r="V715" s="2"/>
-      <c r="W715" s="2"/>
-      <c r="X715" s="2"/>
-      <c r="Y715" s="2"/>
-      <c r="Z715" s="2"/>
-      <c r="AA715" s="2"/>
-      <c r="AB715" s="2"/>
-      <c r="AC715" s="2"/>
-      <c r="AD715" s="2"/>
-      <c r="AE715" s="2"/>
-      <c r="AF715" s="2"/>
+      <c r="U715" s="5">
+        <v>0</v>
+      </c>
+      <c r="V715" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W715" s="6">
+        <v>1446.8</v>
+      </c>
+      <c r="X715" s="7">
+        <v>250318739</v>
+      </c>
+      <c r="Y715" s="6">
+        <v>1443.1</v>
+      </c>
+      <c r="Z715" s="7">
+        <v>237655480</v>
+      </c>
+      <c r="AA715" s="7">
+        <v>-12023101</v>
+      </c>
+      <c r="AB715" s="7">
+        <v>-640158</v>
+      </c>
+      <c r="AC715" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD715" s="7">
+        <v>-20475712</v>
+      </c>
+      <c r="AE715" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF715" s="7">
+        <v>20475712</v>
+      </c>
     </row>
     <row r="716" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A716" s="2"/>
-      <c r="B716" s="2"/>
+      <c r="A716" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B716" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="C716" s="2"/>
-      <c r="D716" s="2"/>
-      <c r="E716" s="2"/>
-      <c r="F716" s="2"/>
-      <c r="G716" s="2"/>
-      <c r="H716" s="2"/>
-      <c r="I716" s="2"/>
-      <c r="J716" s="2"/>
-      <c r="K716" s="2"/>
-      <c r="L716" s="2"/>
-      <c r="M716" s="2"/>
-      <c r="N716" s="2"/>
-      <c r="O716" s="2"/>
-      <c r="P716" s="2"/>
-      <c r="Q716" s="2"/>
-      <c r="R716" s="2"/>
-      <c r="S716" s="2"/>
+      <c r="D716" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E716" s="5">
+        <v>0</v>
+      </c>
+      <c r="F716" s="6">
+        <v>1000</v>
+      </c>
+      <c r="G716" s="5">
+        <v>169.042</v>
+      </c>
+      <c r="H716" s="6">
+        <v>169042.8</v>
+      </c>
+      <c r="I716" s="5">
+        <v>172.5</v>
+      </c>
+      <c r="J716" s="6">
+        <v>172500</v>
+      </c>
+      <c r="K716" s="6">
+        <v>3457.2</v>
+      </c>
+      <c r="L716" s="7">
+        <v>4363627</v>
+      </c>
+      <c r="M716" s="5">
+        <v>0</v>
+      </c>
+      <c r="N716" s="6">
+        <v>-14080</v>
+      </c>
+      <c r="O716" s="5">
+        <v>0</v>
+      </c>
+      <c r="P716" s="6">
+        <v>14080</v>
+      </c>
+      <c r="Q716" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R716" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S716" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="T716" s="2"/>
-      <c r="U716" s="2"/>
-      <c r="V716" s="2"/>
-      <c r="W716" s="2"/>
-      <c r="X716" s="2"/>
-      <c r="Y716" s="2"/>
-      <c r="Z716" s="2"/>
-      <c r="AA716" s="2"/>
-      <c r="AB716" s="2"/>
-      <c r="AC716" s="2"/>
-      <c r="AD716" s="2"/>
-      <c r="AE716" s="2"/>
-      <c r="AF716" s="2"/>
-    </row>
-    <row r="717" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A717" s="2"/>
-      <c r="B717" s="2"/>
+      <c r="U716" s="5">
+        <v>0</v>
+      </c>
+      <c r="V716" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W716" s="6">
+        <v>1446.79</v>
+      </c>
+      <c r="X716" s="7">
+        <v>244571123</v>
+      </c>
+      <c r="Y716" s="6">
+        <v>1443.1</v>
+      </c>
+      <c r="Z716" s="7">
+        <v>248934750</v>
+      </c>
+      <c r="AA716" s="7">
+        <v>4989085</v>
+      </c>
+      <c r="AB716" s="7">
+        <v>-625459</v>
+      </c>
+      <c r="AC716" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD716" s="7">
+        <v>-17266139</v>
+      </c>
+      <c r="AE716" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF716" s="7">
+        <v>17266139</v>
+      </c>
+    </row>
+    <row r="717" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A717" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B717" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="C717" s="2"/>
-      <c r="D717" s="2"/>
-      <c r="E717" s="2"/>
-      <c r="F717" s="2"/>
-      <c r="G717" s="2"/>
-      <c r="H717" s="2"/>
+      <c r="D717" s="5">
+        <v>6869</v>
+      </c>
+      <c r="E717" s="5">
+        <v>0</v>
+      </c>
+      <c r="F717" s="5">
+        <v>0</v>
+      </c>
+      <c r="G717" s="5">
+        <v>0</v>
+      </c>
+      <c r="H717" s="5">
+        <v>0</v>
+      </c>
       <c r="I717" s="2"/>
-      <c r="J717" s="2"/>
-      <c r="K717" s="2"/>
-      <c r="L717" s="2"/>
-      <c r="M717" s="2"/>
-      <c r="N717" s="2"/>
-      <c r="O717" s="2"/>
-      <c r="P717" s="2"/>
-      <c r="Q717" s="2"/>
-      <c r="R717" s="2"/>
-      <c r="S717" s="2"/>
+      <c r="J717" s="5">
+        <v>0</v>
+      </c>
+      <c r="K717" s="5">
+        <v>0</v>
+      </c>
+      <c r="L717" s="5">
+        <v>0</v>
+      </c>
+      <c r="M717" s="5">
+        <v>0</v>
+      </c>
+      <c r="N717" s="6">
+        <v>349976</v>
+      </c>
+      <c r="O717" s="6">
+        <v>349976</v>
+      </c>
+      <c r="P717" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q717" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R717" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S717" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="T717" s="2"/>
-      <c r="U717" s="2"/>
-      <c r="V717" s="2"/>
-      <c r="W717" s="2"/>
-      <c r="X717" s="2"/>
-      <c r="Y717" s="2"/>
-      <c r="Z717" s="2"/>
-      <c r="AA717" s="2"/>
-      <c r="AB717" s="2"/>
-      <c r="AC717" s="2"/>
-      <c r="AD717" s="2"/>
-      <c r="AE717" s="2"/>
-      <c r="AF717" s="2"/>
-    </row>
-    <row r="718" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A718" s="2"/>
-      <c r="B718" s="2"/>
+      <c r="U717" s="5">
+        <v>0</v>
+      </c>
+      <c r="V717" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W717" s="5">
+        <v>0</v>
+      </c>
+      <c r="X717" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y717" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z717" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA717" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB717" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC717" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD717" s="7">
+        <v>72042766</v>
+      </c>
+      <c r="AE717" s="7">
+        <v>72042766</v>
+      </c>
+      <c r="AF717" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="718" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A718" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B718" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="C718" s="2"/>
-      <c r="D718" s="2"/>
-      <c r="E718" s="2"/>
-      <c r="F718" s="2"/>
-      <c r="G718" s="2"/>
-      <c r="H718" s="2"/>
+      <c r="D718" s="5">
+        <v>2359</v>
+      </c>
+      <c r="E718" s="5">
+        <v>0</v>
+      </c>
+      <c r="F718" s="5">
+        <v>0</v>
+      </c>
+      <c r="G718" s="5">
+        <v>0</v>
+      </c>
+      <c r="H718" s="5">
+        <v>0</v>
+      </c>
       <c r="I718" s="2"/>
-      <c r="J718" s="2"/>
-      <c r="K718" s="2"/>
-      <c r="L718" s="2"/>
-      <c r="M718" s="2"/>
-      <c r="N718" s="2"/>
-      <c r="O718" s="2"/>
-      <c r="P718" s="2"/>
-      <c r="Q718" s="2"/>
-      <c r="R718" s="2"/>
-      <c r="S718" s="2"/>
+      <c r="J718" s="5">
+        <v>0</v>
+      </c>
+      <c r="K718" s="5">
+        <v>0</v>
+      </c>
+      <c r="L718" s="5">
+        <v>0</v>
+      </c>
+      <c r="M718" s="5">
+        <v>0</v>
+      </c>
+      <c r="N718" s="6">
+        <v>127080</v>
+      </c>
+      <c r="O718" s="6">
+        <v>127080</v>
+      </c>
+      <c r="P718" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q718" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R718" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S718" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="T718" s="2"/>
-      <c r="U718" s="2"/>
-      <c r="V718" s="2"/>
-      <c r="W718" s="2"/>
-      <c r="X718" s="2"/>
-      <c r="Y718" s="2"/>
-      <c r="Z718" s="2"/>
-      <c r="AA718" s="2"/>
-      <c r="AB718" s="2"/>
-      <c r="AC718" s="2"/>
-      <c r="AD718" s="2"/>
-      <c r="AE718" s="2"/>
-      <c r="AF718" s="2"/>
-    </row>
-    <row r="719" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A719" s="2"/>
-      <c r="B719" s="2"/>
+      <c r="U718" s="5">
+        <v>0</v>
+      </c>
+      <c r="V718" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W718" s="5">
+        <v>0</v>
+      </c>
+      <c r="X718" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y718" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z718" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA718" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB718" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC718" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD718" s="7">
+        <v>16254451</v>
+      </c>
+      <c r="AE718" s="7">
+        <v>16254451</v>
+      </c>
+      <c r="AF718" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="719" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A719" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B719" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="C719" s="2"/>
-      <c r="D719" s="2"/>
-      <c r="E719" s="2"/>
-      <c r="F719" s="2"/>
-      <c r="G719" s="2"/>
-      <c r="H719" s="2"/>
-      <c r="I719" s="2"/>
-      <c r="J719" s="2"/>
-      <c r="K719" s="2"/>
-      <c r="L719" s="2"/>
-      <c r="M719" s="2"/>
-      <c r="N719" s="2"/>
-      <c r="O719" s="2"/>
-      <c r="P719" s="2"/>
-      <c r="Q719" s="2"/>
-      <c r="R719" s="2"/>
-      <c r="S719" s="2"/>
+      <c r="D719" s="5">
+        <v>6680</v>
+      </c>
+      <c r="E719" s="5">
+        <v>0</v>
+      </c>
+      <c r="F719" s="6">
+        <v>130000</v>
+      </c>
+      <c r="G719" s="5">
+        <v>22.469000000000001</v>
+      </c>
+      <c r="H719" s="6">
+        <v>2921022</v>
+      </c>
+      <c r="I719" s="5">
+        <v>22.18</v>
+      </c>
+      <c r="J719" s="6">
+        <v>2883400</v>
+      </c>
+      <c r="K719" s="6">
+        <v>-37622</v>
+      </c>
+      <c r="L719" s="7">
+        <v>-19245533</v>
+      </c>
+      <c r="M719" s="5">
+        <v>0</v>
+      </c>
+      <c r="N719" s="5">
+        <v>0</v>
+      </c>
+      <c r="O719" s="5">
+        <v>0</v>
+      </c>
+      <c r="P719" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q719" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R719" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S719" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="T719" s="2"/>
-      <c r="U719" s="2"/>
-      <c r="V719" s="2"/>
-      <c r="W719" s="2"/>
-      <c r="X719" s="2"/>
-      <c r="Y719" s="2"/>
-      <c r="Z719" s="2"/>
-      <c r="AA719" s="2"/>
-      <c r="AB719" s="2"/>
-      <c r="AC719" s="2"/>
-      <c r="AD719" s="2"/>
-      <c r="AE719" s="2"/>
-      <c r="AF719" s="2"/>
-    </row>
-    <row r="720" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A720" s="2"/>
-      <c r="B720" s="2"/>
+      <c r="U719" s="5">
+        <v>0</v>
+      </c>
+      <c r="V719" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W719" s="5">
+        <v>188.88</v>
+      </c>
+      <c r="X719" s="7">
+        <v>551751845</v>
+      </c>
+      <c r="Y719" s="5">
+        <v>184.68</v>
+      </c>
+      <c r="Z719" s="7">
+        <v>532506312</v>
+      </c>
+      <c r="AA719" s="7">
+        <v>-6948030</v>
+      </c>
+      <c r="AB719" s="7">
+        <v>-12297503</v>
+      </c>
+      <c r="AC719" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD719" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE719" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF719" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="720" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A720" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B720" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="C720" s="2"/>
-      <c r="D720" s="2"/>
-      <c r="E720" s="2"/>
-      <c r="F720" s="2"/>
-      <c r="G720" s="2"/>
-      <c r="H720" s="2"/>
+      <c r="D720" s="5">
+        <v>6181</v>
+      </c>
+      <c r="E720" s="5">
+        <v>0</v>
+      </c>
+      <c r="F720" s="5">
+        <v>0</v>
+      </c>
+      <c r="G720" s="5">
+        <v>0</v>
+      </c>
+      <c r="H720" s="5">
+        <v>0</v>
+      </c>
       <c r="I720" s="2"/>
-      <c r="J720" s="2"/>
-      <c r="K720" s="2"/>
-      <c r="L720" s="2"/>
-      <c r="M720" s="2"/>
-      <c r="N720" s="2"/>
-      <c r="O720" s="2"/>
-      <c r="P720" s="2"/>
-      <c r="Q720" s="2"/>
-      <c r="R720" s="2"/>
-      <c r="S720" s="2"/>
+      <c r="J720" s="5">
+        <v>0</v>
+      </c>
+      <c r="K720" s="5">
+        <v>0</v>
+      </c>
+      <c r="L720" s="5">
+        <v>0</v>
+      </c>
+      <c r="M720" s="5">
+        <v>0</v>
+      </c>
+      <c r="N720" s="6">
+        <v>-6374.88</v>
+      </c>
+      <c r="O720" s="5">
+        <v>0</v>
+      </c>
+      <c r="P720" s="6">
+        <v>6374.88</v>
+      </c>
+      <c r="Q720" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R720" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S720" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="T720" s="2"/>
-      <c r="U720" s="2"/>
-      <c r="V720" s="2"/>
-      <c r="W720" s="2"/>
-      <c r="X720" s="2"/>
-      <c r="Y720" s="2"/>
-      <c r="Z720" s="2"/>
-      <c r="AA720" s="2"/>
-      <c r="AB720" s="2"/>
-      <c r="AC720" s="2"/>
-      <c r="AD720" s="2"/>
-      <c r="AE720" s="2"/>
-      <c r="AF720" s="2"/>
-    </row>
-    <row r="721" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A721" s="2"/>
-      <c r="B721" s="2"/>
+      <c r="U720" s="5">
+        <v>0</v>
+      </c>
+      <c r="V720" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W720" s="5">
+        <v>0</v>
+      </c>
+      <c r="X720" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y720" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z720" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA720" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB720" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC720" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD720" s="7">
+        <v>1362525</v>
+      </c>
+      <c r="AE720" s="7">
+        <v>1362525</v>
+      </c>
+      <c r="AF720" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="721" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A721" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B721" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="C721" s="2"/>
-      <c r="D721" s="2"/>
-      <c r="E721" s="2"/>
-      <c r="F721" s="2"/>
-      <c r="G721" s="2"/>
-      <c r="H721" s="2"/>
-      <c r="I721" s="2"/>
-      <c r="J721" s="2"/>
-      <c r="K721" s="2"/>
-      <c r="L721" s="2"/>
-      <c r="M721" s="2"/>
-      <c r="N721" s="2"/>
-      <c r="O721" s="2"/>
-      <c r="P721" s="2"/>
-      <c r="Q721" s="2"/>
-      <c r="R721" s="2"/>
-      <c r="S721" s="2"/>
+      <c r="D721" s="5">
+        <v>3750</v>
+      </c>
+      <c r="E721" s="5">
+        <v>0</v>
+      </c>
+      <c r="F721" s="6">
+        <v>6000</v>
+      </c>
+      <c r="G721" s="5">
+        <v>511.88299999999998</v>
+      </c>
+      <c r="H721" s="6">
+        <v>3071299.8</v>
+      </c>
+      <c r="I721" s="5">
+        <v>531.5</v>
+      </c>
+      <c r="J721" s="6">
+        <v>3189000</v>
+      </c>
+      <c r="K721" s="6">
+        <v>117700.2</v>
+      </c>
+      <c r="L721" s="7">
+        <v>13505790</v>
+      </c>
+      <c r="M721" s="5">
+        <v>0</v>
+      </c>
+      <c r="N721" s="5">
+        <v>0</v>
+      </c>
+      <c r="O721" s="5">
+        <v>0</v>
+      </c>
+      <c r="P721" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q721" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R721" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S721" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="T721" s="2"/>
-      <c r="U721" s="2"/>
-      <c r="V721" s="2"/>
-      <c r="W721" s="2"/>
-      <c r="X721" s="2"/>
-      <c r="Y721" s="2"/>
-      <c r="Z721" s="2"/>
-      <c r="AA721" s="2"/>
-      <c r="AB721" s="2"/>
-      <c r="AC721" s="2"/>
-      <c r="AD721" s="2"/>
-      <c r="AE721" s="2"/>
-      <c r="AF721" s="2"/>
-    </row>
-    <row r="722" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A722" s="2"/>
-      <c r="B722" s="2"/>
+      <c r="U721" s="5">
+        <v>0</v>
+      </c>
+      <c r="V721" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W721" s="5">
+        <v>187.35</v>
+      </c>
+      <c r="X721" s="7">
+        <v>575438730</v>
+      </c>
+      <c r="Y721" s="5">
+        <v>184.68</v>
+      </c>
+      <c r="Z721" s="7">
+        <v>588944520</v>
+      </c>
+      <c r="AA721" s="7">
+        <v>21736872</v>
+      </c>
+      <c r="AB721" s="7">
+        <v>-8231083</v>
+      </c>
+      <c r="AC721" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD721" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE721" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF721" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="722" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A722" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B722" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="C722" s="2"/>
-      <c r="D722" s="2"/>
-      <c r="E722" s="2"/>
-      <c r="F722" s="2"/>
-      <c r="G722" s="2"/>
-      <c r="H722" s="2"/>
+      <c r="D722" s="5">
+        <v>6082</v>
+      </c>
+      <c r="E722" s="5">
+        <v>0</v>
+      </c>
+      <c r="F722" s="5">
+        <v>0</v>
+      </c>
+      <c r="G722" s="5">
+        <v>0</v>
+      </c>
+      <c r="H722" s="5">
+        <v>0</v>
+      </c>
       <c r="I722" s="2"/>
-      <c r="J722" s="2"/>
-      <c r="K722" s="2"/>
-      <c r="L722" s="2"/>
-      <c r="M722" s="2"/>
-      <c r="N722" s="2"/>
-      <c r="O722" s="2"/>
-      <c r="P722" s="2"/>
-      <c r="Q722" s="2"/>
-      <c r="R722" s="2"/>
-      <c r="S722" s="2"/>
+      <c r="J722" s="5">
+        <v>0</v>
+      </c>
+      <c r="K722" s="5">
+        <v>0</v>
+      </c>
+      <c r="L722" s="5">
+        <v>0</v>
+      </c>
+      <c r="M722" s="5">
+        <v>0</v>
+      </c>
+      <c r="N722" s="6">
+        <v>205980</v>
+      </c>
+      <c r="O722" s="6">
+        <v>205980</v>
+      </c>
+      <c r="P722" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q722" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R722" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S722" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="T722" s="2"/>
-      <c r="U722" s="2"/>
-      <c r="V722" s="2"/>
-      <c r="W722" s="2"/>
-      <c r="X722" s="2"/>
-      <c r="Y722" s="2"/>
-      <c r="Z722" s="2"/>
-      <c r="AA722" s="2"/>
-      <c r="AB722" s="2"/>
-      <c r="AC722" s="2"/>
-      <c r="AD722" s="2"/>
-      <c r="AE722" s="2"/>
-      <c r="AF722" s="2"/>
-    </row>
-    <row r="723" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A723" s="2"/>
-      <c r="B723" s="2"/>
+      <c r="U722" s="5">
+        <v>0</v>
+      </c>
+      <c r="V722" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W722" s="5">
+        <v>0</v>
+      </c>
+      <c r="X722" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y722" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z722" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA722" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB722" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC722" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD722" s="7">
+        <v>49395681</v>
+      </c>
+      <c r="AE722" s="7">
+        <v>49395681</v>
+      </c>
+      <c r="AF722" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="723" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A723" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B723" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="C723" s="2"/>
-      <c r="D723" s="2"/>
-      <c r="E723" s="2"/>
-      <c r="F723" s="2"/>
-      <c r="G723" s="2"/>
-      <c r="H723" s="2"/>
-      <c r="I723" s="2"/>
-      <c r="J723" s="2"/>
-      <c r="K723" s="2"/>
-      <c r="L723" s="2"/>
-      <c r="M723" s="2"/>
-      <c r="N723" s="2"/>
-      <c r="O723" s="2"/>
-      <c r="P723" s="2"/>
-      <c r="Q723" s="2"/>
-      <c r="R723" s="2"/>
-      <c r="S723" s="2"/>
+      <c r="D723" s="5">
+        <v>3033</v>
+      </c>
+      <c r="E723" s="5">
+        <v>0</v>
+      </c>
+      <c r="F723" s="6">
+        <v>1000000</v>
+      </c>
+      <c r="G723" s="5">
+        <v>5.7130000000000001</v>
+      </c>
+      <c r="H723" s="6">
+        <v>5713300</v>
+      </c>
+      <c r="I723" s="5">
+        <v>5.26</v>
+      </c>
+      <c r="J723" s="6">
+        <v>5260000</v>
+      </c>
+      <c r="K723" s="6">
+        <v>-453300</v>
+      </c>
+      <c r="L723" s="7">
+        <v>-74745563</v>
+      </c>
+      <c r="M723" s="5">
+        <v>0</v>
+      </c>
+      <c r="N723" s="5">
+        <v>0</v>
+      </c>
+      <c r="O723" s="5">
+        <v>0</v>
+      </c>
+      <c r="P723" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q723" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R723" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S723" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="T723" s="2"/>
-      <c r="U723" s="2"/>
-      <c r="V723" s="2"/>
-      <c r="W723" s="2"/>
-      <c r="X723" s="2"/>
-      <c r="Y723" s="2"/>
-      <c r="Z723" s="2"/>
-      <c r="AA723" s="2"/>
-      <c r="AB723" s="2"/>
-      <c r="AC723" s="2"/>
-      <c r="AD723" s="2"/>
-      <c r="AE723" s="2"/>
-      <c r="AF723" s="2"/>
-    </row>
-    <row r="724" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A724" s="2"/>
-      <c r="B724" s="2"/>
+      <c r="U723" s="5">
+        <v>0</v>
+      </c>
+      <c r="V723" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="W723" s="5">
+        <v>183.11</v>
+      </c>
+      <c r="X723" s="7">
+        <v>1046162363</v>
+      </c>
+      <c r="Y723" s="5">
+        <v>184.68</v>
+      </c>
+      <c r="Z723" s="7">
+        <v>971416800</v>
+      </c>
+      <c r="AA723" s="7">
+        <v>-83715444</v>
+      </c>
+      <c r="AB723" s="7">
+        <v>8969881</v>
+      </c>
+      <c r="AC723" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD723" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE723" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF723" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="724" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A724" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B724" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="C724" s="2"/>
-      <c r="D724" s="2"/>
-      <c r="E724" s="2"/>
-      <c r="F724" s="2"/>
-      <c r="G724" s="2"/>
-      <c r="H724" s="2"/>
-      <c r="I724" s="2"/>
-      <c r="J724" s="2"/>
-      <c r="K724" s="2"/>
-      <c r="L724" s="2"/>
-      <c r="M724" s="2"/>
-      <c r="N724" s="2"/>
-      <c r="O724" s="2"/>
-      <c r="P724" s="2"/>
-      <c r="Q724" s="2"/>
-      <c r="R724" s="2"/>
-      <c r="S724" s="2"/>
+      <c r="D724" s="5">
+        <v>2800</v>
+      </c>
+      <c r="E724" s="5">
+        <v>0</v>
+      </c>
+      <c r="F724" s="6">
+        <v>100000</v>
+      </c>
+      <c r="G724" s="5">
+        <v>27.495000000000001</v>
+      </c>
+      <c r="H724" s="6">
+        <v>2749550</v>
+      </c>
+      <c r="I724" s="5">
+        <v>26.98</v>
+      </c>
+      <c r="J724" s="6">
+        <v>2698000</v>
+      </c>
+      <c r="K724" s="6">
+        <v>-51550</v>
+      </c>
+      <c r="L724" s="7">
+        <v>-14386957</v>
+      </c>
+      <c r="M724" s="5">
+        <v>0</v>
+      </c>
+      <c r="N724" s="5">
+        <v>0</v>
+      </c>
+      <c r="O724" s="5">
+        <v>0</v>
+      </c>
+      <c r="P724" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q724" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R724" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S724" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="T724" s="2"/>
-      <c r="U724" s="2"/>
-      <c r="V724" s="2"/>
-      <c r="W724" s="2"/>
-      <c r="X724" s="2"/>
-      <c r="Y724" s="2"/>
-      <c r="Z724" s="2"/>
-      <c r="AA724" s="2"/>
-      <c r="AB724" s="2"/>
-      <c r="AC724" s="2"/>
-      <c r="AD724" s="2"/>
-      <c r="AE724" s="2"/>
-      <c r="AF724" s="2"/>
-    </row>
-    <row r="725" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A725" s="2"/>
-      <c r="B725" s="2"/>
+      <c r="U724" s="5">
+        <v>0</v>
+      </c>
+      <c r="V724" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="W724" s="5">
+        <v>186.44</v>
+      </c>
+      <c r="X724" s="7">
+        <v>512653597</v>
+      </c>
+      <c r="Y724" s="5">
+        <v>184.68</v>
+      </c>
+      <c r="Z724" s="7">
+        <v>498266640</v>
+      </c>
+      <c r="AA724" s="7">
+        <v>-9520254</v>
+      </c>
+      <c r="AB724" s="7">
+        <v>-4866703</v>
+      </c>
+      <c r="AC724" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD724" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE724" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF724" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="725" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A725" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B725" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="C725" s="2"/>
-      <c r="D725" s="2"/>
-      <c r="E725" s="2"/>
-      <c r="F725" s="2"/>
-      <c r="G725" s="2"/>
-      <c r="H725" s="2"/>
-      <c r="I725" s="2"/>
-      <c r="J725" s="2"/>
-      <c r="K725" s="2"/>
-      <c r="L725" s="2"/>
-      <c r="M725" s="2"/>
-      <c r="N725" s="2"/>
-      <c r="O725" s="2"/>
-      <c r="P725" s="2"/>
-      <c r="Q725" s="2"/>
-      <c r="R725" s="2"/>
-      <c r="S725" s="2"/>
+      <c r="D725" s="5">
+        <v>9988</v>
+      </c>
+      <c r="E725" s="5">
+        <v>0</v>
+      </c>
+      <c r="F725" s="6">
+        <v>35500</v>
+      </c>
+      <c r="G725" s="5">
+        <v>147.79</v>
+      </c>
+      <c r="H725" s="6">
+        <v>5246547.5199999996</v>
+      </c>
+      <c r="I725" s="5">
+        <v>154.69999999999999</v>
+      </c>
+      <c r="J725" s="6">
+        <v>5491850</v>
+      </c>
+      <c r="K725" s="6">
+        <v>245302.49</v>
+      </c>
+      <c r="L725" s="7">
+        <v>39974570</v>
+      </c>
+      <c r="M725" s="5">
+        <v>0</v>
+      </c>
+      <c r="N725" s="6">
+        <v>431288.52</v>
+      </c>
+      <c r="O725" s="6">
+        <v>431288.52</v>
+      </c>
+      <c r="P725" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q725" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R725" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S725" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="T725" s="2"/>
-      <c r="U725" s="2"/>
-      <c r="V725" s="2"/>
-      <c r="W725" s="2"/>
-      <c r="X725" s="2"/>
-      <c r="Y725" s="2"/>
-      <c r="Z725" s="2"/>
-      <c r="AA725" s="2"/>
-      <c r="AB725" s="2"/>
-      <c r="AC725" s="2"/>
-      <c r="AD725" s="2"/>
-      <c r="AE725" s="2"/>
-      <c r="AF725" s="2"/>
+      <c r="U725" s="5">
+        <v>0</v>
+      </c>
+      <c r="V725" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W725" s="5">
+        <v>185.69</v>
+      </c>
+      <c r="X725" s="7">
+        <v>974260288</v>
+      </c>
+      <c r="Y725" s="5">
+        <v>184.68</v>
+      </c>
+      <c r="Z725" s="7">
+        <v>1014234858</v>
+      </c>
+      <c r="AA725" s="7">
+        <v>45302462</v>
+      </c>
+      <c r="AB725" s="7">
+        <v>-5327893</v>
+      </c>
+      <c r="AC725" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD725" s="7">
+        <v>84316487</v>
+      </c>
+      <c r="AE725" s="7">
+        <v>84316487</v>
+      </c>
+      <c r="AF725" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="726" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A726" s="2"/>
-      <c r="B726" s="2"/>
+      <c r="A726" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B726" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="C726" s="2"/>
-      <c r="D726" s="2"/>
-      <c r="E726" s="2"/>
-      <c r="F726" s="2"/>
-      <c r="G726" s="2"/>
-      <c r="H726" s="2"/>
-      <c r="I726" s="2"/>
-      <c r="J726" s="2"/>
-      <c r="K726" s="2"/>
-      <c r="L726" s="2"/>
-      <c r="M726" s="2"/>
-      <c r="N726" s="2"/>
-      <c r="O726" s="2"/>
-      <c r="P726" s="2"/>
-      <c r="Q726" s="2"/>
-      <c r="R726" s="2"/>
-      <c r="S726" s="2"/>
+      <c r="D726" s="5">
+        <v>6861</v>
+      </c>
+      <c r="E726" s="5">
+        <v>0</v>
+      </c>
+      <c r="F726" s="6">
+        <v>1100</v>
+      </c>
+      <c r="G726" s="6">
+        <v>55916.79</v>
+      </c>
+      <c r="H726" s="6">
+        <v>61508468.420000002</v>
+      </c>
+      <c r="I726" s="6">
+        <v>60220</v>
+      </c>
+      <c r="J726" s="6">
+        <v>66242000</v>
+      </c>
+      <c r="K726" s="6">
+        <v>4733531.58</v>
+      </c>
+      <c r="L726" s="7">
+        <v>49171577</v>
+      </c>
+      <c r="M726" s="5">
+        <v>0</v>
+      </c>
+      <c r="N726" s="6">
+        <v>984568.42</v>
+      </c>
+      <c r="O726" s="6">
+        <v>984568.42</v>
+      </c>
+      <c r="P726" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q726" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R726" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="S726" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="T726" s="2"/>
-      <c r="U726" s="2"/>
-      <c r="V726" s="2"/>
-      <c r="W726" s="2"/>
-      <c r="X726" s="2"/>
-      <c r="Y726" s="2"/>
-      <c r="Z726" s="2"/>
-      <c r="AA726" s="2"/>
-      <c r="AB726" s="2"/>
-      <c r="AC726" s="2"/>
-      <c r="AD726" s="2"/>
-      <c r="AE726" s="2"/>
-      <c r="AF726" s="2"/>
+      <c r="U726" s="5">
+        <v>0</v>
+      </c>
+      <c r="V726" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W726" s="5">
+        <v>924.45</v>
+      </c>
+      <c r="X726" s="7">
+        <v>568621187</v>
+      </c>
+      <c r="Y726" s="5">
+        <v>932.63</v>
+      </c>
+      <c r="Z726" s="7">
+        <v>617792764</v>
+      </c>
+      <c r="AA726" s="7">
+        <v>44146335</v>
+      </c>
+      <c r="AB726" s="7">
+        <v>5025242</v>
+      </c>
+      <c r="AC726" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD726" s="7">
+        <v>20453721</v>
+      </c>
+      <c r="AE726" s="7">
+        <v>20453721</v>
+      </c>
+      <c r="AF726" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="727" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A727" s="2"/>
-      <c r="B727" s="2"/>
+      <c r="A727" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B727" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="C727" s="2"/>
-      <c r="D727" s="2"/>
-      <c r="E727" s="2"/>
-      <c r="F727" s="2"/>
-      <c r="G727" s="2"/>
-      <c r="H727" s="2"/>
+      <c r="D727" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E727" s="5">
+        <v>0</v>
+      </c>
+      <c r="F727" s="5">
+        <v>0</v>
+      </c>
+      <c r="G727" s="5">
+        <v>0</v>
+      </c>
+      <c r="H727" s="5">
+        <v>0</v>
+      </c>
       <c r="I727" s="2"/>
-      <c r="J727" s="2"/>
-      <c r="K727" s="2"/>
-      <c r="L727" s="2"/>
-      <c r="M727" s="2"/>
-      <c r="N727" s="2"/>
-      <c r="O727" s="2"/>
-      <c r="P727" s="2"/>
-      <c r="Q727" s="2"/>
-      <c r="R727" s="2"/>
-      <c r="S727" s="2"/>
+      <c r="J727" s="5">
+        <v>0</v>
+      </c>
+      <c r="K727" s="5">
+        <v>0</v>
+      </c>
+      <c r="L727" s="5">
+        <v>0</v>
+      </c>
+      <c r="M727" s="5">
+        <v>0</v>
+      </c>
+      <c r="N727" s="6">
+        <v>4911499</v>
+      </c>
+      <c r="O727" s="6">
+        <v>4911499</v>
+      </c>
+      <c r="P727" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q727" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R727" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="S727" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="T727" s="2"/>
-      <c r="U727" s="2"/>
-      <c r="V727" s="2"/>
-      <c r="W727" s="2"/>
-      <c r="X727" s="2"/>
-      <c r="Y727" s="2"/>
-      <c r="Z727" s="2"/>
-      <c r="AA727" s="2"/>
-      <c r="AB727" s="2"/>
-      <c r="AC727" s="2"/>
-      <c r="AD727" s="2"/>
-      <c r="AE727" s="2"/>
-      <c r="AF727" s="2"/>
+      <c r="U727" s="5">
+        <v>0</v>
+      </c>
+      <c r="V727" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W727" s="5">
+        <v>0</v>
+      </c>
+      <c r="X727" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y727" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z727" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA727" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB727" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC727" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD727" s="7">
+        <v>42855505</v>
+      </c>
+      <c r="AE727" s="7">
+        <v>42855505</v>
+      </c>
+      <c r="AF727" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="728" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A728" s="2"/>
-      <c r="B728" s="2"/>
+      <c r="A728" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B728" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C728" s="2"/>
-      <c r="D728" s="2"/>
-      <c r="E728" s="2"/>
-      <c r="F728" s="2"/>
-      <c r="G728" s="2"/>
-      <c r="H728" s="2"/>
-      <c r="I728" s="2"/>
-      <c r="J728" s="2"/>
-      <c r="K728" s="2"/>
-      <c r="L728" s="2"/>
-      <c r="M728" s="2"/>
-      <c r="N728" s="2"/>
-      <c r="O728" s="2"/>
-      <c r="P728" s="2"/>
-      <c r="Q728" s="2"/>
-      <c r="R728" s="2"/>
-      <c r="S728" s="2"/>
+      <c r="D728" s="5">
+        <v>9984</v>
+      </c>
+      <c r="E728" s="5">
+        <v>0</v>
+      </c>
+      <c r="F728" s="6">
+        <v>13000</v>
+      </c>
+      <c r="G728" s="6">
+        <v>4066.73</v>
+      </c>
+      <c r="H728" s="6">
+        <v>52867552.170000002</v>
+      </c>
+      <c r="I728" s="6">
+        <v>4440</v>
+      </c>
+      <c r="J728" s="6">
+        <v>57720000</v>
+      </c>
+      <c r="K728" s="6">
+        <v>4852447.83</v>
+      </c>
+      <c r="L728" s="7">
+        <v>48485592</v>
+      </c>
+      <c r="M728" s="5">
+        <v>0</v>
+      </c>
+      <c r="N728" s="6">
+        <v>4615632.17</v>
+      </c>
+      <c r="O728" s="6">
+        <v>4615632.17</v>
+      </c>
+      <c r="P728" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q728" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R728" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="S728" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="T728" s="2"/>
-      <c r="U728" s="2"/>
-      <c r="V728" s="2"/>
-      <c r="W728" s="2"/>
-      <c r="X728" s="2"/>
-      <c r="Y728" s="2"/>
-      <c r="Z728" s="2"/>
-      <c r="AA728" s="2"/>
-      <c r="AB728" s="2"/>
-      <c r="AC728" s="2"/>
-      <c r="AD728" s="2"/>
-      <c r="AE728" s="2"/>
-      <c r="AF728" s="2"/>
+      <c r="U728" s="5">
+        <v>0</v>
+      </c>
+      <c r="V728" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W728" s="5">
+        <v>926.51</v>
+      </c>
+      <c r="X728" s="7">
+        <v>489828444</v>
+      </c>
+      <c r="Y728" s="5">
+        <v>932.63</v>
+      </c>
+      <c r="Z728" s="7">
+        <v>538314036</v>
+      </c>
+      <c r="AA728" s="7">
+        <v>45255384</v>
+      </c>
+      <c r="AB728" s="7">
+        <v>3230207</v>
+      </c>
+      <c r="AC728" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD728" s="7">
+        <v>48366259</v>
+      </c>
+      <c r="AE728" s="7">
+        <v>48366259</v>
+      </c>
+      <c r="AF728" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="729" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A729" s="2"/>
-      <c r="B729" s="2"/>
+      <c r="A729" s="3">
+        <v>46072</v>
+      </c>
+      <c r="B729" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="C729" s="2"/>
-      <c r="D729" s="2"/>
-      <c r="E729" s="2"/>
-      <c r="F729" s="2"/>
-      <c r="G729" s="2"/>
-      <c r="H729" s="2"/>
+      <c r="D729" s="5">
+        <v>6954</v>
+      </c>
+      <c r="E729" s="5">
+        <v>0</v>
+      </c>
+      <c r="F729" s="5">
+        <v>0</v>
+      </c>
+      <c r="G729" s="5">
+        <v>0</v>
+      </c>
+      <c r="H729" s="5">
+        <v>0</v>
+      </c>
       <c r="I729" s="2"/>
-      <c r="J729" s="2"/>
-      <c r="K729" s="2"/>
-      <c r="L729" s="2"/>
-      <c r="M729" s="2"/>
-      <c r="N729" s="2"/>
-      <c r="O729" s="2"/>
-      <c r="P729" s="2"/>
-      <c r="Q729" s="2"/>
-      <c r="R729" s="2"/>
-      <c r="S729" s="2"/>
+      <c r="J729" s="5">
+        <v>0</v>
+      </c>
+      <c r="K729" s="5">
+        <v>0</v>
+      </c>
+      <c r="L729" s="5">
+        <v>0</v>
+      </c>
+      <c r="M729" s="5">
+        <v>0</v>
+      </c>
+      <c r="N729" s="6">
+        <v>1652400</v>
+      </c>
+      <c r="O729" s="6">
+        <v>1652400</v>
+      </c>
+      <c r="P729" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q729" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R729" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="S729" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="T729" s="2"/>
-      <c r="U729" s="2"/>
-      <c r="V729" s="2"/>
-      <c r="W729" s="2"/>
-      <c r="X729" s="2"/>
-      <c r="Y729" s="2"/>
-      <c r="Z729" s="2"/>
-      <c r="AA729" s="2"/>
-      <c r="AB729" s="2"/>
-      <c r="AC729" s="2"/>
-      <c r="AD729" s="2"/>
-      <c r="AE729" s="2"/>
-      <c r="AF729" s="2"/>
+      <c r="U729" s="5">
+        <v>0</v>
+      </c>
+      <c r="V729" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W729" s="5">
+        <v>0</v>
+      </c>
+      <c r="X729" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y729" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z729" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA729" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB729" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC729" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD729" s="7">
+        <v>30313594</v>
+      </c>
+      <c r="AE729" s="7">
+        <v>30313594</v>
+      </c>
+      <c r="AF729" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="730" spans="1:32" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A730" s="2"/>

</xml_diff>